<commit_message>
intro & variable table updates
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\mnn1\Chapter 1\Write up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856B0DDD-7A35-4583-AD04-FC2164696E15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B20941-5657-48A0-9FFB-9F79791BEA73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>GDP growth</t>
-  </si>
-  <si>
     <t>Billions USD</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Development flows to agriculture</t>
   </si>
   <si>
-    <t>development flows to environment</t>
-  </si>
-  <si>
     <t>FAO</t>
   </si>
   <si>
@@ -125,12 +119,6 @@
     <t>Global</t>
   </si>
   <si>
-    <t>IMF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index of global monthly prices for timber, cotton, wool, rubber, and hides. Annual mean calculated an used. </t>
-  </si>
-  <si>
     <t>Relative level of the aggregate volume of agricultural production for each year in comparison with the base period 2004-2006</t>
   </si>
   <si>
@@ -140,9 +128,6 @@
     <t xml:space="preserve">Crop Production </t>
   </si>
   <si>
-    <t xml:space="preserve">Agricultural Raw Materials </t>
-  </si>
-  <si>
     <t>Relative level of the aggregate volume of non-food agricultural production for each year in comparison with the base period 2004-2006</t>
   </si>
   <si>
@@ -153,6 +138,60 @@
   </si>
   <si>
     <t>Total production values for industrial roundwood, non-coniferous tropical wood, other industrial roundwood, sawlogs and veneer logs (coniferous and non-coniferous), and sawnwood (coniferous and non-coniferous</t>
+  </si>
+  <si>
+    <t>Proportion of national GDP</t>
+  </si>
+  <si>
+    <t>Development flows to environment</t>
+  </si>
+  <si>
+    <t>Price of rice</t>
+  </si>
+  <si>
+    <t>Price of corn</t>
+  </si>
+  <si>
+    <t>Price of rubber</t>
+  </si>
+  <si>
+    <t>Price of sugar</t>
+  </si>
+  <si>
+    <t>USD/ton</t>
+  </si>
+  <si>
+    <t>Median annual global market price of rice</t>
+  </si>
+  <si>
+    <t>Annual global market price of corn</t>
+  </si>
+  <si>
+    <t>Regional</t>
+  </si>
+  <si>
+    <t>RASCE</t>
+  </si>
+  <si>
+    <t>Monthly regional market value of rubber on the Singapore Exchange</t>
+  </si>
+  <si>
+    <t>Annual global market price of sugar</t>
+  </si>
+  <si>
+    <t>Producer prices</t>
+  </si>
+  <si>
+    <t>Producer price of rubber</t>
+  </si>
+  <si>
+    <t>Producer price of cassava</t>
+  </si>
+  <si>
+    <t>Producer price of corn</t>
+  </si>
+  <si>
+    <t>Producer price of sugar</t>
   </si>
 </sst>
 </file>
@@ -525,23 +564,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="55.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="5" max="5" width="61" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -561,192 +600,257 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intro, methods, data table updates
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B20941-5657-48A0-9FFB-9F79791BEA73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46104FA6-4ED0-438B-A072-7585C74574C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Resolution</t>
   </si>
   <si>
-    <t>References</t>
-  </si>
-  <si>
     <t>Economy</t>
   </si>
   <si>
@@ -192,6 +189,12 @@
   </si>
   <si>
     <t>Producer price of sugar</t>
+  </si>
+  <si>
+    <t>Producer price of Rice</t>
+  </si>
+  <si>
+    <t>Farmgate prices for Cambodian producers</t>
   </si>
 </sst>
 </file>
@@ -243,13 +246,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,10 +581,9 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -594,263 +597,325 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E14" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor additions to methods and data sources tables
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46104FA6-4ED0-438B-A072-7585C74574C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480EB7E9-3AB3-43B1-B132-18B1139C71C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -195,6 +196,60 @@
   </si>
   <si>
     <t>Farmgate prices for Cambodian producers</t>
+  </si>
+  <si>
+    <t>Set</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Demographics</t>
+  </si>
+  <si>
+    <t>Total population</t>
+  </si>
+  <si>
+    <t>Number indigenous</t>
+  </si>
+  <si>
+    <t>Proportion of total population</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Transformation for analysis</t>
+  </si>
+  <si>
+    <t>Total number of people who are indigneous/ethnic minority. Transformed into the proportion of people who are indigenous</t>
+  </si>
+  <si>
+    <t>Males aged 6 - 24 in school</t>
+  </si>
+  <si>
+    <t>Proportion of total number of males aged 6 - 24</t>
+  </si>
+  <si>
+    <t>Number of males aged 16 - 24 in full time education. Transformed into a proportion of the total population of males aged 16 - 24</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Number of adults employed in primary sector</t>
+  </si>
+  <si>
+    <t>Number of adults employed in secondary sector</t>
+  </si>
+  <si>
+    <t>Proportion of total adult population</t>
+  </si>
+  <si>
+    <t>The primary sector includes agriculture (rice and other crop farming), fishing, livestock farming, forestry, and non-timber forest product collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The secondary sector includes wood-based production (e.g. furniture), metal- and glass-based production, foodstuff production, plastic- and rubber-based production, textiles production </t>
   </si>
 </sst>
 </file>
@@ -570,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +634,7 @@
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
   </cols>
   <sheetData>
@@ -794,7 +849,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -922,4 +977,102 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" customWidth="1"/>
+    <col min="4" max="4" width="69" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Methods tables (Table 1 & 2)
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480EB7E9-3AB3-43B1-B132-18B1139C71C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D560C4F-B14C-411B-BB67-854DC7B66232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -222,18 +222,12 @@
     <t>Transformation for analysis</t>
   </si>
   <si>
-    <t>Total number of people who are indigneous/ethnic minority. Transformed into the proportion of people who are indigenous</t>
-  </si>
-  <si>
     <t>Males aged 6 - 24 in school</t>
   </si>
   <si>
     <t>Proportion of total number of males aged 6 - 24</t>
   </si>
   <si>
-    <t>Number of males aged 16 - 24 in full time education. Transformed into a proportion of the total population of males aged 16 - 24</t>
-  </si>
-  <si>
     <t>Employment</t>
   </si>
   <si>
@@ -246,10 +240,121 @@
     <t>Proportion of total adult population</t>
   </si>
   <si>
-    <t>The primary sector includes agriculture (rice and other crop farming), fishing, livestock farming, forestry, and non-timber forest product collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The secondary sector includes wood-based production (e.g. furniture), metal- and glass-based production, foodstuff production, plastic- and rubber-based production, textiles production </t>
+    <t>Total number of people who are indigneous/ethnic minority</t>
+  </si>
+  <si>
+    <t>Number of males aged 16 - 24 in full time education</t>
+  </si>
+  <si>
+    <t>Economic security</t>
+  </si>
+  <si>
+    <t>Number of families with &lt;1ha farmland (including no farmland)</t>
+  </si>
+  <si>
+    <t>Proportion of total number of families</t>
+  </si>
+  <si>
+    <t>Number of families who keep pigs</t>
+  </si>
+  <si>
+    <t>Access to services</t>
+  </si>
+  <si>
+    <t>Distance to nearest school</t>
+  </si>
+  <si>
+    <t>Median distance from any village in the commune to the nearest school (primary or secondary)</t>
+  </si>
+  <si>
+    <t>Number of families with access to waste collection</t>
+  </si>
+  <si>
+    <t>Distance to the Commune Office</t>
+  </si>
+  <si>
+    <t>Median distance from any village in the commune to the Commune Office (government administration office)</t>
+  </si>
+  <si>
+    <t>Social justice</t>
+  </si>
+  <si>
+    <t>Number of criminal cases</t>
+  </si>
+  <si>
+    <t>Criminal cases per capita</t>
+  </si>
+  <si>
+    <t>Includes murder, theft, and other criminal cases</t>
+  </si>
+  <si>
+    <t>Number of land conflict cases</t>
+  </si>
+  <si>
+    <t>In the previous 12 months</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>Number of in-migrants</t>
+  </si>
+  <si>
+    <t>Number of out-migrants</t>
+  </si>
+  <si>
+    <t>Migration into the commune</t>
+  </si>
+  <si>
+    <t>Migration out of the commune</t>
+  </si>
+  <si>
+    <t>Mean elevation (masl)</t>
+  </si>
+  <si>
+    <t>Mean elevation for the commune</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Distance to international border (km)</t>
+  </si>
+  <si>
+    <t>Distance from the centre of the commune to the nearest international border</t>
+  </si>
+  <si>
+    <t>Distance to Provincial Capital (km)</t>
+  </si>
+  <si>
+    <t>Distance from the centre of the commune to the centre of the provincial capital (town or city)</t>
+  </si>
+  <si>
+    <t>Presence of economic land concessions</t>
+  </si>
+  <si>
+    <t>Binary. 1 = part or all of an economic land concession falls within the boundary of the commune, 0 = no economic land concession falls within the commune boundary</t>
+  </si>
+  <si>
+    <t>Protected area category</t>
+  </si>
+  <si>
+    <t>Presence of Protected area</t>
+  </si>
+  <si>
+    <t>Binary. 1 = part or all of an protected area falls within the boundary of the commune, 0 = no protected area falls within the commune boundary. "Protected area" includes Wildlife Sanctuary, National Park, Protected Landscapes, Multiple-use areas, RAMSAR sites</t>
+  </si>
+  <si>
+    <t>None = no protected area falls within commune, MULTI = more than one category of protected area falls within commune, WS = wildlife sanctuary, NP = national park, PL = protected landscape, MUA = multiple-use area, RMS = RAMSAR</t>
+  </si>
+  <si>
+    <t>Includes women, men, and children of all ages</t>
+  </si>
+  <si>
+    <t>The primary sector includes agriculture (rice and other crop farming), fishing, livestock farming, forestry, and non-timber forest product collection (Kenessey 1987)</t>
+  </si>
+  <si>
+    <t>The secondary sector includes wood-based production (e.g. furniture), metal- and glass-based production, foodstuff production, plastic- and rubber-based production, textiles production (Kenessey 1987)</t>
   </si>
 </sst>
 </file>
@@ -981,31 +1086,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
     <col min="4" max="4" width="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1016,13 +1121,16 @@
       <c r="B2" t="s">
         <v>57</v>
       </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>58</v>
       </c>
@@ -1030,7 +1138,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1038,41 +1146,180 @@
         <v>60</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding table S1 and Table SX
Table S1 is the full list of macroeconomic predictors (including those that were not included in final modelling). Table Sx is the ESA CCI bands used to calculate forest cover
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D560C4F-B14C-411B-BB67-854DC7B66232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947FE241-0F3E-44A8-82BB-2FFF4B784731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Table Sx - CCI bands" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="150">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -355,6 +357,135 @@
   </si>
   <si>
     <t>The secondary sector includes wood-based production (e.g. furniture), metal- and glass-based production, foodstuff production, plastic- and rubber-based production, textiles production (Kenessey 1987)</t>
+  </si>
+  <si>
+    <t>GPD growth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD </t>
+  </si>
+  <si>
+    <t>GNI per capita</t>
+  </si>
+  <si>
+    <t>Gross National Income per capita. Calculated as gross national income divded by the mid-year population at current USD rates</t>
+  </si>
+  <si>
+    <t>Industrial sector value of GDP</t>
+  </si>
+  <si>
+    <t>IMF</t>
+  </si>
+  <si>
+    <t>Price index for global agricultural raw materials including timber, cotton, wool, rubber, and hides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agricultural Raw Materials </t>
+  </si>
+  <si>
+    <t>Forest remaining</t>
+  </si>
+  <si>
+    <t>km2</t>
+  </si>
+  <si>
+    <t>ESACCI</t>
+  </si>
+  <si>
+    <t>Total forested area</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>No data</t>
+  </si>
+  <si>
+    <t>Cropland, rainfed</t>
+  </si>
+  <si>
+    <t>Herbaceous cover</t>
+  </si>
+  <si>
+    <t>Tree or shrub cover</t>
+  </si>
+  <si>
+    <t>Cropland, irrigated or post-flooding</t>
+  </si>
+  <si>
+    <t>Mosaic cropland (&gt;50%) / natural vegetation (tree, shrub, herbaceous cover) (&lt;50%)</t>
+  </si>
+  <si>
+    <t>Mosaic natural vegetation (tree, shrub, herbaceous cover) (&gt;50%) / cropland (&lt;50%)</t>
+  </si>
+  <si>
+    <t>Tree cover, broadleaved, evergreen, cosed to open (&gt;15%)</t>
+  </si>
+  <si>
+    <t>Tree cover, broadleaved, deciduous, closed to open (&gt;15%)</t>
+  </si>
+  <si>
+    <t>Tree cover, broadleaves, decisuous, closed (&gt;40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, deciduous, closed to open (&gt;15%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, evergreen, closed to open (&gt;15%)</t>
+  </si>
+  <si>
+    <t>Tree cover, broadleaves, deciduous, open (15 - 40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, evergreen, closed (&gt;40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, evergreen, open (15 - 40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, deciduous, closed (&gt;40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, needleleaved, deciduous, open (15 - 40%)</t>
+  </si>
+  <si>
+    <t>Tree cover, mixed leaf type (broadleaved and needleleaved)</t>
+  </si>
+  <si>
+    <t>Mosaic tree and shrub (&gt;50%) / herbaceous cover (&lt;50%)</t>
+  </si>
+  <si>
+    <t>Mosaic herbaceous cover (&gt;50%) / tree and shrub (&lt;50%)</t>
+  </si>
+  <si>
+    <t>Shrubland</t>
+  </si>
+  <si>
+    <t>Evergreen shrubland</t>
+  </si>
+  <si>
+    <t>Deciduous shrubland</t>
+  </si>
+  <si>
+    <t>Grassland</t>
+  </si>
+  <si>
+    <t>Lichens and mosses</t>
+  </si>
+  <si>
+    <t>Sparse vegetation (tree, shrub, herbaceous cover) (&lt;15%)</t>
+  </si>
+  <si>
+    <t>Sparse shrub (&lt;15%)</t>
+  </si>
+  <si>
+    <t>Sparse herbaceous cover (&lt;15%)</t>
+  </si>
+  <si>
+    <t>Tree cover, flooded, fresh or brakish water</t>
   </si>
 </sst>
 </file>
@@ -386,12 +517,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -406,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -414,6 +551,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,11 +1223,459 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858278ED-196A-4B59-8830-674E5B382BAC}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1322,4 +1908,262 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661002B2-E508-42DE-AAF7-55B64A4B61E8}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="74.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>50</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>60</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>61</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>62</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>70</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
+        <v>71</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>72</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>80</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>81</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>82</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>90</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>100</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>110</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>120</v>
+      </c>
+      <c r="B22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>121</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>122</v>
+      </c>
+      <c r="B24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>140</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>153</v>
+      </c>
+      <c r="B29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>160</v>
+      </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tables - minor update
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947FE241-0F3E-44A8-82BB-2FFF4B784731}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8954E46-FE80-4DCE-AA86-6BF303AEA3E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
@@ -869,7 +869,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Methods tables minor additions
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8954E46-FE80-4DCE-AA86-6BF303AEA3E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376C678-1AEE-4471-B90D-0CE9BE6D287E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1024,7 +1024,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1674,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tables - minor updates
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A376C678-1AEE-4471-B90D-0CE9BE6D287E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473D6D1D-727A-4B13-9765-C4DC6DAFA655}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
@@ -251,9 +251,6 @@
     <t>Economic security</t>
   </si>
   <si>
-    <t>Number of families with &lt;1ha farmland (including no farmland)</t>
-  </si>
-  <si>
     <t>Proportion of total number of families</t>
   </si>
   <si>
@@ -486,6 +483,9 @@
   </si>
   <si>
     <t>Tree cover, flooded, fresh or brakish water</t>
+  </si>
+  <si>
+    <t>Number of families with &lt;1ha rice land (including no rice land)</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1309,7 +1309,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1348,7 +1348,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
@@ -1427,10 +1427,10 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1644,24 +1644,24 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
         <v>115</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
         <v>116</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,7 +1708,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1752,7 +1752,7 @@
         <v>67</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -1763,7 +1763,7 @@
         <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1771,137 +1771,137 @@
         <v>70</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" t="s">
         <v>81</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1925,10 +1925,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
         <v>119</v>
-      </c>
-      <c r="B1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1936,7 +1936,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1944,7 +1944,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1952,7 +1952,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1960,7 +1960,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1968,7 +1968,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1976,7 +1976,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1984,7 +1984,7 @@
         <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1992,7 +1992,7 @@
         <v>50</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2000,7 +2000,7 @@
         <v>60</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2008,7 +2008,7 @@
         <v>61</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2016,7 +2016,7 @@
         <v>62</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2024,7 +2024,7 @@
         <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2032,7 +2032,7 @@
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2040,7 +2040,7 @@
         <v>72</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2048,7 +2048,7 @@
         <v>80</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2056,7 +2056,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2064,7 +2064,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2072,7 +2072,7 @@
         <v>90</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2080,7 +2080,7 @@
         <v>100</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2088,7 +2088,7 @@
         <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2096,7 +2096,7 @@
         <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2104,7 +2104,7 @@
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2112,7 +2112,7 @@
         <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2120,7 +2120,7 @@
         <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2128,7 +2128,7 @@
         <v>140</v>
       </c>
       <c r="B26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2136,7 +2136,7 @@
         <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2144,7 +2144,7 @@
         <v>152</v>
       </c>
       <c r="B28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2152,7 +2152,7 @@
         <v>153</v>
       </c>
       <c r="B29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2160,7 +2160,7 @@
         <v>160</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tables - new column added Table 2
to highlight which socioecon vars were converted to categorical in the province-level analysis
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA97DA7C-54A1-4531-9B11-73855BC84ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69467E95-45FE-4506-8BDB-9474DB1C309D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="153">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -486,6 +486,15 @@
   </si>
   <si>
     <t>Number of families with &lt;1ha rice land (including no rice land)</t>
+  </si>
+  <si>
+    <t>Province-level class</t>
+  </si>
+  <si>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1672,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1683,10 +1692,11 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="33.5546875" customWidth="1"/>
     <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="69" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -1697,10 +1707,13 @@
         <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1708,26 +1721,32 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -1737,11 +1756,14 @@
       <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1751,22 +1773,28 @@
       <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -1776,27 +1804,36 @@
       <c r="C8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>76</v>
       </c>
@@ -1804,15 +1841,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1823,18 +1860,24 @@
         <v>81</v>
       </c>
       <c r="D13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -1842,18 +1885,24 @@
         <v>86</v>
       </c>
       <c r="D15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -1861,46 +1910,55 @@
         <v>90</v>
       </c>
       <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creating results tables - ongoing
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69467E95-45FE-4506-8BDB-9474DB1C309D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7C0D6E-0107-4268-A4C9-D611CD8EDADA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table S1" sheetId="3" r:id="rId2"/>
-    <sheet name="Table 2" sheetId="2" r:id="rId3"/>
-    <sheet name="Table Sx - CCI bands" sheetId="4" r:id="rId4"/>
+    <sheet name="Table 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table 3" sheetId="5" r:id="rId3"/>
+    <sheet name="Table 4" sheetId="6" r:id="rId4"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId5"/>
+    <sheet name="Table S2 - CCI bands" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="184">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -495,6 +497,99 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>People per km2</t>
+  </si>
+  <si>
+    <t>GDP</t>
+  </si>
+  <si>
+    <t>Agricultural proportion of GDP</t>
+  </si>
+  <si>
+    <t>Development flows - environment</t>
+  </si>
+  <si>
+    <t>Foreign direct investment</t>
+  </si>
+  <si>
+    <t>GDP growth</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macroeconomic </t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Development flows - agriculture</t>
+  </si>
+  <si>
+    <t>Commodity / production</t>
+  </si>
+  <si>
+    <t>Lag</t>
+  </si>
+  <si>
+    <t>z value</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Random effects</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Fixed effects</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Std.Dev</t>
+  </si>
+  <si>
+    <t>Z value</t>
+  </si>
+  <si>
+    <t>Mean elevation</t>
+  </si>
+  <si>
+    <t>Distance to In'tl border</t>
+  </si>
+  <si>
+    <t>Distance to Provincial capital</t>
+  </si>
+  <si>
+    <t>ELC presence</t>
+  </si>
+  <si>
+    <t>PA presence</t>
+  </si>
+  <si>
+    <t>Commune (intercept)</t>
+  </si>
+  <si>
+    <t>Province (intercept)</t>
+  </si>
+  <si>
+    <t>Year/Commune (slope)</t>
+  </si>
+  <si>
+    <t>Year/Province (slope)</t>
+  </si>
+  <si>
+    <t>-8.03 x 10-7</t>
   </si>
 </sst>
 </file>
@@ -552,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -561,6 +656,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -878,7 +974,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1010,6 +1106,9 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1232,6 +1331,590 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="69" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908CB573-80D5-4D21-A446-EADEBAD25FBE}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3">
+        <v>10.45</v>
+      </c>
+      <c r="C3">
+        <v>3.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="C4">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5">
+        <v>6.77</v>
+      </c>
+      <c r="C5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="C6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>-7.51</v>
+      </c>
+      <c r="E9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F9">
+        <v>-6.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D10">
+        <v>1.05</v>
+      </c>
+      <c r="E10">
+        <v>0.12</v>
+      </c>
+      <c r="F10">
+        <v>8.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D11">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E11">
+        <v>0.2</v>
+      </c>
+      <c r="F11">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>176</v>
+      </c>
+      <c r="D12">
+        <v>0.69</v>
+      </c>
+      <c r="E12">
+        <v>0.11</v>
+      </c>
+      <c r="F12">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.64700000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858278ED-196A-4B59-8830-674E5B382BAC}">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -1679,301 +2362,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" customWidth="1"/>
-    <col min="5" max="5" width="69" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>92</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661002B2-E508-42DE-AAF7-55B64A4B61E8}">
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating SI results tables - model outputs
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984D8A3B-4A74-4868-94AF-A53E312763AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A6E028-F3DA-4F57-BD58-EB73A9A8499D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Table 4" sheetId="6" r:id="rId4"/>
     <sheet name="Table S1" sheetId="3" r:id="rId5"/>
     <sheet name="Table S2 - CCI bands" sheetId="4" r:id="rId6"/>
+    <sheet name="Tables S3_S5" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="233">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -656,13 +658,98 @@
   </si>
   <si>
     <t>Producer price of cassava*</t>
+  </si>
+  <si>
+    <t>Economic predictors</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Macroeconomic models with ELC response</t>
+  </si>
+  <si>
+    <t>Agricultural proportion GDP</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>m.econ.top</t>
+  </si>
+  <si>
+    <t>m.econ.lag1.top</t>
+  </si>
+  <si>
+    <t>Development flows - agriculture</t>
+  </si>
+  <si>
+    <t>Model weight</t>
+  </si>
+  <si>
+    <t>Table Sx. Model coefficients from the top economic model with a 1 year time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>Table Sx. Model coefficients from the top economic model with no time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>Model averaged coefficients</t>
+  </si>
+  <si>
+    <t>Table Sx. Raw model coefficients and full averaged coefficients from the top economic models with a 2 year time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>Commodity predictors</t>
+  </si>
+  <si>
+    <t>Table Sx. Model coefficients from the top commodity model with no time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>m.com.topa</t>
+  </si>
+  <si>
+    <t>Median corn price</t>
+  </si>
+  <si>
+    <t>Non-food production index</t>
+  </si>
+  <si>
+    <t>Median rice price</t>
+  </si>
+  <si>
+    <t>Median rubber price</t>
+  </si>
+  <si>
+    <t>Median sugar price</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>Forest production</t>
+  </si>
+  <si>
+    <t>Crop production index</t>
+  </si>
+  <si>
+    <t>Table Sx. Raw model coefficients and full average coefficients from the top commodity models with 1 year time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>Table Sx. Raw model coefficients and full average coefficients from the top commodity models with 2 year time lag. Coefficeints are on the link (log) scale</t>
+  </si>
+  <si>
+    <t>(Intercept)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +782,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -722,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -735,6 +839,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1699,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908CB573-80D5-4D21-A446-EADEBAD25FBE}">
-  <dimension ref="A1:M60"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,14 +1826,15 @@
     <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" customWidth="1"/>
+    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" customWidth="1"/>
+    <col min="12" max="12" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
@@ -1731,24 +1847,26 @@
       <c r="D1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>154</v>
       </c>
@@ -1761,17 +1879,19 @@
       <c r="D3">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>-4.34</v>
       </c>
-      <c r="G3">
+      <c r="I3">
+        <f>EXP(C3)</f>
         <v>0.98511193960306265</v>
       </c>
-      <c r="H3">
+      <c r="J3">
+        <f>EXP(D3)</f>
         <v>1.0034057865562385</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>182</v>
       </c>
@@ -1784,17 +1904,19 @@
       <c r="D4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>6.43</v>
       </c>
-      <c r="G4">
+      <c r="I4">
+        <f>EXP(C4)</f>
         <v>0.97433508960874937</v>
       </c>
-      <c r="H4">
+      <c r="J4">
+        <f>EXP(D4)</f>
         <v>1.0039076148961468</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>155</v>
       </c>
@@ -1807,20 +1929,22 @@
       <c r="D5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>4.08</v>
       </c>
-      <c r="G5">
+      <c r="I5">
+        <f t="shared" ref="I5:I60" si="0">EXP(C5)</f>
         <v>1.3099644507332473</v>
       </c>
-      <c r="H5">
+      <c r="J5">
+        <f t="shared" ref="J5:J60" si="1">EXP(D5)</f>
         <v>1.0725081812542165</v>
       </c>
-      <c r="M5" t="s">
+      <c r="L5" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>155</v>
       </c>
@@ -1833,17 +1957,19 @@
       <c r="D6">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>3.83</v>
       </c>
-      <c r="G6">
+      <c r="I6">
+        <f t="shared" si="0"/>
         <v>1.2840254166877414</v>
       </c>
-      <c r="H6">
+      <c r="J6">
+        <f t="shared" si="1"/>
         <v>1.0682267171659934</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>184</v>
       </c>
@@ -1856,17 +1982,19 @@
       <c r="D7">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>0.44</v>
       </c>
-      <c r="G7">
+      <c r="I7">
+        <f t="shared" si="0"/>
         <v>0.96657150463750663</v>
       </c>
-      <c r="H7">
+      <c r="J7">
+        <f t="shared" si="1"/>
         <v>1.0789625741572839</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>187</v>
       </c>
@@ -1879,17 +2007,19 @@
       <c r="D8">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>0.2</v>
       </c>
-      <c r="G8">
+      <c r="I8">
+        <f t="shared" si="0"/>
         <v>0.99995000124997913</v>
       </c>
-      <c r="H8">
+      <c r="J8">
+        <f t="shared" si="1"/>
         <v>1.0002000200013335</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>156</v>
       </c>
@@ -1902,17 +2032,19 @@
       <c r="D9">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>7.42</v>
       </c>
-      <c r="G9">
+      <c r="I9">
+        <f t="shared" si="0"/>
         <v>1.0314855038865227</v>
       </c>
-      <c r="H9">
+      <c r="J9">
+        <f t="shared" si="1"/>
         <v>1.0040080106773419</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>185</v>
       </c>
@@ -1925,17 +2057,19 @@
       <c r="D10">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G10">
+      <c r="I10">
+        <f t="shared" si="0"/>
         <v>0.99740337707256976</v>
       </c>
-      <c r="H10">
+      <c r="J10">
+        <f t="shared" si="1"/>
         <v>1.0045101402046013</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>157</v>
       </c>
@@ -1948,17 +2082,19 @@
       <c r="D11">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>7.87</v>
       </c>
-      <c r="G11">
+      <c r="I11">
+        <f t="shared" si="0"/>
         <v>1.0036064877830035</v>
       </c>
-      <c r="H11">
+      <c r="J11">
+        <f t="shared" si="1"/>
         <v>1.0005001250208359</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>186</v>
       </c>
@@ -1971,17 +2107,19 @@
       <c r="D12">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>0.65</v>
       </c>
-      <c r="G12">
+      <c r="I12">
+        <f t="shared" si="0"/>
         <v>1.0004000800106678</v>
       </c>
-      <c r="H12">
+      <c r="J12">
+        <f t="shared" si="1"/>
         <v>1.0006001800360054</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1994,17 +2132,19 @@
       <c r="D13">
         <v>0.85</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>-5.2</v>
       </c>
-      <c r="G13">
+      <c r="I13">
+        <f t="shared" si="0"/>
         <v>1.1914489672789647E-2</v>
       </c>
-      <c r="H13">
+      <c r="J13">
+        <f t="shared" si="1"/>
         <v>2.3396468519259908</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2017,17 +2157,19 @@
       <c r="D14">
         <v>0.81</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>-7.47</v>
       </c>
-      <c r="G14">
+      <c r="I14">
+        <f t="shared" si="0"/>
         <v>2.265408914814322E-3</v>
       </c>
-      <c r="H14">
+      <c r="J14">
+        <f t="shared" si="1"/>
         <v>2.2479079866764717</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>183</v>
       </c>
@@ -2040,17 +2182,19 @@
       <c r="D15">
         <v>0.95</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>7.7</v>
       </c>
-      <c r="G15">
+      <c r="I15">
+        <f t="shared" si="0"/>
         <v>4.619748987816513E-4</v>
       </c>
-      <c r="H15">
+      <c r="J15">
+        <f t="shared" si="1"/>
         <v>2.585709659315846</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>114</v>
       </c>
@@ -2063,17 +2207,19 @@
       <c r="D16">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>-7.62</v>
       </c>
-      <c r="G16">
+      <c r="I16">
+        <f t="shared" si="0"/>
         <v>0.99970004499550036</v>
       </c>
-      <c r="H16">
+      <c r="J16">
+        <f t="shared" si="1"/>
         <v>1.0000400008000108</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>114</v>
       </c>
@@ -2086,17 +2232,19 @@
       <c r="D17">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="G17">
+      <c r="I17">
+        <f t="shared" si="0"/>
         <v>0.99996000079998937</v>
       </c>
-      <c r="H17">
+      <c r="J17">
+        <f t="shared" si="1"/>
         <v>1.0000400008000108</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>180</v>
       </c>
@@ -2109,29 +2257,33 @@
       <c r="D18">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>0.75</v>
       </c>
-      <c r="G18">
+      <c r="I18">
+        <f t="shared" si="0"/>
         <v>1.0000400008000108</v>
       </c>
-      <c r="H18">
+      <c r="J18">
+        <f t="shared" si="1"/>
         <v>1.0000500012500209</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>161</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="G19">
+      <c r="I19">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="J19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>188</v>
       </c>
@@ -2144,17 +2296,19 @@
       <c r="D20">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>4.1500000000000004</v>
       </c>
-      <c r="G20">
+      <c r="I20">
+        <f t="shared" si="0"/>
         <v>1.026340948473442</v>
       </c>
-      <c r="H20">
+      <c r="J20">
+        <f t="shared" si="1"/>
         <v>1.0062192597829778</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>193</v>
       </c>
@@ -2167,17 +2321,19 @@
       <c r="D21">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>1.08</v>
       </c>
-      <c r="G21">
+      <c r="I21">
+        <f t="shared" si="0"/>
         <v>1.0070648390547696</v>
       </c>
-      <c r="H21">
+      <c r="J21">
+        <f t="shared" si="1"/>
         <v>1.0064909756631124</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>193</v>
       </c>
@@ -2190,17 +2346,19 @@
       <c r="D22">
         <v>3.29E-3</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>1.0900000000000001</v>
       </c>
-      <c r="G22">
+      <c r="I22">
+        <f t="shared" si="0"/>
         <v>0.99635665315286914</v>
       </c>
-      <c r="H22">
+      <c r="J22">
+        <f t="shared" si="1"/>
         <v>1.0032954179900997</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>189</v>
       </c>
@@ -2213,17 +2371,19 @@
       <c r="D23">
         <v>2.8E-3</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>-2.31</v>
       </c>
-      <c r="G23">
+      <c r="I23">
+        <f t="shared" si="0"/>
         <v>0.99302444293323511</v>
       </c>
-      <c r="H23">
+      <c r="J23">
+        <f t="shared" si="1"/>
         <v>1.0028039236612292</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>196</v>
       </c>
@@ -2236,17 +2396,19 @@
       <c r="D24">
         <v>2.7200000000000002E-3</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>1.56</v>
       </c>
-      <c r="G24">
+      <c r="I24">
+        <f t="shared" si="0"/>
         <v>0.99571918890516931</v>
       </c>
-      <c r="H24">
+      <c r="J24">
+        <f t="shared" si="1"/>
         <v>1.0027237025562232</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>196</v>
       </c>
@@ -2259,17 +2421,19 @@
       <c r="D25">
         <v>5.7899999999999998E-4</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>0.06</v>
       </c>
-      <c r="G25">
+      <c r="I25">
+        <f t="shared" si="0"/>
         <v>1.0000357006372527</v>
       </c>
-      <c r="H25">
+      <c r="J25">
+        <f t="shared" si="1"/>
         <v>1.0005791676528555</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>190</v>
       </c>
@@ -2282,17 +2446,19 @@
       <c r="D26">
         <v>3.1E-4</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>-2.86</v>
       </c>
-      <c r="G26">
+      <c r="I26">
+        <f t="shared" si="0"/>
         <v>0.99910040487852736</v>
       </c>
-      <c r="H26">
+      <c r="J26">
+        <f t="shared" si="1"/>
         <v>1.0003100480549656</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>197</v>
       </c>
@@ -2305,17 +2471,19 @@
       <c r="D27">
         <v>2.206E-4</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>0.86</v>
       </c>
-      <c r="G27">
+      <c r="I27">
+        <f t="shared" si="0"/>
         <v>1.0001890178616253</v>
       </c>
-      <c r="H27">
+      <c r="J27">
+        <f t="shared" si="1"/>
         <v>1.0002206243339693</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>197</v>
       </c>
@@ -2328,17 +2496,19 @@
       <c r="D28">
         <v>9.1299999999999997E-5</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>0.4</v>
       </c>
-      <c r="G28">
+      <c r="I28">
+        <f t="shared" si="0"/>
         <v>0.9999617007334356</v>
       </c>
-      <c r="H28">
+      <c r="J28">
+        <f t="shared" si="1"/>
         <v>1.0000913041679718</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>191</v>
       </c>
@@ -2351,17 +2521,19 @@
       <c r="D29">
         <v>1.5E-3</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>8.92</v>
       </c>
-      <c r="G29">
+      <c r="I29">
+        <f t="shared" si="0"/>
         <v>1.0134496435678366</v>
       </c>
-      <c r="H29">
+      <c r="J29">
+        <f t="shared" si="1"/>
         <v>1.0015011255627111</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>194</v>
       </c>
@@ -2374,17 +2546,19 @@
       <c r="D30">
         <v>1.268E-3</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>5.23</v>
       </c>
-      <c r="G30">
+      <c r="I30">
+        <f t="shared" si="0"/>
         <v>1.0071091508825412</v>
       </c>
-      <c r="H30">
+      <c r="J30">
+        <f t="shared" si="1"/>
         <v>1.0012688042518945</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>194</v>
       </c>
@@ -2397,17 +2571,19 @@
       <c r="D31">
         <v>1.24E-3</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>6.64</v>
       </c>
-      <c r="G31">
+      <c r="I31">
+        <f t="shared" si="0"/>
         <v>1.0088085691179383</v>
       </c>
-      <c r="H31">
+      <c r="J31">
+        <f t="shared" si="1"/>
         <v>1.0012407691178693</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>192</v>
       </c>
@@ -2420,17 +2596,19 @@
       <c r="D32">
         <v>2.9499999999999999E-3</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>2.23</v>
       </c>
-      <c r="G32">
+      <c r="I32">
+        <f t="shared" si="0"/>
         <v>1.0066117618272168</v>
       </c>
-      <c r="H32">
+      <c r="J32">
+        <f t="shared" si="1"/>
         <v>1.0029543555318865</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>195</v>
       </c>
@@ -2443,17 +2621,19 @@
       <c r="D33">
         <v>2.64E-3</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>2.5099999999999998</v>
       </c>
-      <c r="G33">
+      <c r="I33">
+        <f t="shared" si="0"/>
         <v>1.0067426298624924</v>
       </c>
-      <c r="H33">
+      <c r="J33">
+        <f t="shared" si="1"/>
         <v>1.002643487868649</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>195</v>
       </c>
@@ -2466,17 +2646,19 @@
       <c r="D34">
         <v>2.0300000000000001E-3</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>0.72</v>
       </c>
-      <c r="G34">
+      <c r="I34">
+        <f t="shared" si="0"/>
         <v>0.99851110949888044</v>
       </c>
-      <c r="H34">
+      <c r="J34">
+        <f t="shared" si="1"/>
         <v>1.0020320618449456</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>199</v>
       </c>
@@ -2489,17 +2671,19 @@
       <c r="D35">
         <v>1.4400000000000001E-3</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G35">
+      <c r="I35">
+        <f t="shared" si="0"/>
         <v>1.0004220890545266</v>
       </c>
-      <c r="H35">
+      <c r="J35">
+        <f t="shared" si="1"/>
         <v>1.0014410372978433</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>199</v>
       </c>
@@ -2512,17 +2696,19 @@
       <c r="D36">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>0.76</v>
       </c>
-      <c r="G36">
+      <c r="I36">
+        <f t="shared" si="0"/>
         <v>0.99672537332356081</v>
       </c>
-      <c r="H36">
+      <c r="J36">
+        <f t="shared" si="1"/>
         <v>1.0042791294396105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>198</v>
       </c>
@@ -2535,17 +2721,19 @@
       <c r="D37">
         <v>5.0299999999999999E-7</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>0.36</v>
       </c>
-      <c r="G37">
+      <c r="I37">
+        <f t="shared" si="0"/>
         <v>1.0000001868000175</v>
       </c>
-      <c r="H37">
+      <c r="J37">
+        <f t="shared" si="1"/>
         <v>1.0000005030001264</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>198</v>
       </c>
@@ -2558,17 +2746,19 @@
       <c r="D38">
         <v>1.6E-7</v>
       </c>
-      <c r="E38">
+      <c r="G38">
         <v>0.1</v>
       </c>
-      <c r="G38">
+      <c r="I38">
+        <f t="shared" si="0"/>
         <v>0.99999998280000013</v>
       </c>
-      <c r="H38">
+      <c r="J38">
+        <f t="shared" si="1"/>
         <v>1.0000001600000128</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>114</v>
       </c>
@@ -2581,17 +2771,19 @@
       <c r="D39">
         <v>3.6600000000000002E-5</v>
       </c>
-      <c r="E39">
+      <c r="G39">
         <v>-4.63</v>
       </c>
-      <c r="G39">
+      <c r="I39">
+        <f t="shared" si="0"/>
         <v>0.99983101427969556</v>
       </c>
-      <c r="H39">
+      <c r="J39">
+        <f t="shared" si="1"/>
         <v>1.0000366006697883</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>180</v>
       </c>
@@ -2604,17 +2796,19 @@
       <c r="D40">
         <v>2.51E-5</v>
       </c>
-      <c r="E40">
+      <c r="G40">
         <v>6.49</v>
       </c>
-      <c r="G40">
+      <c r="I40">
+        <f t="shared" si="0"/>
         <v>0.99982531525915641</v>
       </c>
-      <c r="H40">
+      <c r="J40">
+        <f t="shared" si="1"/>
         <v>1.0000251003150076</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>180</v>
       </c>
@@ -2627,28 +2821,32 @@
       <c r="D41">
         <v>2.55E-5</v>
       </c>
-      <c r="E41">
+      <c r="G41">
         <v>4.76</v>
       </c>
-      <c r="G41">
+      <c r="I41">
+        <f t="shared" si="0"/>
         <v>0.99987200819165045</v>
       </c>
-      <c r="H41">
+      <c r="J41">
+        <f t="shared" si="1"/>
         <v>1.0000255003251277</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G42">
+      <c r="I42">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H42">
+      <c r="J42">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -2661,17 +2859,19 @@
       <c r="D43">
         <v>3.5500000000000002E-3</v>
       </c>
-      <c r="E43">
+      <c r="G43">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G43">
+      <c r="I43">
+        <f t="shared" si="0"/>
         <v>1.0041586231745985</v>
       </c>
-      <c r="H43">
+      <c r="J43">
+        <f t="shared" si="1"/>
         <v>1.0035563087131014</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>201</v>
       </c>
@@ -2684,17 +2884,19 @@
       <c r="D44">
         <v>2.395E-3</v>
       </c>
-      <c r="E44">
+      <c r="G44">
         <v>4.32</v>
       </c>
-      <c r="G44">
+      <c r="I44">
+        <f t="shared" si="0"/>
         <v>1.0109899506711895</v>
       </c>
-      <c r="H44">
+      <c r="J44">
+        <f t="shared" si="1"/>
         <v>1.0023978703035015</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>201</v>
       </c>
@@ -2707,17 +2909,19 @@
       <c r="D45">
         <v>8.1450000000000001E-4</v>
       </c>
-      <c r="E45">
+      <c r="G45">
         <v>0.17</v>
       </c>
-      <c r="G45">
+      <c r="I45">
+        <f t="shared" si="0"/>
         <v>1.0001439103541017</v>
       </c>
-      <c r="H45">
+      <c r="J45">
+        <f t="shared" si="1"/>
         <v>1.0008148317952013</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>200</v>
       </c>
@@ -2730,17 +2934,19 @@
       <c r="D46">
         <v>4.3600000000000002E-3</v>
       </c>
-      <c r="E46">
+      <c r="G46">
         <v>5.25</v>
       </c>
-      <c r="G46">
+      <c r="I46">
+        <f t="shared" si="0"/>
         <v>0.97565133024224471</v>
       </c>
-      <c r="H46">
+      <c r="J46">
+        <f t="shared" si="1"/>
         <v>1.0043695186287127</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>202</v>
       </c>
@@ -2753,17 +2959,19 @@
       <c r="D47">
         <v>5.6389999999999999E-3</v>
       </c>
-      <c r="E47">
+      <c r="G47">
         <v>0.95</v>
       </c>
-      <c r="G47">
+      <c r="I47">
+        <f t="shared" si="0"/>
         <v>1.0045302306083088</v>
       </c>
-      <c r="H47">
+      <c r="J47">
+        <f t="shared" si="1"/>
         <v>1.0056549290878001</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>202</v>
       </c>
@@ -2776,17 +2984,19 @@
       <c r="D48">
         <v>4.7349999999999996E-3</v>
       </c>
-      <c r="E48">
+      <c r="G48">
         <v>2.56</v>
       </c>
-      <c r="G48">
+      <c r="I48">
+        <f t="shared" si="0"/>
         <v>1.0126594610570951</v>
       </c>
-      <c r="H48">
+      <c r="J48">
+        <f t="shared" si="1"/>
         <v>1.0047462278267585</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
@@ -2799,17 +3009,19 @@
       <c r="D49">
         <v>4.0099999999999997E-3</v>
       </c>
-      <c r="E49">
+      <c r="G49">
         <v>7.93</v>
       </c>
-      <c r="G49">
+      <c r="I49">
+        <f t="shared" si="0"/>
         <v>1.0348329368321532</v>
       </c>
-      <c r="H49">
+      <c r="J49">
+        <f t="shared" si="1"/>
         <v>1.0040180508076493</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>203</v>
       </c>
@@ -2822,17 +3034,19 @@
       <c r="D50">
         <v>2.2780000000000001E-3</v>
       </c>
-      <c r="E50">
+      <c r="G50">
         <v>0.32</v>
       </c>
-      <c r="G50">
+      <c r="I50">
+        <f t="shared" si="0"/>
         <v>0.9992539784125809</v>
       </c>
-      <c r="H50">
+      <c r="J50">
+        <f t="shared" si="1"/>
         <v>1.0022805966133208</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>203</v>
       </c>
@@ -2845,17 +3059,19 @@
       <c r="D51">
         <v>4.6719999999999999E-3</v>
       </c>
-      <c r="E51">
+      <c r="G51">
         <v>0.9</v>
       </c>
-      <c r="G51">
+      <c r="I51">
+        <f t="shared" si="0"/>
         <v>0.99570425322935363</v>
       </c>
-      <c r="H51">
+      <c r="J51">
+        <f t="shared" si="1"/>
         <v>1.0046829308082825</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2868,17 +3084,19 @@
       <c r="D52">
         <v>9.7419999999999999E-5</v>
       </c>
-      <c r="E52">
+      <c r="G52">
         <v>0.35799999999999998</v>
       </c>
-      <c r="G52">
+      <c r="I52">
+        <f t="shared" si="0"/>
         <v>1.0000361306526964</v>
       </c>
-      <c r="H52">
+      <c r="J52">
+        <f t="shared" si="1"/>
         <v>1.0000974247454824</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>204</v>
       </c>
@@ -2891,17 +3109,19 @@
       <c r="D53">
         <v>1.7550000000000001E-4</v>
       </c>
-      <c r="E53">
+      <c r="G53">
         <v>0.87</v>
       </c>
-      <c r="G53">
+      <c r="I53">
+        <f t="shared" si="0"/>
         <v>1.0001564122311177</v>
       </c>
-      <c r="H53">
+      <c r="J53">
+        <f t="shared" si="1"/>
         <v>1.0001755154010259</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>204</v>
       </c>
@@ -2914,17 +3134,19 @@
       <c r="D54">
         <v>5.8400000000000003E-5</v>
       </c>
-      <c r="E54">
+      <c r="G54">
         <v>0.08</v>
       </c>
-      <c r="G54">
+      <c r="I54">
+        <f t="shared" si="0"/>
         <v>1.0000048990120001</v>
       </c>
-      <c r="H54">
+      <c r="J54">
+        <f t="shared" si="1"/>
         <v>1.0000584017053131</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>49</v>
       </c>
@@ -2937,17 +3159,19 @@
       <c r="D55">
         <v>1.2340000000000001E-3</v>
       </c>
-      <c r="E55">
+      <c r="G55">
         <v>0.25</v>
       </c>
-      <c r="G55">
+      <c r="I55">
+        <f t="shared" si="0"/>
         <v>1.0003212515902435</v>
       </c>
-      <c r="H55">
+      <c r="J55">
+        <f t="shared" si="1"/>
         <v>1.0012347616912769</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>205</v>
       </c>
@@ -2960,17 +3184,19 @@
       <c r="D56">
         <v>7.5509999999999998E-4</v>
       </c>
-      <c r="E56">
+      <c r="G56">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G56">
+      <c r="I56">
+        <f t="shared" si="0"/>
         <v>1.0000555515429299</v>
       </c>
-      <c r="H56">
+      <c r="J56">
+        <f t="shared" si="1"/>
         <v>1.0007553851597752</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>205</v>
       </c>
@@ -2983,17 +3209,19 @@
       <c r="D57">
         <v>2.1419999999999998E-3</v>
       </c>
-      <c r="E57">
+      <c r="G57">
         <v>7.81</v>
       </c>
-      <c r="G57">
+      <c r="I57">
+        <f t="shared" si="0"/>
         <v>0.98224943082908445</v>
       </c>
-      <c r="H57">
+      <c r="J57">
+        <f t="shared" si="1"/>
         <v>1.002144295720852</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>114</v>
       </c>
@@ -3006,17 +3234,19 @@
       <c r="D58">
         <v>2.3779999999999999E-5</v>
       </c>
-      <c r="E58">
+      <c r="G58">
         <v>8.81</v>
       </c>
-      <c r="G58">
+      <c r="I58">
+        <f t="shared" si="0"/>
         <v>0.99977342567184091</v>
       </c>
-      <c r="H58">
+      <c r="J58">
+        <f t="shared" si="1"/>
         <v>1.0000237802827465</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>180</v>
       </c>
@@ -3029,17 +3259,19 @@
       <c r="D59">
         <v>2.124E-5</v>
       </c>
-      <c r="E59">
+      <c r="G59">
         <v>6.71</v>
       </c>
-      <c r="G59">
+      <c r="I59">
+        <f t="shared" si="0"/>
         <v>0.99984711168860929</v>
       </c>
-      <c r="H59">
+      <c r="J59">
+        <f t="shared" si="1"/>
         <v>1.0000212402255704</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>180</v>
       </c>
@@ -3052,13 +3284,15 @@
       <c r="D60">
         <v>2.035E-5</v>
       </c>
-      <c r="E60">
+      <c r="G60">
         <v>6.01</v>
       </c>
-      <c r="G60">
+      <c r="I60">
+        <f t="shared" si="0"/>
         <v>0.99986930854087286</v>
       </c>
-      <c r="H60">
+      <c r="J60">
+        <f t="shared" si="1"/>
         <v>1.0000203502070626</v>
       </c>
     </row>
@@ -3955,4 +4189,2929 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED94DC-32EE-4CB2-B393-F68209908457}">
+  <dimension ref="A1:K58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="12">
+        <v>33.24</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="D8" s="12">
+        <v>3.134E-2</v>
+      </c>
+      <c r="E8" s="12">
+        <v>-2.786E-4</v>
+      </c>
+      <c r="F8" s="12">
+        <v>-4.431</v>
+      </c>
+      <c r="G8" s="12">
+        <v>2.7829999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="12">
+        <v>14.27</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.25380000000000003</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3.5560000000000001E-3</v>
+      </c>
+      <c r="E14" s="12">
+        <v>-1.473E-2</v>
+      </c>
+      <c r="F14" s="12">
+        <v>-4.3730000000000003E-5</v>
+      </c>
+      <c r="G14" s="12">
+        <v>-6.0869999999999997</v>
+      </c>
+      <c r="H14" s="12">
+        <v>1.892E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>241</v>
+      </c>
+      <c r="B20" s="15">
+        <v>6.6577263465689303</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" s="13">
+        <v>7.1648600465405699E-5</v>
+      </c>
+      <c r="H20" s="13">
+        <v>-2.42075494754182E-2</v>
+      </c>
+      <c r="I20" s="13">
+        <v>-7.9423267642772997</v>
+      </c>
+      <c r="J20" s="13">
+        <v>-7.5531829857057304E-4</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0.10369970956619</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>225</v>
+      </c>
+      <c r="B21" s="15">
+        <v>12.294263524564601</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="13">
+        <v>-2.3538523362456501E-2</v>
+      </c>
+      <c r="I21" s="13">
+        <v>-7.24144472475116</v>
+      </c>
+      <c r="J21" s="13">
+        <v>-7.2160075516953495E-4</v>
+      </c>
+      <c r="K21" s="12">
+        <v>9.8063920429909995E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>226</v>
+      </c>
+      <c r="B22" s="15">
+        <v>12.681351200019201</v>
+      </c>
+      <c r="C22" s="13">
+        <v>-0.15479254954763999</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="13">
+        <v>-2.9557149153573201E-2</v>
+      </c>
+      <c r="I22" s="13">
+        <v>-7.4997735820671299</v>
+      </c>
+      <c r="J22" s="13">
+        <v>-1.1510724777572701E-3</v>
+      </c>
+      <c r="K22" s="12">
+        <v>8.4483626762579603E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>253</v>
+      </c>
+      <c r="B23" s="15">
+        <v>4.4330242111632501</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="13">
+        <v>-9.4680115383093504E-3</v>
+      </c>
+      <c r="F23" s="13">
+        <v>1.2398333558075101E-3</v>
+      </c>
+      <c r="G23" s="13">
+        <v>9.2561581580113804E-5</v>
+      </c>
+      <c r="H23" s="13">
+        <v>-2.7419728027834801E-2</v>
+      </c>
+      <c r="I23" s="13">
+        <v>-7.69757585848867</v>
+      </c>
+      <c r="J23" s="13">
+        <v>-7.7929173315284105E-4</v>
+      </c>
+      <c r="K23" s="12">
+        <v>6.9131053949685606E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>249</v>
+      </c>
+      <c r="B24" s="15">
+        <v>4.67480715503984</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="13">
+        <v>8.1348750630312703E-4</v>
+      </c>
+      <c r="G24" s="13">
+        <v>9.4741896471335797E-5</v>
+      </c>
+      <c r="H24" s="13">
+        <v>-2.5967536329348902E-2</v>
+      </c>
+      <c r="I24" s="13">
+        <v>-8.0650988940893207</v>
+      </c>
+      <c r="J24" s="13">
+        <v>-6.6113227206490396E-4</v>
+      </c>
+      <c r="K24" s="12">
+        <v>6.2257467290390001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>229</v>
+      </c>
+      <c r="B25" s="15">
+        <v>12.075408022277101</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="13">
+        <v>-5.6700453113410704E-3</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="13">
+        <v>-2.3928355840988801E-2</v>
+      </c>
+      <c r="I25" s="13">
+        <v>-7.0486481585438101</v>
+      </c>
+      <c r="J25" s="13">
+        <v>-8.4592551481215902E-4</v>
+      </c>
+      <c r="K25" s="12">
+        <v>5.2644899787010799E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>237</v>
+      </c>
+      <c r="B26" s="15">
+        <v>11.6489307228752</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="13">
+        <v>-9.4456062827953206E-3</v>
+      </c>
+      <c r="F26" s="13">
+        <v>9.5611753879598497E-4</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="13">
+        <v>-2.59805811501236E-2</v>
+      </c>
+      <c r="I26" s="13">
+        <v>-6.7264443885076401</v>
+      </c>
+      <c r="J26" s="13">
+        <v>-7.92430951473976E-4</v>
+      </c>
+      <c r="K26" s="12">
+        <v>4.75310252839828E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>242</v>
+      </c>
+      <c r="B27" s="15">
+        <v>7.8104871363126698</v>
+      </c>
+      <c r="C27" s="13">
+        <v>-0.123407849611191</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="13">
+        <v>6.0940222758079997E-5</v>
+      </c>
+      <c r="H27" s="13">
+        <v>-2.8870193294159099E-2</v>
+      </c>
+      <c r="I27" s="13">
+        <v>-8.0462249642338808</v>
+      </c>
+      <c r="J27" s="13">
+        <v>-1.09943859255636E-3</v>
+      </c>
+      <c r="K27" s="12">
+        <v>3.96086377869743E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>121</v>
+      </c>
+      <c r="B28" s="15">
+        <v>5.4593661315485198</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1.04373354744386E-3</v>
+      </c>
+      <c r="G28" s="13">
+        <v>9.5321676272091703E-5</v>
+      </c>
+      <c r="H28" s="13">
+        <v>-2.68998931477973E-2</v>
+      </c>
+      <c r="I28" s="13">
+        <v>-8.7292321274126294</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K28" s="12">
+        <v>3.6312562219110701E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>230</v>
+      </c>
+      <c r="B29" s="15">
+        <v>12.4974292082817</v>
+      </c>
+      <c r="C29" s="13">
+        <v>-0.15724169888539299</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E29" s="13">
+        <v>-5.7950050633008296E-3</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" s="13">
+        <v>-3.0063609147960298E-2</v>
+      </c>
+      <c r="I29" s="13">
+        <v>-7.33506951800954</v>
+      </c>
+      <c r="J29" s="13">
+        <v>-1.2870486487244601E-3</v>
+      </c>
+      <c r="K29" s="12">
+        <v>3.6182080213633297E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>245</v>
+      </c>
+      <c r="B30" s="15">
+        <v>6.8089900938854404</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="13">
+        <v>-5.2819613727082496E-3</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="13">
+        <v>6.72446699777052E-5</v>
+      </c>
+      <c r="H30" s="13">
+        <v>-2.44744725164967E-2</v>
+      </c>
+      <c r="I30" s="13">
+        <v>-7.7281006020100804</v>
+      </c>
+      <c r="J30" s="13">
+        <v>-8.6746128446837597E-4</v>
+      </c>
+      <c r="K30" s="12">
+        <v>3.58931195948324E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>233</v>
+      </c>
+      <c r="B31" s="15">
+        <v>12.144384309126</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F31" s="13">
+        <v>4.7291213656367403E-4</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" s="13">
+        <v>-2.4366398949382799E-2</v>
+      </c>
+      <c r="I31" s="13">
+        <v>-7.1384868200544904</v>
+      </c>
+      <c r="J31" s="13">
+        <v>-6.6618935106226105E-4</v>
+      </c>
+      <c r="K31" s="12">
+        <v>3.0916377696869099E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>97</v>
+      </c>
+      <c r="B32" s="15">
+        <v>13.3254718425282</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="13">
+        <v>-2.4037808586488199E-2</v>
+      </c>
+      <c r="I32" s="13">
+        <v>-8.05183496003513</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K32" s="12">
+        <v>2.5130877274107101E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>125</v>
+      </c>
+      <c r="B33" s="15">
+        <v>5.3159384844634996</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="13">
+        <v>-7.4109468305472801E-3</v>
+      </c>
+      <c r="F33" s="13">
+        <v>1.4568061713278501E-3</v>
+      </c>
+      <c r="G33" s="13">
+        <v>9.3367015204468695E-5</v>
+      </c>
+      <c r="H33" s="13">
+        <v>-2.82291875475233E-2</v>
+      </c>
+      <c r="I33" s="13">
+        <v>-8.4592073469413496</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K33" s="12">
+        <v>2.13686829816273E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>227</v>
+      </c>
+      <c r="B34" s="15">
+        <v>12.3835530399621</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D34" s="13">
+        <v>-2.4453325781880299E-4</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" s="13">
+        <v>-2.3972950810061299E-2</v>
+      </c>
+      <c r="I34" s="13">
+        <v>-7.2998882306830799</v>
+      </c>
+      <c r="J34" s="13">
+        <v>-6.821480915003E-4</v>
+      </c>
+      <c r="K34" s="12">
+        <v>1.9328435801142001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>234</v>
+      </c>
+      <c r="B35" s="15">
+        <v>12.5208330495347</v>
+      </c>
+      <c r="C35" s="13">
+        <v>-0.14983924993961301</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="13">
+        <v>4.4772922791313998E-4</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H35" s="13">
+        <v>-3.01329537740333E-2</v>
+      </c>
+      <c r="I35" s="13">
+        <v>-7.3885129602676498</v>
+      </c>
+      <c r="J35" s="13">
+        <v>-1.07716197419668E-3</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1.9283139700367401E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>113</v>
+      </c>
+      <c r="B36" s="15">
+        <v>8.5041803061742804</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="13">
+        <v>6.1533708927344802E-5</v>
+      </c>
+      <c r="H36" s="13">
+        <v>-2.4697564191045601E-2</v>
+      </c>
+      <c r="I36" s="13">
+        <v>-8.66697458306278</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1.9011487577530399E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>238</v>
+      </c>
+      <c r="B37" s="15">
+        <v>12.070499048719199</v>
+      </c>
+      <c r="C37" s="13">
+        <v>-0.140027557369508</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="13">
+        <v>-8.9676385623647503E-3</v>
+      </c>
+      <c r="F37" s="13">
+        <v>8.7383872263720099E-4</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="13">
+        <v>-3.1215926060276698E-2</v>
+      </c>
+      <c r="I37" s="13">
+        <v>-7.0167813566364403</v>
+      </c>
+      <c r="J37" s="13">
+        <v>-1.17204946675765E-3</v>
+      </c>
+      <c r="K37" s="12">
+        <v>1.77576668004794E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>105</v>
+      </c>
+      <c r="B38" s="15">
+        <v>13.0176117905841</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="13">
+        <v>6.6076221538480099E-4</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="13">
+        <v>-2.5123953674202702E-2</v>
+      </c>
+      <c r="I38" s="13">
+        <v>-7.8316152342105596</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1.7180574260496101E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>243</v>
+      </c>
+      <c r="B39" s="15">
+        <v>6.7374969803151696</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="13">
+        <v>-2.4462953605274099E-4</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G39" s="13">
+        <v>7.1695751216051994E-5</v>
+      </c>
+      <c r="H39" s="13">
+        <v>-2.4636392139545701E-2</v>
+      </c>
+      <c r="I39" s="13">
+        <v>-7.9971533983548797</v>
+      </c>
+      <c r="J39" s="13">
+        <v>-7.2402608464253095E-4</v>
+      </c>
+      <c r="K39" s="12">
+        <v>1.57303525698427E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>109</v>
+      </c>
+      <c r="B40" s="15">
+        <v>12.6735063020949</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="13">
+        <v>-7.4615269574088297E-3</v>
+      </c>
+      <c r="F40" s="13">
+        <v>1.11406284596919E-3</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="13">
+        <v>-2.6571362829857701E-2</v>
+      </c>
+      <c r="I40" s="13">
+        <v>-7.5429681708158904</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K40" s="12">
+        <v>1.35886053493911E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>250</v>
+      </c>
+      <c r="B41" s="15">
+        <v>5.9130404840911197</v>
+      </c>
+      <c r="C41" s="13">
+        <v>-0.104083585193199</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="13">
+        <v>7.3919704540352201E-4</v>
+      </c>
+      <c r="G41" s="13">
+        <v>8.2315466738116798E-5</v>
+      </c>
+      <c r="H41" s="13">
+        <v>-2.9683023745793902E-2</v>
+      </c>
+      <c r="I41" s="13">
+        <v>-8.1155767707103408</v>
+      </c>
+      <c r="J41" s="13">
+        <v>-9.5288950996885605E-4</v>
+      </c>
+      <c r="K41" s="12">
+        <v>1.3290977639491001E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>228</v>
+      </c>
+      <c r="B42" s="15">
+        <v>12.676274577639299</v>
+      </c>
+      <c r="C42" s="13">
+        <v>-0.156226536764355</v>
+      </c>
+      <c r="D42" s="13">
+        <v>2.71724197963771E-5</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" s="13">
+        <v>-2.95644358117562E-2</v>
+      </c>
+      <c r="I42" s="13">
+        <v>-7.4967131034113699</v>
+      </c>
+      <c r="J42" s="13">
+        <v>-1.1591593178791599E-3</v>
+      </c>
+      <c r="K42" s="12">
+        <v>1.14501712440759E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>246</v>
+      </c>
+      <c r="B43" s="15">
+        <v>8.0203339871518704</v>
+      </c>
+      <c r="C43" s="13">
+        <v>-0.127003228075976</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="13">
+        <v>-5.4197533202280596E-3</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G43" s="13">
+        <v>5.6145190790488502E-5</v>
+      </c>
+      <c r="H43" s="13">
+        <v>-2.9303015231557199E-2</v>
+      </c>
+      <c r="I43" s="13">
+        <v>-7.8494799162363202</v>
+      </c>
+      <c r="J43" s="13">
+        <v>-1.22560394929741E-3</v>
+      </c>
+      <c r="K43" s="12">
+        <v>1.04828078025496E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>99</v>
+      </c>
+      <c r="B44" s="15">
+        <v>13.4388269266975</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="13">
+        <v>-5.5017061103566705E-4</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H44" s="13">
+        <v>-2.48774005887232E-2</v>
+      </c>
+      <c r="I44" s="13">
+        <v>-8.1184155681197492</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K44" s="12">
+        <v>1.03570121158232E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>123</v>
+      </c>
+      <c r="B45" s="15">
+        <v>5.63090314394272</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D45" s="13">
+        <v>-6.3102050734726504E-4</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="13">
+        <v>1.06294836481853E-3</v>
+      </c>
+      <c r="G45" s="13">
+        <v>9.4965203320998394E-5</v>
+      </c>
+      <c r="H45" s="13">
+        <v>-2.7854430119676799E-2</v>
+      </c>
+      <c r="I45" s="13">
+        <v>-8.8157156323637107</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K45" s="12">
+        <v>9.8734750089715592E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>231</v>
+      </c>
+      <c r="B46" s="15">
+        <v>12.171173031553501</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="13">
+        <v>-2.9759219701262898E-4</v>
+      </c>
+      <c r="E46" s="13">
+        <v>-5.8051286756944697E-3</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H46" s="13">
+        <v>-2.44530880427603E-2</v>
+      </c>
+      <c r="I46" s="13">
+        <v>-7.1093851380961404</v>
+      </c>
+      <c r="J46" s="13">
+        <v>-8.0597360612797103E-4</v>
+      </c>
+      <c r="K46" s="12">
+        <v>8.5991097839925208E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>254</v>
+      </c>
+      <c r="B47" s="15">
+        <v>5.6025796726485897</v>
+      </c>
+      <c r="C47" s="13">
+        <v>-9.0519285187150703E-2</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="13">
+        <v>-9.0234633673697603E-3</v>
+      </c>
+      <c r="F47" s="13">
+        <v>1.13428279413161E-3</v>
+      </c>
+      <c r="G47" s="13">
+        <v>8.1037451407073495E-5</v>
+      </c>
+      <c r="H47" s="13">
+        <v>-3.0529916241988801E-2</v>
+      </c>
+      <c r="I47" s="13">
+        <v>-7.7639240338047397</v>
+      </c>
+      <c r="J47" s="13">
+        <v>-1.03021480695148E-3</v>
+      </c>
+      <c r="K47" s="12">
+        <v>8.2371824929863106E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>251</v>
+      </c>
+      <c r="B48" s="15">
+        <v>4.7405965613938097</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="13">
+        <v>-3.2486580329555402E-4</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="13">
+        <v>8.3795146436588101E-4</v>
+      </c>
+      <c r="G48" s="13">
+        <v>9.52927508930287E-5</v>
+      </c>
+      <c r="H48" s="13">
+        <v>-2.6570649158355001E-2</v>
+      </c>
+      <c r="I48" s="13">
+        <v>-8.1428597275327199</v>
+      </c>
+      <c r="J48" s="13">
+        <v>-6.1781215362750202E-4</v>
+      </c>
+      <c r="K48" s="12">
+        <v>7.40536508342451E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>101</v>
+      </c>
+      <c r="B49" s="15">
+        <v>13.2774792284053</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="13">
+        <v>-2.6660184680529901E-3</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" s="13">
+        <v>-2.42549642058799E-2</v>
+      </c>
+      <c r="I49" s="13">
+        <v>-8.0029682184913096</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K49" s="12">
+        <v>7.0639181431942097E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>255</v>
+      </c>
+      <c r="B50" s="15">
+        <v>4.4650647516263398</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="13">
+        <v>-4.8887287634538797E-4</v>
+      </c>
+      <c r="E50" s="13">
+        <v>-9.7926065182413497E-3</v>
+      </c>
+      <c r="F50" s="13">
+        <v>1.29238423285232E-3</v>
+      </c>
+      <c r="G50" s="13">
+        <v>9.3889233407591305E-5</v>
+      </c>
+      <c r="H50" s="13">
+        <v>-2.8345270948966501E-2</v>
+      </c>
+      <c r="I50" s="13">
+        <v>-7.7978803419517204</v>
+      </c>
+      <c r="J50" s="13">
+        <v>-7.2829487411157304E-4</v>
+      </c>
+      <c r="K50" s="12">
+        <v>6.8425154033204504E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>239</v>
+      </c>
+      <c r="B51" s="15">
+        <v>11.772844411233301</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D51" s="13">
+        <v>-4.2121711391996601E-4</v>
+      </c>
+      <c r="E51" s="13">
+        <v>-9.7137823412995206E-3</v>
+      </c>
+      <c r="F51" s="13">
+        <v>1.0041589878974401E-3</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H51" s="13">
+        <v>-2.6788463591373501E-2</v>
+      </c>
+      <c r="I51" s="13">
+        <v>-6.80544189071923</v>
+      </c>
+      <c r="J51" s="13">
+        <v>-7.3195599159088499E-4</v>
+      </c>
+      <c r="K51" s="12">
+        <v>6.6078853556245402E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>115</v>
+      </c>
+      <c r="B52" s="15">
+        <v>8.6599622378655603</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="13">
+        <v>-5.6432670583311101E-4</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G52" s="13">
+        <v>6.1210817841934195E-5</v>
+      </c>
+      <c r="H52" s="13">
+        <v>-2.5536739734570501E-2</v>
+      </c>
+      <c r="I52" s="13">
+        <v>-8.7445392436269493</v>
+      </c>
+      <c r="J52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K52" s="12">
+        <v>6.2290666616617203E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>107</v>
+      </c>
+      <c r="B53" s="15">
+        <v>13.1317421457767</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="13">
+        <v>-5.9611506646303997E-4</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="13">
+        <v>6.8571184326861399E-4</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H53" s="13">
+        <v>-2.60709986132115E-2</v>
+      </c>
+      <c r="I53" s="13">
+        <v>-7.8980992213254702</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K53" s="12">
+        <v>6.1678476538054496E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>127</v>
+      </c>
+      <c r="B54" s="15">
+        <v>5.4869233586800901</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="13">
+        <v>-8.08014833098685E-4</v>
+      </c>
+      <c r="E54" s="13">
+        <v>-8.1188975348640002E-3</v>
+      </c>
+      <c r="F54" s="13">
+        <v>1.5217425200530199E-3</v>
+      </c>
+      <c r="G54" s="13">
+        <v>9.3348382710313704E-5</v>
+      </c>
+      <c r="H54" s="13">
+        <v>-2.9526736574810201E-2</v>
+      </c>
+      <c r="I54" s="13">
+        <v>-8.5635486249797097</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K54" s="12">
+        <v>6.1171839569778797E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>98</v>
+      </c>
+      <c r="B55" s="15">
+        <v>13.264139940151299</v>
+      </c>
+      <c r="C55" s="13">
+        <v>8.9829134755711904E-3</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H55" s="13">
+        <v>-2.36883778462245E-2</v>
+      </c>
+      <c r="I55" s="13">
+        <v>-8.0057129234447792</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K55" s="12">
+        <v>5.4243807458146803E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>122</v>
+      </c>
+      <c r="B56" s="15">
+        <v>5.0029054002102598</v>
+      </c>
+      <c r="C56" s="13">
+        <v>2.6828033598519801E-2</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" s="13">
+        <v>1.02953965311668E-3</v>
+      </c>
+      <c r="G56" s="13">
+        <v>9.9072559212344796E-5</v>
+      </c>
+      <c r="H56" s="13">
+        <v>-2.5880938015084998E-2</v>
+      </c>
+      <c r="I56" s="13">
+        <v>-8.6452582072973403</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K56" s="12">
+        <v>5.4187318417726399E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>111</v>
+      </c>
+      <c r="B57" s="15">
+        <v>12.8032078068348</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="13">
+        <v>-7.4800084455504598E-4</v>
+      </c>
+      <c r="E57" s="13">
+        <v>-8.14013893829061E-3</v>
+      </c>
+      <c r="F57" s="13">
+        <v>1.1865087032122399E-3</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H57" s="13">
+        <v>-2.7831736519945E-2</v>
+      </c>
+      <c r="I57" s="13">
+        <v>-7.6164145003573998</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K57" s="12">
+        <v>5.3280661703617197E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B58" s="12">
+        <v>9.3680000000000003</v>
+      </c>
+      <c r="C58" s="12">
+        <v>-3.4090000000000002E-2</v>
+      </c>
+      <c r="D58" s="12">
+        <v>-4.7410000000000002E-5</v>
+      </c>
+      <c r="E58" s="12">
+        <v>-2.6440000000000001E-3</v>
+      </c>
+      <c r="F58" s="12">
+        <v>3.9290000000000001E-4</v>
+      </c>
+      <c r="G58" s="12">
+        <v>3.8430000000000003E-5</v>
+      </c>
+      <c r="H58" s="12">
+        <v>-2.631E-2</v>
+      </c>
+      <c r="I58" s="12">
+        <v>-7.6840000000000002</v>
+      </c>
+      <c r="J58" s="12">
+        <v>-7.002E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B568554-EE5E-4148-B92D-3C63A1452433}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="12">
+        <v>17.18</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2.5569999999999999E-2</v>
+      </c>
+      <c r="D9" s="12">
+        <v>6.5979999999999997E-3</v>
+      </c>
+      <c r="E9" s="12">
+        <v>-6.5440000000000003E-3</v>
+      </c>
+      <c r="F9" s="12">
+        <v>-8.9479999999999996E-4</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1.336E-2</v>
+      </c>
+      <c r="H9" s="12">
+        <v>-1.698</v>
+      </c>
+      <c r="I9" s="12">
+        <v>5.0750000000000003E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" t="s">
+        <v>227</v>
+      </c>
+      <c r="C13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K13" t="s">
+        <v>210</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>186</v>
+      </c>
+      <c r="B15" s="13">
+        <v>19.009683355491202</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1.29608290177501E-2</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="13">
+        <v>-1.84532899937581E-4</v>
+      </c>
+      <c r="G15" s="13">
+        <v>8.9895527555435301E-3</v>
+      </c>
+      <c r="H15" s="13">
+        <v>-6.7625486018793599E-3</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J15" s="13">
+        <v>7.3849377864736903E-3</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L15" s="12">
+        <v>0.266233744495813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
+        <v>249</v>
+      </c>
+      <c r="B16" s="13">
+        <v>17.791917474132401</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="13">
+        <v>-1.7143199173686401E-4</v>
+      </c>
+      <c r="G16" s="13">
+        <v>4.09785003072615E-3</v>
+      </c>
+      <c r="H16" s="13">
+        <v>-1.5871515486556901E-3</v>
+      </c>
+      <c r="I16" s="13">
+        <v>4.39231821585213E-4</v>
+      </c>
+      <c r="J16" s="13">
+        <v>6.72550356216593E-3</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0.178477643773784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>250</v>
+      </c>
+      <c r="B17" s="13">
+        <v>18.238780266223401</v>
+      </c>
+      <c r="C17" s="13">
+        <v>7.2257116178215302E-3</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="13">
+        <v>-1.7614452199371801E-4</v>
+      </c>
+      <c r="G17" s="13">
+        <v>6.7506961184131001E-3</v>
+      </c>
+      <c r="H17" s="13">
+        <v>-4.4415916510793501E-3</v>
+      </c>
+      <c r="I17" s="13">
+        <v>2.2030303542616499E-4</v>
+      </c>
+      <c r="J17" s="13">
+        <v>6.8796476315811997E-3</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L17" s="12">
+        <v>8.1447073791342306E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>446</v>
+      </c>
+      <c r="B18" s="13">
+        <v>16.292790577390001</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1.09740411901045E-2</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1.41862161101489E-6</v>
+      </c>
+      <c r="F18" s="13">
+        <v>-1.5489787022817899E-4</v>
+      </c>
+      <c r="G18" s="13">
+        <v>8.4352556606180195E-3</v>
+      </c>
+      <c r="H18" s="13">
+        <v>-5.5961388582716001E-3</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J18" s="13">
+        <v>8.1371661521309306E-3</v>
+      </c>
+      <c r="K18" s="13">
+        <v>7.0453351777090495E-4</v>
+      </c>
+      <c r="L18" s="12">
+        <v>8.0380629516945801E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>442</v>
+      </c>
+      <c r="B19" s="13">
+        <v>18.933888188050801</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1.27204007729679E-2</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" s="13">
+        <v>-1.83613354627066E-4</v>
+      </c>
+      <c r="G19" s="13">
+        <v>9.2651727566647798E-3</v>
+      </c>
+      <c r="H19" s="13">
+        <v>-6.7871509061906699E-3</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19" s="13">
+        <v>7.4565847270431198E-3</v>
+      </c>
+      <c r="K19" s="13">
+        <v>3.6907273823718299E-4</v>
+      </c>
+      <c r="L19" s="12">
+        <v>7.3310335878910393E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>251</v>
+      </c>
+      <c r="B20" s="13">
+        <v>17.249397001262501</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3.8451081773854799E-3</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="13">
+        <v>-1.6666525775224701E-4</v>
+      </c>
+      <c r="G20" s="13">
+        <v>4.1277007854361204E-3</v>
+      </c>
+      <c r="H20" s="13">
+        <v>-1.9347858632567899E-3</v>
+      </c>
+      <c r="I20" s="13">
+        <v>4.0482648807792102E-4</v>
+      </c>
+      <c r="J20" s="13">
+        <v>5.9564273387460098E-3</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L20" s="12">
+        <v>7.2547265918478904E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>190</v>
+      </c>
+      <c r="B21" s="13">
+        <v>17.891599666362001</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1.2108022021667501E-2</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" s="13">
+        <v>7.23686347282587E-7</v>
+      </c>
+      <c r="F21" s="13">
+        <v>-1.72433083556121E-4</v>
+      </c>
+      <c r="G21" s="13">
+        <v>8.3822834474565101E-3</v>
+      </c>
+      <c r="H21" s="13">
+        <v>-6.0963889412872204E-3</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J21" s="13">
+        <v>7.6684196861511204E-3</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" s="12">
+        <v>6.9527526338365897E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>188</v>
+      </c>
+      <c r="B22" s="13">
+        <v>18.5920030366721</v>
+      </c>
+      <c r="C22" s="13">
+        <v>1.2207173055958E-2</v>
+      </c>
+      <c r="D22" s="13">
+        <v>2.0443801661234398E-3</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="13">
+        <v>-1.80610406572904E-4</v>
+      </c>
+      <c r="G22" s="13">
+        <v>8.7601465733685192E-3</v>
+      </c>
+      <c r="H22" s="13">
+        <v>-6.66542893793201E-3</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J22" s="13">
+        <v>7.0199032768215397E-3</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L22" s="12">
+        <v>4.0171754058928102E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>218</v>
+      </c>
+      <c r="B23" s="13">
+        <v>17.811374600908302</v>
+      </c>
+      <c r="C23" s="13">
+        <v>-2.75211460807106E-3</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="13">
+        <v>-1.71820579369805E-4</v>
+      </c>
+      <c r="G23" s="13">
+        <v>2.8246973996307301E-3</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" s="13">
+        <v>5.2987624187635801E-4</v>
+      </c>
+      <c r="J23" s="13">
+        <v>6.6093939776072199E-3</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L23" s="12">
+        <v>3.2169456070832797E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>217</v>
+      </c>
+      <c r="B24" s="13">
+        <v>17.982687422475699</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="13">
+        <v>-1.7365512747779201E-4</v>
+      </c>
+      <c r="G24" s="13">
+        <v>3.13788101386714E-3</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" s="13">
+        <v>4.5986822953149602E-4</v>
+      </c>
+      <c r="J24" s="13">
+        <v>6.35203075536448E-3</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L24" s="12">
+        <v>3.0135542544931199E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>253</v>
+      </c>
+      <c r="B25" s="13">
+        <v>17.3599049168132</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="13">
+        <v>3.0202037120308401E-7</v>
+      </c>
+      <c r="F25" s="13">
+        <v>-1.6676584263045999E-4</v>
+      </c>
+      <c r="G25" s="13">
+        <v>3.9975876375509898E-3</v>
+      </c>
+      <c r="H25" s="13">
+        <v>-1.45756291327818E-3</v>
+      </c>
+      <c r="I25" s="13">
+        <v>4.22830045051132E-4</v>
+      </c>
+      <c r="J25" s="13">
+        <v>6.90671508065428E-3</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L25" s="12">
+        <v>2.26474393626315E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>505</v>
+      </c>
+      <c r="B26" s="13">
+        <v>17.848673967184599</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="13">
+        <v>-1.7203748206080601E-4</v>
+      </c>
+      <c r="G26" s="13">
+        <v>4.2449302038568898E-3</v>
+      </c>
+      <c r="H26" s="13">
+        <v>-1.6423675450923201E-3</v>
+      </c>
+      <c r="I26" s="13">
+        <v>4.30725117609008E-4</v>
+      </c>
+      <c r="J26" s="13">
+        <v>6.8075216947054203E-3</v>
+      </c>
+      <c r="K26" s="13">
+        <v>1.2572313639363399E-4</v>
+      </c>
+      <c r="L26" s="12">
+        <v>2.1730668619851401E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>221</v>
+      </c>
+      <c r="B27" s="13">
+        <v>16.911549401152701</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="13">
+        <v>9.5109173465066103E-7</v>
+      </c>
+      <c r="F27" s="13">
+        <v>-1.6215742624764499E-4</v>
+      </c>
+      <c r="G27" s="13">
+        <v>3.1039446438607802E-3</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I27" s="13">
+        <v>4.0263140725682801E-4</v>
+      </c>
+      <c r="J27" s="13">
+        <v>7.0342366376967601E-3</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1.6463050402586301E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>220</v>
+      </c>
+      <c r="B28" s="13">
+        <v>17.224218560369501</v>
+      </c>
+      <c r="C28" s="13">
+        <v>-3.9155880576206897E-3</v>
+      </c>
+      <c r="D28" s="13">
+        <v>4.1841045266635003E-3</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="13">
+        <v>-1.66687416045079E-4</v>
+      </c>
+      <c r="G28" s="13">
+        <v>2.4886482796275598E-3</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I28" s="13">
+        <v>5.2644999811742998E-4</v>
+      </c>
+      <c r="J28" s="13">
+        <v>5.7417922381403502E-3</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="L28" s="12">
+        <v>1.47578692265985E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="12">
+        <v>18.09</v>
+      </c>
+      <c r="C29" s="12">
+        <v>7.0400000000000003E-3</v>
+      </c>
+      <c r="D29" s="12">
+        <v>4.2279999999999998E-4</v>
+      </c>
+      <c r="E29" s="12">
+        <v>1.8680000000000001E-7</v>
+      </c>
+      <c r="F29" s="12">
+        <v>-1.7469999999999999E-4</v>
+      </c>
+      <c r="G29" s="12">
+        <v>6.7219999999999997E-3</v>
+      </c>
+      <c r="H29" s="12">
+        <v>-4.2940000000000001E-3</v>
+      </c>
+      <c r="I29" s="12">
+        <v>1.8990000000000001E-4</v>
+      </c>
+      <c r="J29" s="12">
+        <v>7.084E-3</v>
+      </c>
+      <c r="K29" s="12">
+        <v>8.6420000000000003E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" t="s">
+        <v>222</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E33" t="s">
+        <v>228</v>
+      </c>
+      <c r="F33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="K33" t="s">
+        <v>210</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>410</v>
+      </c>
+      <c r="B35" s="13">
+        <v>12.2030866660689</v>
+      </c>
+      <c r="C35" s="13">
+        <v>-6.7019935890024699E-3</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F35" s="13">
+        <v>-1.1118693345988001E-4</v>
+      </c>
+      <c r="G35" s="13">
+        <v>-3.6025136466945299E-3</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J35" s="13">
+        <v>8.18196829626564E-3</v>
+      </c>
+      <c r="K35" s="13">
+        <v>-1.1024210994762E-3</v>
+      </c>
+      <c r="L35">
+        <v>0.290088335638363</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>395</v>
+      </c>
+      <c r="B36" s="13">
+        <v>16.331518985578501</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="13">
+        <v>-9.2205756109065493E-3</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F36" s="13">
+        <v>-1.5286706634028499E-4</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J36" s="13">
+        <v>9.7018334379725905E-3</v>
+      </c>
+      <c r="K36" s="13">
+        <v>-8.8792403223106504E-4</v>
+      </c>
+      <c r="L36">
+        <v>0.133297053622733</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>459</v>
+      </c>
+      <c r="B37" s="13">
+        <v>15.177145875226801</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D37" s="13">
+        <v>-6.7163087448920402E-3</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="13">
+        <v>-1.4083336345925901E-4</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I37" s="13">
+        <v>-1.7429952558927801E-4</v>
+      </c>
+      <c r="J37" s="13">
+        <v>9.6427767895367993E-3</v>
+      </c>
+      <c r="K37" s="13">
+        <v>-8.0688455088703196E-4</v>
+      </c>
+      <c r="L37">
+        <v>0.12458991421073499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>396</v>
+      </c>
+      <c r="B38" s="13">
+        <v>14.7796214596646</v>
+      </c>
+      <c r="C38" s="13">
+        <v>-3.0024683268318102E-3</v>
+      </c>
+      <c r="D38" s="13">
+        <v>-5.8202868137717401E-3</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="13">
+        <v>-1.3683483081216799E-4</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J38" s="13">
+        <v>9.1604464318543102E-3</v>
+      </c>
+      <c r="K38" s="13">
+        <v>-7.9094434579269799E-4</v>
+      </c>
+      <c r="L38">
+        <v>9.0814849494256097E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>394</v>
+      </c>
+      <c r="B39" s="13">
+        <v>13.4169021279987</v>
+      </c>
+      <c r="C39" s="13">
+        <v>-4.8970846317684903E-3</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F39" s="13">
+        <v>-1.23464167016551E-4</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" s="13">
+        <v>8.0177530532582197E-3</v>
+      </c>
+      <c r="K39" s="13">
+        <v>-7.9967030200243396E-4</v>
+      </c>
+      <c r="L39">
+        <v>8.8559745096395096E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>457</v>
+      </c>
+      <c r="B40" s="13">
+        <v>13.6913485165172</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" s="13">
+        <v>-1.26274995775291E-4</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" s="13">
+        <v>-2.7754840618315701E-4</v>
+      </c>
+      <c r="J40" s="13">
+        <v>8.5616687138373102E-3</v>
+      </c>
+      <c r="K40" s="13">
+        <v>-8.4000287358655798E-4</v>
+      </c>
+      <c r="L40">
+        <v>3.9086879040320002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>442</v>
+      </c>
+      <c r="B41" s="13">
+        <v>12.668914949325</v>
+      </c>
+      <c r="C41" s="13">
+        <v>-7.8816161433989708E-3</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="13">
+        <v>-1.1614389368061701E-4</v>
+      </c>
+      <c r="G41" s="13">
+        <v>-3.72582925220617E-3</v>
+      </c>
+      <c r="H41" s="13">
+        <v>1.4845949725894099E-3</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J41" s="13">
+        <v>8.3059087769866997E-3</v>
+      </c>
+      <c r="K41" s="13">
+        <v>-1.10556489826584E-3</v>
+      </c>
+      <c r="L41">
+        <v>3.55257783815522E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>414</v>
+      </c>
+      <c r="B42" s="13">
+        <v>12.548012938183501</v>
+      </c>
+      <c r="C42" s="13">
+        <v>-6.6835771811303499E-3</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="13">
+        <v>-3.4227810960955603E-7</v>
+      </c>
+      <c r="F42" s="13">
+        <v>-1.14899608093455E-4</v>
+      </c>
+      <c r="G42" s="13">
+        <v>-3.6521784818772502E-3</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J42" s="13">
+        <v>7.9971310623995605E-3</v>
+      </c>
+      <c r="K42" s="13">
+        <v>-1.2008813565588801E-3</v>
+      </c>
+      <c r="L42">
+        <v>3.3274437595173602E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>412</v>
+      </c>
+      <c r="B43" s="13">
+        <v>12.8706734877037</v>
+      </c>
+      <c r="C43" s="13">
+        <v>-5.7333571960685404E-3</v>
+      </c>
+      <c r="D43" s="13">
+        <v>-2.0100716640069202E-3</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F43" s="13">
+        <v>-1.1779100757794399E-4</v>
+      </c>
+      <c r="G43" s="13">
+        <v>-2.9951338928099099E-3</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" s="13">
+        <v>8.5515852096896793E-3</v>
+      </c>
+      <c r="K43" s="13">
+        <v>-1.0485054959573001E-3</v>
+      </c>
+      <c r="L43">
+        <v>3.3108590822126999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>474</v>
+      </c>
+      <c r="B44" s="13">
+        <v>12.203412151650101</v>
+      </c>
+      <c r="C44" s="13">
+        <v>-6.6987750581719401E-3</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="13">
+        <v>-1.11189944282559E-4</v>
+      </c>
+      <c r="G44" s="13">
+        <v>-3.6011187443048798E-3</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I44" s="13">
+        <v>-2.1970005569780001E-7</v>
+      </c>
+      <c r="J44" s="13">
+        <v>8.1822602798279093E-3</v>
+      </c>
+      <c r="K44" s="13">
+        <v>-1.10227617282494E-3</v>
+      </c>
+      <c r="L44">
+        <v>2.8861098774862599E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>458</v>
+      </c>
+      <c r="B45" s="13">
+        <v>13.362492790886799</v>
+      </c>
+      <c r="C45" s="13">
+        <v>-3.2835830629038701E-3</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="13">
+        <v>-1.22792049285E-4</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I45" s="13">
+        <v>-1.36845196802897E-4</v>
+      </c>
+      <c r="J45" s="13">
+        <v>8.2983232930694591E-3</v>
+      </c>
+      <c r="K45" s="13">
+        <v>-7.8439712462329599E-4</v>
+      </c>
+      <c r="L45">
+        <v>2.6801590006555201E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>427</v>
+      </c>
+      <c r="B46" s="13">
+        <v>15.712482738359499</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="13">
+        <v>-8.3779499907201908E-3</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" s="13">
+        <v>-1.4643067424642401E-4</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H46" s="13">
+        <v>-8.3198412283799598E-4</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J46" s="13">
+        <v>9.4998563183490703E-3</v>
+      </c>
+      <c r="K46" s="13">
+        <v>-8.7572285577487404E-4</v>
+      </c>
+      <c r="L46">
+        <v>2.0473486954457502E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>399</v>
+      </c>
+      <c r="B47" s="13">
+        <v>16.692819279833</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D47" s="13">
+        <v>-9.1529615648768096E-3</v>
+      </c>
+      <c r="E47" s="13">
+        <v>-2.8587048338658701E-7</v>
+      </c>
+      <c r="F47" s="13">
+        <v>-1.56789502445103E-4</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J47" s="13">
+        <v>9.5337004311087693E-3</v>
+      </c>
+      <c r="K47" s="13">
+        <v>-9.7464282233480795E-4</v>
+      </c>
+      <c r="L47">
+        <v>2.0290060899236601E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>411</v>
+      </c>
+      <c r="B48" s="13">
+        <v>16.364609687305101</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="13">
+        <v>-9.24282117747139E-3</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F48" s="13">
+        <v>-1.53167102547072E-4</v>
+      </c>
+      <c r="G48" s="13">
+        <v>2.0694220439543E-4</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J48" s="13">
+        <v>9.7054910083236405E-3</v>
+      </c>
+      <c r="K48" s="13">
+        <v>-8.6381988833561995E-4</v>
+      </c>
+      <c r="L48">
+        <v>1.8285093453651501E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>460</v>
+      </c>
+      <c r="B49" s="13">
+        <v>14.701126711804999</v>
+      </c>
+      <c r="C49" s="13">
+        <v>-1.6307691413593099E-3</v>
+      </c>
+      <c r="D49" s="13">
+        <v>-5.6138266669088404E-3</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F49" s="13">
+        <v>-1.3595817354291299E-4</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I49" s="13">
+        <v>-1.21901158409955E-4</v>
+      </c>
+      <c r="J49" s="13">
+        <v>9.3525931796689405E-3</v>
+      </c>
+      <c r="K49" s="13">
+        <v>-7.7968330795068598E-4</v>
+      </c>
+      <c r="L49">
+        <v>1.6943086009582099E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" s="11">
+        <v>13.89</v>
+      </c>
+      <c r="C50" s="11">
+        <v>-3.6519999999999999E-3</v>
+      </c>
+      <c r="D50" s="11">
+        <v>-3.2820000000000002E-3</v>
+      </c>
+      <c r="E50" s="11">
+        <v>-1.719E-8</v>
+      </c>
+      <c r="F50" s="11">
+        <v>-1.281E-4</v>
+      </c>
+      <c r="G50" s="11">
+        <v>-1.498E-3</v>
+      </c>
+      <c r="H50" s="11">
+        <v>3.5710000000000002E-5</v>
+      </c>
+      <c r="I50" s="11">
+        <v>-3.8300000000000003E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added SM table of all socioecon models
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9CD3FE-CA08-4B7E-8BD6-5E0EDDF0CC5E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EECEF36-BCFE-4B8B-B080-C3B383D7AF74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" activeTab="4" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="7" activeTab="13" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Tables S12_S14" sheetId="11" r:id="rId11"/>
     <sheet name="Tables S15_S17" sheetId="12" r:id="rId12"/>
     <sheet name="Tables S18_S20" sheetId="13" r:id="rId13"/>
+    <sheet name="Table S21" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="321">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -834,6 +835,180 @@
   </si>
   <si>
     <t>Presence of PAs (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commune-level </t>
+  </si>
+  <si>
+    <t>Set-specific models</t>
+  </si>
+  <si>
+    <t>Population demographics</t>
+  </si>
+  <si>
+    <t>popdem.m1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proportion indigenous </t>
+  </si>
+  <si>
+    <t>popdem.m2</t>
+  </si>
+  <si>
+    <t>edu.m1</t>
+  </si>
+  <si>
+    <t>Proportion males in school</t>
+  </si>
+  <si>
+    <t>emp.m1</t>
+  </si>
+  <si>
+    <t>emp.m2</t>
+  </si>
+  <si>
+    <t>Proportion primary sector</t>
+  </si>
+  <si>
+    <t>Proportion secondary sector</t>
+  </si>
+  <si>
+    <t>econ.m1</t>
+  </si>
+  <si>
+    <t>econ.m2</t>
+  </si>
+  <si>
+    <t>Proportion no farmland</t>
+  </si>
+  <si>
+    <t>Proportion with pigs</t>
+  </si>
+  <si>
+    <t>acc.m1</t>
+  </si>
+  <si>
+    <t>acc.m2</t>
+  </si>
+  <si>
+    <t>acc.m3</t>
+  </si>
+  <si>
+    <t>Distance to school</t>
+  </si>
+  <si>
+    <t>Access to waste collection</t>
+  </si>
+  <si>
+    <t>Distance to commune office</t>
+  </si>
+  <si>
+    <t>Social Justice</t>
+  </si>
+  <si>
+    <t>jus.m1</t>
+  </si>
+  <si>
+    <t>jus.m2</t>
+  </si>
+  <si>
+    <t>Criminal cases</t>
+  </si>
+  <si>
+    <t>Land conflicts</t>
+  </si>
+  <si>
+    <t>mig.m1</t>
+  </si>
+  <si>
+    <t>mig.m2</t>
+  </si>
+  <si>
+    <t>Out-migration</t>
+  </si>
+  <si>
+    <t>In-migration *</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ** all models included offset</t>
+  </si>
+  <si>
+    <t>* represents an interaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In-migration </t>
+  </si>
+  <si>
+    <t>mig.m3</t>
+  </si>
+  <si>
+    <t>mig.m4</t>
+  </si>
+  <si>
+    <t>env.m1</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>hum.m1</t>
+  </si>
+  <si>
+    <t>hum.m2</t>
+  </si>
+  <si>
+    <t>Distance to Int'l border</t>
+  </si>
+  <si>
+    <t>Distance to provincial capital</t>
+  </si>
+  <si>
+    <t>Presence of ELC</t>
+  </si>
+  <si>
+    <t>Presence of PA</t>
+  </si>
+  <si>
+    <t>PA category</t>
+  </si>
+  <si>
+    <t>Final candidate model set</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>m5</t>
+  </si>
+  <si>
+    <t>m6</t>
+  </si>
+  <si>
+    <t>m7</t>
+  </si>
+  <si>
+    <t>m8</t>
+  </si>
+  <si>
+    <t>distance to school</t>
+  </si>
+  <si>
+    <t>m9</t>
+  </si>
+  <si>
+    <t>Propotion primary sector</t>
+  </si>
+  <si>
+    <t>m10</t>
   </si>
 </sst>
 </file>
@@ -845,7 +1020,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +1064,14 @@
     <font>
       <b/>
       <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -973,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1022,6 +1205,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8086,6 +8277,543 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
+  <dimension ref="A1:I40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" t="s">
+        <v>283</v>
+      </c>
+      <c r="D15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" t="s">
+        <v>293</v>
+      </c>
+      <c r="C22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B23" t="s">
+        <v>296</v>
+      </c>
+      <c r="C23" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="B25" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B28" t="s">
+        <v>303</v>
+      </c>
+      <c r="C28" t="s">
+        <v>304</v>
+      </c>
+      <c r="D28" t="s">
+        <v>305</v>
+      </c>
+      <c r="E28" t="s">
+        <v>306</v>
+      </c>
+      <c r="F28" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>300</v>
+      </c>
+      <c r="D31" t="s">
+        <v>303</v>
+      </c>
+      <c r="E31" t="s">
+        <v>304</v>
+      </c>
+      <c r="F31" t="s">
+        <v>305</v>
+      </c>
+      <c r="G31" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="C32" t="s">
+        <v>300</v>
+      </c>
+      <c r="D32" t="s">
+        <v>303</v>
+      </c>
+      <c r="E32" t="s">
+        <v>304</v>
+      </c>
+      <c r="F32" t="s">
+        <v>305</v>
+      </c>
+      <c r="G32" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="C33" t="s">
+        <v>300</v>
+      </c>
+      <c r="D33" t="s">
+        <v>303</v>
+      </c>
+      <c r="E33" t="s">
+        <v>304</v>
+      </c>
+      <c r="F33" t="s">
+        <v>305</v>
+      </c>
+      <c r="G33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="C34" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" t="s">
+        <v>303</v>
+      </c>
+      <c r="E34" t="s">
+        <v>304</v>
+      </c>
+      <c r="F34" t="s">
+        <v>305</v>
+      </c>
+      <c r="G34" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="C35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D35" t="s">
+        <v>303</v>
+      </c>
+      <c r="E35" t="s">
+        <v>304</v>
+      </c>
+      <c r="F35" t="s">
+        <v>305</v>
+      </c>
+      <c r="G35" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B36" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="C36" t="s">
+        <v>300</v>
+      </c>
+      <c r="D36" t="s">
+        <v>303</v>
+      </c>
+      <c r="E36" t="s">
+        <v>304</v>
+      </c>
+      <c r="F36" t="s">
+        <v>305</v>
+      </c>
+      <c r="G36" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C37" t="s">
+        <v>300</v>
+      </c>
+      <c r="D37" t="s">
+        <v>303</v>
+      </c>
+      <c r="E37" t="s">
+        <v>304</v>
+      </c>
+      <c r="F37" t="s">
+        <v>305</v>
+      </c>
+      <c r="G37" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>270</v>
+      </c>
+      <c r="C38" t="s">
+        <v>317</v>
+      </c>
+      <c r="D38" t="s">
+        <v>300</v>
+      </c>
+      <c r="E38" t="s">
+        <v>303</v>
+      </c>
+      <c r="F38" t="s">
+        <v>304</v>
+      </c>
+      <c r="G38" t="s">
+        <v>305</v>
+      </c>
+      <c r="H38" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B39" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="C39" t="s">
+        <v>292</v>
+      </c>
+      <c r="D39" t="s">
+        <v>300</v>
+      </c>
+      <c r="E39" t="s">
+        <v>303</v>
+      </c>
+      <c r="F39" t="s">
+        <v>304</v>
+      </c>
+      <c r="G39" t="s">
+        <v>305</v>
+      </c>
+      <c r="H39" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>270</v>
+      </c>
+      <c r="D40" t="s">
+        <v>300</v>
+      </c>
+      <c r="E40" t="s">
+        <v>303</v>
+      </c>
+      <c r="F40" t="s">
+        <v>304</v>
+      </c>
+      <c r="G40" t="s">
+        <v>305</v>
+      </c>
+      <c r="H40" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92F3726-DBC4-4CC1-932D-C346E9CAF478}">
   <dimension ref="A1:E22"/>
@@ -9803,7 +10531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Completed SM table of all socioecon models
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EECEF36-BCFE-4B8B-B080-C3B383D7AF74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ABFF8A-9F9B-4DD4-9784-141329E3DDFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="7" activeTab="13" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="340">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -924,6 +924,9 @@
     <t>mig.m2</t>
   </si>
   <si>
+    <t>In-migration</t>
+  </si>
+  <si>
     <t>Out-migration</t>
   </si>
   <si>
@@ -1009,6 +1012,60 @@
   </si>
   <si>
     <t>m10</t>
+  </si>
+  <si>
+    <t>Province level (categorical)</t>
+  </si>
+  <si>
+    <t>Males in school</t>
+  </si>
+  <si>
+    <t>Primary sector</t>
+  </si>
+  <si>
+    <t>Pig ownership</t>
+  </si>
+  <si>
+    <t>popden.mcat</t>
+  </si>
+  <si>
+    <t>socjus.mcat</t>
+  </si>
+  <si>
+    <t>mig.mcat</t>
+  </si>
+  <si>
+    <t>edu.mcat</t>
+  </si>
+  <si>
+    <t>emp.mcat</t>
+  </si>
+  <si>
+    <t>Secondary sector</t>
+  </si>
+  <si>
+    <t>econ.mcat</t>
+  </si>
+  <si>
+    <t>No farmland</t>
+  </si>
+  <si>
+    <t>Owns pigs</t>
+  </si>
+  <si>
+    <t>acc.mcat</t>
+  </si>
+  <si>
+    <t>elev.mcat</t>
+  </si>
+  <si>
+    <t>hum.mcat</t>
+  </si>
+  <si>
+    <t>areas.mcat</t>
+  </si>
+  <si>
+    <t>Presence of PAs</t>
   </si>
 </sst>
 </file>
@@ -8279,15 +8336,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="3" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="6" width="24.77734375" bestFit="1" customWidth="1"/>
@@ -8305,7 +8362,7 @@
         <v>264</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -8330,7 +8387,7 @@
         <v>267</v>
       </c>
       <c r="I4" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -8341,7 +8398,7 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -8478,10 +8535,10 @@
         <v>290</v>
       </c>
       <c r="B22" t="s">
+        <v>294</v>
+      </c>
+      <c r="C22" t="s">
         <v>293</v>
-      </c>
-      <c r="C22" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -8489,26 +8546,26 @@
         <v>291</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B25" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -8518,98 +8575,98 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E28" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F28" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B31" s="31" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D31" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E31" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F31" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G31" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B32" s="31" t="s">
         <v>270</v>
       </c>
       <c r="C32" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D32" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E32" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F32" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G32" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -8620,168 +8677,168 @@
         <v>273</v>
       </c>
       <c r="C33" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D33" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E33" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F33" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G33" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B34" s="31" t="s">
         <v>278</v>
       </c>
       <c r="C34" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D34" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E34" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F34" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G34" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>282</v>
       </c>
       <c r="C35" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D35" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E35" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F35" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G35" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B36" s="31" t="s">
         <v>288</v>
       </c>
       <c r="C36" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E36" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F36" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G36" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C37" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D37" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="E37" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F37" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G37" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B38" s="31" t="s">
         <v>270</v>
       </c>
       <c r="C38" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D38" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E38" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F38" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G38" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H38" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C39" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D39" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E39" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F39" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="G39" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="H39" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B40" s="31" t="s">
         <v>22</v>
@@ -8790,19 +8847,335 @@
         <v>270</v>
       </c>
       <c r="D40" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="E40" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F40" t="s">
+        <v>305</v>
+      </c>
+      <c r="G40" t="s">
+        <v>306</v>
+      </c>
+      <c r="H40" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="C43" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="C44" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="C46" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="C47" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B50" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="G40" t="s">
+      <c r="C50" t="s">
         <v>305</v>
       </c>
-      <c r="H40" t="s">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B51" s="31" t="s">
         <v>306</v>
+      </c>
+      <c r="C51" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>301</v>
+      </c>
+      <c r="D52" t="s">
+        <v>304</v>
+      </c>
+      <c r="E52" t="s">
+        <v>305</v>
+      </c>
+      <c r="F52" t="s">
+        <v>306</v>
+      </c>
+      <c r="G52" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" t="s">
+        <v>323</v>
+      </c>
+      <c r="C53" t="s">
+        <v>301</v>
+      </c>
+      <c r="D53" t="s">
+        <v>304</v>
+      </c>
+      <c r="E53" t="s">
+        <v>305</v>
+      </c>
+      <c r="F53" t="s">
+        <v>306</v>
+      </c>
+      <c r="G53" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>324</v>
+      </c>
+      <c r="C54" t="s">
+        <v>301</v>
+      </c>
+      <c r="D54" t="s">
+        <v>304</v>
+      </c>
+      <c r="E54" t="s">
+        <v>305</v>
+      </c>
+      <c r="F54" t="s">
+        <v>306</v>
+      </c>
+      <c r="G54" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B55" t="s">
+        <v>325</v>
+      </c>
+      <c r="C55" t="s">
+        <v>301</v>
+      </c>
+      <c r="D55" t="s">
+        <v>304</v>
+      </c>
+      <c r="E55" t="s">
+        <v>305</v>
+      </c>
+      <c r="F55" t="s">
+        <v>306</v>
+      </c>
+      <c r="G55" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B56" t="s">
+        <v>282</v>
+      </c>
+      <c r="C56" t="s">
+        <v>301</v>
+      </c>
+      <c r="D56" t="s">
+        <v>304</v>
+      </c>
+      <c r="E56" t="s">
+        <v>305</v>
+      </c>
+      <c r="F56" t="s">
+        <v>306</v>
+      </c>
+      <c r="G56" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B57" t="s">
+        <v>288</v>
+      </c>
+      <c r="C57" t="s">
+        <v>301</v>
+      </c>
+      <c r="D57" t="s">
+        <v>304</v>
+      </c>
+      <c r="E57" t="s">
+        <v>305</v>
+      </c>
+      <c r="F57" t="s">
+        <v>306</v>
+      </c>
+      <c r="G57" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B58" t="s">
+        <v>293</v>
+      </c>
+      <c r="C58" t="s">
+        <v>301</v>
+      </c>
+      <c r="D58" t="s">
+        <v>304</v>
+      </c>
+      <c r="E58" t="s">
+        <v>305</v>
+      </c>
+      <c r="F58" t="s">
+        <v>306</v>
+      </c>
+      <c r="G58" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B59" t="s">
+        <v>323</v>
+      </c>
+      <c r="C59" t="s">
+        <v>318</v>
+      </c>
+      <c r="D59" t="s">
+        <v>301</v>
+      </c>
+      <c r="E59" t="s">
+        <v>304</v>
+      </c>
+      <c r="F59" t="s">
+        <v>305</v>
+      </c>
+      <c r="G59" t="s">
+        <v>306</v>
+      </c>
+      <c r="H59" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B60" t="s">
+        <v>324</v>
+      </c>
+      <c r="C60" t="s">
+        <v>293</v>
+      </c>
+      <c r="D60" t="s">
+        <v>301</v>
+      </c>
+      <c r="E60" t="s">
+        <v>304</v>
+      </c>
+      <c r="F60" t="s">
+        <v>305</v>
+      </c>
+      <c r="G60" t="s">
+        <v>306</v>
+      </c>
+      <c r="H60" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tables updated and results section structure updated
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ABFF8A-9F9B-4DD4-9784-141329E3DDFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784F6521-F7EA-4E34-8016-4AA616A6A3D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="7" activeTab="13" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="4" activeTab="4" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -8338,7 +8338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -10904,7 +10904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixing errors with variable tables
Moving population density and forest remaining to control variables, and editing the methods text to reflect this. Fixing errors in the text relating to number of variables etc. Fucking concentrate next time.
Now I need to remove pop_den from the macroecon plots (forest loss as response). See "results summary" doc
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A33649-476C-4095-858D-E2E7A891A080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE689D-E6FB-41A3-BAE3-AC172F8751C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="766" activeTab="4" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" activeTab="5" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D7CE8D-180E-4CEC-92B5-D81875E97DBC}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11000,7 +11000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11346,10 +11346,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858278ED-196A-4B59-8830-674E5B382BAC}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11519,20 +11519,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
@@ -11784,6 +11770,20 @@
       </c>
       <c r="E28" s="2" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -12054,7 +12054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED94DC-32EE-4CB2-B393-F68209908457}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -13619,7 +13619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B568554-EE5E-4148-B92D-3C63A1452433}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added sheet to ID largest effects
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEE689D-E6FB-41A3-BAE3-AC172F8751C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66EAF9-FF9D-47B7-8E15-2AB7772FC1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" activeTab="5" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="6" activeTab="10" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,8 @@
     <sheet name="Tables S12_S14" sheetId="11" r:id="rId11"/>
     <sheet name="Tables S15_S17" sheetId="12" r:id="rId12"/>
     <sheet name="Tables S18_S20" sheetId="13" r:id="rId13"/>
-    <sheet name="Table S21" sheetId="14" r:id="rId14"/>
+    <sheet name="Largest_effects" sheetId="15" r:id="rId14"/>
+    <sheet name="Table S21" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="351">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -753,9 +754,6 @@
     <t>Macroeconomic models with Forest Cover response</t>
   </si>
   <si>
-    <t>Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with no time lag. Coefficeints are on the link (log) scale</t>
-  </si>
-  <si>
     <t>Table Sx. Raw model coefficients and full average coefficients from the top producer price models (dAIC &lt;6) with no time lag. Coefficeints are on the link (log) scale</t>
   </si>
   <si>
@@ -777,9 +775,6 @@
     <t>GDP growth</t>
   </si>
   <si>
-    <t>Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with 1 year time lag. Coefficeints are on the link (log) scale</t>
-  </si>
-  <si>
     <t>Table Sx. Raw model coefficients and full averaged coefficients from the top commodity models (dAIC &lt; 6) with no time lag. Coefficeints are on the link (log) scale</t>
   </si>
   <si>
@@ -1066,16 +1061,56 @@
   </si>
   <si>
     <t>Presence of PAs</t>
+  </si>
+  <si>
+    <t>Forest cover respsonse</t>
+  </si>
+  <si>
+    <t>Econ no lag</t>
+  </si>
+  <si>
+    <t>econ 1 year lag</t>
+  </si>
+  <si>
+    <t>econ 2 year lag</t>
+  </si>
+  <si>
+    <t>commodity no lag</t>
+  </si>
+  <si>
+    <t>commodity 1 year lag</t>
+  </si>
+  <si>
+    <t>commodity 2 year lag</t>
+  </si>
+  <si>
+    <t>producer no lag</t>
+  </si>
+  <si>
+    <t>producer 1 year lag</t>
+  </si>
+  <si>
+    <t>producer 2 year lag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with no time lag. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with 1 year time lag. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with 2 year time lag. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1213,7 +1248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1269,6 +1304,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1973,7 +2014,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2362,7 +2403,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3039,7 +3080,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -3490,1290 +3531,1659 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C9C45A-A9C7-442D-AE82-61DCD6C978E2}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.77734375" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" customWidth="1"/>
+    <col min="17" max="17" width="5.44140625" customWidth="1"/>
+    <col min="18" max="18" width="15.77734375" customWidth="1"/>
+    <col min="19" max="19" width="6.44140625" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" customWidth="1"/>
+    <col min="21" max="21" width="5.77734375" customWidth="1"/>
+    <col min="22" max="22" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
     </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>224</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G6" t="s">
+      <c r="K6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" t="s">
         <v>113</v>
       </c>
-      <c r="H6" t="s">
+      <c r="M6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N6" t="s">
         <v>153</v>
       </c>
-      <c r="I6" t="s">
-        <v>242</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="O6" t="s">
+        <v>159</v>
+      </c>
+      <c r="P6" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>159</v>
+      </c>
+      <c r="R6" t="s">
         <v>22</v>
       </c>
-      <c r="K6" t="s">
+      <c r="S6" t="s">
+        <v>159</v>
+      </c>
+      <c r="T6" t="s">
         <v>205</v>
       </c>
-      <c r="L6" t="s">
+      <c r="U6" t="s">
+        <v>159</v>
+      </c>
+      <c r="V6" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>401</v>
       </c>
       <c r="B8" s="11">
         <v>-6308.3030343853698</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E8" s="11"/>
       <c r="F8" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11">
         <v>8.4559885706867594E-2</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="M8" s="11"/>
+      <c r="N8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11">
         <v>-599.40449984545796</v>
       </c>
-      <c r="K8" s="11">
+      <c r="S8" s="11"/>
+      <c r="T8" s="11">
         <v>1.069884203999</v>
       </c>
-      <c r="L8" s="11">
+      <c r="U8" s="11"/>
+      <c r="V8" s="11">
         <v>0.38318454094990001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>403</v>
       </c>
       <c r="B9" s="11">
         <v>-6309.3054759343804</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11">
         <v>3.1687146317798502E-2</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11">
         <v>8.4572168725124006E-2</v>
       </c>
-      <c r="H9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="M9" s="11"/>
+      <c r="N9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11">
         <v>-599.55993059887703</v>
       </c>
-      <c r="K9" s="11">
+      <c r="S9" s="11"/>
+      <c r="T9" s="11">
         <v>1.0663151600044301</v>
       </c>
-      <c r="L9" s="11">
+      <c r="U9" s="11"/>
+      <c r="V9" s="11">
         <v>0.10532750448926501</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>433</v>
       </c>
       <c r="B10" s="11">
         <v>-6415.6669186009003</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E10" s="11"/>
       <c r="F10" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11">
         <v>8.5521342124284694E-2</v>
       </c>
-      <c r="H10" s="11">
+      <c r="M10" s="11"/>
+      <c r="N10" s="11">
         <v>0.406390633113557</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J10" s="11">
+      <c r="O10" s="11"/>
+      <c r="P10" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11">
         <v>-595.85651814227197</v>
       </c>
-      <c r="K10" s="11">
+      <c r="S10" s="11"/>
+      <c r="T10" s="11">
         <v>1.0676859302886501</v>
       </c>
-      <c r="L10" s="11">
+      <c r="U10" s="11"/>
+      <c r="V10" s="11">
         <v>0.100650949675003</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>402</v>
       </c>
       <c r="B11" s="11">
         <v>-6311.9879119696097</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11">
         <v>-3.7761443316380001</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11">
         <v>8.4640895569966207E-2</v>
       </c>
-      <c r="H11" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J11" s="11">
+      <c r="M11" s="11"/>
+      <c r="N11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11">
         <v>-605.29680317580699</v>
       </c>
-      <c r="K11" s="11">
+      <c r="S11" s="11"/>
+      <c r="T11" s="11">
         <v>1.0621905847242801</v>
       </c>
-      <c r="L11" s="11">
+      <c r="U11" s="11"/>
+      <c r="V11" s="11">
         <v>6.0672586039059402E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>405</v>
       </c>
       <c r="B12" s="11">
         <v>-6302.7892806128002</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11">
         <v>0.18397128136112001</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="I12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11">
         <v>8.4467743934626596E-2</v>
       </c>
-      <c r="H12" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J12" s="11">
+      <c r="M12" s="11"/>
+      <c r="N12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11">
         <v>-597.45033186743001</v>
       </c>
-      <c r="K12" s="11">
+      <c r="S12" s="11"/>
+      <c r="T12" s="11">
         <v>1.0708287089774899</v>
       </c>
-      <c r="L12" s="11">
+      <c r="U12" s="11"/>
+      <c r="V12" s="11">
         <v>5.6946570890238503E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>465</v>
       </c>
       <c r="B13" s="11">
         <v>-6299.4243811653696</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C13" s="11"/>
       <c r="D13" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E13" s="11"/>
       <c r="F13" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11">
         <v>8.4439259986960502E-2</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I13" s="11">
+      <c r="M13" s="11"/>
+      <c r="N13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11">
         <v>-1.0351048775199201</v>
       </c>
-      <c r="J13" s="11">
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11">
         <v>-597.87412681642104</v>
       </c>
-      <c r="K13" s="11">
+      <c r="S13" s="11"/>
+      <c r="T13" s="11">
         <v>1.07430847380711</v>
       </c>
-      <c r="L13" s="11">
+      <c r="U13" s="11"/>
+      <c r="V13" s="11">
         <v>5.5848885640612897E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>409</v>
       </c>
       <c r="B14" s="11">
         <v>-6313.1017999754704</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11">
         <v>1.11549242118668E-2</v>
       </c>
-      <c r="G14" s="11">
+      <c r="K14" s="11"/>
+      <c r="L14" s="11">
         <v>8.4564625199625501E-2</v>
       </c>
-      <c r="H14" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J14" s="11">
+      <c r="M14" s="11"/>
+      <c r="N14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11">
         <v>-596.83542901517296</v>
       </c>
-      <c r="K14" s="11">
+      <c r="S14" s="11"/>
+      <c r="T14" s="11">
         <v>1.07120450761708</v>
       </c>
-      <c r="L14" s="11">
+      <c r="U14" s="11"/>
+      <c r="V14" s="11">
         <v>5.0235415343249101E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>497</v>
       </c>
       <c r="B15" s="11">
         <v>-6456.2504986620197</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C15" s="11"/>
       <c r="D15" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E15" s="11"/>
       <c r="F15" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G15" s="11"/>
+      <c r="H15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11">
         <v>8.5776758226278199E-2</v>
       </c>
-      <c r="H15" s="11">
+      <c r="M15" s="11"/>
+      <c r="N15" s="11">
         <v>0.64829432385031804</v>
       </c>
-      <c r="I15" s="11">
+      <c r="O15" s="11"/>
+      <c r="P15" s="11">
         <v>-2.71927435962463</v>
       </c>
-      <c r="J15" s="11">
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11">
         <v>-589.72421538852905</v>
       </c>
-      <c r="K15" s="11">
+      <c r="S15" s="11"/>
+      <c r="T15" s="11">
         <v>1.07800019660462</v>
       </c>
-      <c r="L15" s="11">
+      <c r="U15" s="11"/>
+      <c r="V15" s="11">
         <v>2.3110921911661701E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>435</v>
       </c>
       <c r="B16" s="11">
         <v>-6418.8962276665497</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="11">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11">
         <v>3.2303523471663001E-2</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G16" s="11">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11">
         <v>8.5553631316205497E-2</v>
       </c>
-      <c r="H16" s="11">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11">
         <v>0.41474589811565299</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J16" s="11">
+      <c r="O16" s="11"/>
+      <c r="P16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11">
         <v>-595.94202692858505</v>
       </c>
-      <c r="K16" s="11">
+      <c r="S16" s="11"/>
+      <c r="T16" s="11">
         <v>1.0640022655636201</v>
       </c>
-      <c r="L16" s="11">
+      <c r="U16" s="11"/>
+      <c r="V16" s="11">
         <v>2.1588103832451602E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="32">
         <v>-6327</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="32">
+        <v>167.5</v>
+      </c>
+      <c r="D17" s="32">
         <v>-0.26719999999999999</v>
       </c>
-      <c r="D17" s="11">
+      <c r="E17" s="32">
+        <v>1.911</v>
+      </c>
+      <c r="F17" s="32">
         <v>4.705E-3</v>
       </c>
-      <c r="E17" s="11">
+      <c r="G17" s="32">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="H17" s="32">
         <v>1.222E-2</v>
       </c>
-      <c r="F17" s="11">
-        <v>6.5339999999999998</v>
-      </c>
-      <c r="G17" s="11">
+      <c r="I17" s="32">
+        <v>0.1014</v>
+      </c>
+      <c r="J17" s="32">
+        <v>6.5340000000000005E-4</v>
+      </c>
+      <c r="K17" s="32">
+        <v>9.6550000000000004E-3</v>
+      </c>
+      <c r="L17" s="32">
         <v>8.4720000000000004E-2</v>
       </c>
-      <c r="H17" s="11">
+      <c r="M17" s="33">
+        <v>2.2339999999999999E-3</v>
+      </c>
+      <c r="N17" s="32">
         <v>7.5609999999999997E-2</v>
       </c>
-      <c r="I17" s="11">
+      <c r="O17" s="32">
+        <v>0.23280000000000001</v>
+      </c>
+      <c r="P17" s="32">
         <v>-0.14069999999999999</v>
       </c>
-      <c r="J17" s="11">
+      <c r="Q17" s="32">
+        <v>0.82130000000000003</v>
+      </c>
+      <c r="R17" s="32">
         <v>-598.70000000000005</v>
       </c>
-      <c r="K17" s="11">
+      <c r="S17" s="32">
+        <v>46.15</v>
+      </c>
+      <c r="T17" s="32">
         <v>1.069</v>
       </c>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U17" s="32">
+        <v>1.804E-2</v>
+      </c>
+      <c r="V17" s="32"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>224</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="I21" s="2"/>
+      <c r="J21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G21" t="s">
+      <c r="K21" s="2"/>
+      <c r="L21" t="s">
         <v>113</v>
       </c>
-      <c r="H21" t="s">
+      <c r="N21" t="s">
         <v>153</v>
       </c>
-      <c r="I21" t="s">
-        <v>242</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="P21" t="s">
+        <v>241</v>
+      </c>
+      <c r="R21" t="s">
         <v>22</v>
       </c>
-      <c r="K21" t="s">
+      <c r="T21" t="s">
         <v>205</v>
       </c>
-      <c r="L21" t="s">
+      <c r="V21" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="20">
         <v>402</v>
       </c>
       <c r="B23" s="11">
         <v>-6743.7441437123198</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="11"/>
+      <c r="D23" s="11">
         <v>-16.975868612314599</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E23" s="11"/>
       <c r="F23" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="11"/>
+      <c r="H23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11">
         <v>8.9738794158530297E-2</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J23" s="11">
+      <c r="M23" s="11"/>
+      <c r="N23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11">
         <v>-635.97332007850503</v>
       </c>
-      <c r="K23" s="11">
+      <c r="S23" s="11"/>
+      <c r="T23" s="11">
         <v>1.10400938742123</v>
       </c>
-      <c r="L23" s="10">
+      <c r="U23" s="11"/>
+      <c r="V23" s="10">
         <v>0.56443989802633698</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="20">
         <v>401</v>
       </c>
       <c r="B24" s="11">
         <v>-6806.1559461658899</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E24" s="11"/>
       <c r="F24" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="11"/>
+      <c r="H24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11">
         <v>9.0352100854232398E-2</v>
       </c>
-      <c r="H24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J24" s="11">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11">
         <v>-616.65277005778705</v>
       </c>
-      <c r="K24" s="11">
+      <c r="S24" s="11"/>
+      <c r="T24" s="11">
         <v>1.09681007948467</v>
       </c>
-      <c r="L24" s="10">
+      <c r="U24" s="11"/>
+      <c r="V24" s="10">
         <v>7.4009714742238997E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="20">
         <v>410</v>
       </c>
       <c r="B25" s="11">
         <v>-6714.4223894438601</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
         <v>-16.3940340053047</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F25" s="11">
+      <c r="E25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11">
         <v>-2.8291141657706399E-2</v>
       </c>
-      <c r="G25" s="11">
+      <c r="K25" s="11"/>
+      <c r="L25" s="11">
         <v>8.9500479288881801E-2</v>
       </c>
-      <c r="H25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J25" s="11">
+      <c r="M25" s="11"/>
+      <c r="N25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11">
         <v>-639.33391793484998</v>
       </c>
-      <c r="K25" s="11">
+      <c r="S25" s="11"/>
+      <c r="T25" s="11">
         <v>1.10528838656039</v>
       </c>
-      <c r="L25" s="10">
+      <c r="U25" s="11"/>
+      <c r="V25" s="10">
         <v>5.5169128859670603E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="20">
         <v>434</v>
       </c>
       <c r="B26" s="11">
         <v>-6804.8067023150297</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11">
         <v>-15.5826666580887</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E26" s="11"/>
       <c r="F26" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11">
         <v>9.0266217789299899E-2</v>
       </c>
-      <c r="H26" s="11">
+      <c r="M26" s="11"/>
+      <c r="N26" s="11">
         <v>0.243409188115466</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J26" s="11">
+      <c r="O26" s="11"/>
+      <c r="P26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11">
         <v>-631.50656393377596</v>
       </c>
-      <c r="K26" s="11">
+      <c r="S26" s="11"/>
+      <c r="T26" s="11">
         <v>1.1057572986278501</v>
       </c>
-      <c r="L26" s="10">
+      <c r="U26" s="11"/>
+      <c r="V26" s="10">
         <v>4.9149854246231597E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="20">
         <v>406</v>
       </c>
       <c r="B27" s="11">
         <v>-6747.2784392261701</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11">
         <v>-17.255597295728901</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="11">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11">
         <v>0.16036442937949799</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G27" s="11">
+      <c r="I27" s="11"/>
+      <c r="J27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11">
         <v>8.9747875789960296E-2</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J27" s="11">
+      <c r="M27" s="11"/>
+      <c r="N27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11">
         <v>-634.30014853525802</v>
       </c>
-      <c r="K27" s="11">
+      <c r="S27" s="11"/>
+      <c r="T27" s="11">
         <v>1.1012511520520301</v>
       </c>
-      <c r="L27" s="10">
+      <c r="U27" s="11"/>
+      <c r="V27" s="10">
         <v>4.6328284305815801E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>404</v>
       </c>
       <c r="B28" s="11">
         <v>-6708.9527654527301</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11">
         <v>-17.234818020677</v>
       </c>
-      <c r="D28" s="11">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11">
         <v>-1.6701071998145099E-2</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G28" s="11">
+      <c r="G28" s="11"/>
+      <c r="H28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11">
         <v>8.9244889027861707E-2</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J28" s="11">
+      <c r="M28" s="11"/>
+      <c r="N28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11">
         <v>-627.77287665384597</v>
       </c>
-      <c r="K28" s="11">
+      <c r="S28" s="11"/>
+      <c r="T28" s="11">
         <v>1.10315040225587</v>
       </c>
-      <c r="L28" s="10">
+      <c r="U28" s="11"/>
+      <c r="V28" s="10">
         <v>4.5026667413762503E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>466</v>
       </c>
       <c r="B29" s="11">
         <v>-6750.6626417638499</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11">
         <v>-16.677549742447201</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E29" s="11"/>
       <c r="F29" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="11"/>
+      <c r="H29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11">
         <v>8.9816498834961497E-2</v>
       </c>
-      <c r="H29" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I29" s="11">
+      <c r="M29" s="11"/>
+      <c r="N29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11">
         <v>0.30261550819902699</v>
       </c>
-      <c r="J29" s="11">
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11">
         <v>-635.79731861115999</v>
       </c>
-      <c r="K29" s="11">
+      <c r="S29" s="11"/>
+      <c r="T29" s="11">
         <v>1.1025318621628699</v>
       </c>
-      <c r="L29" s="10">
+      <c r="U29" s="11"/>
+      <c r="V29" s="10">
         <v>4.2684856922751202E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="20">
         <v>433</v>
       </c>
       <c r="B30" s="11">
         <v>-6983.52730041412</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E30" s="11"/>
       <c r="F30" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="11"/>
+      <c r="H30" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11">
         <v>9.1864817831643505E-2</v>
       </c>
-      <c r="H30" s="11">
+      <c r="M30" s="11"/>
+      <c r="N30" s="11">
         <v>0.77178173299634001</v>
       </c>
-      <c r="I30" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J30" s="11">
+      <c r="O30" s="11"/>
+      <c r="P30" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11">
         <v>-607.51752998181405</v>
       </c>
-      <c r="K30" s="11">
+      <c r="S30" s="11"/>
+      <c r="T30" s="11">
         <v>1.1042256111251201</v>
       </c>
-      <c r="L30" s="10">
+      <c r="U30" s="11"/>
+      <c r="V30" s="10">
         <v>2.9458201644763801E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B31" s="11">
         <v>-6757</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11">
         <v>-14.94</v>
       </c>
-      <c r="D31" s="11">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11">
         <v>-8.298E-4</v>
       </c>
-      <c r="E31" s="11">
+      <c r="G31" s="11"/>
+      <c r="H31" s="11">
         <v>8.1980000000000004E-3</v>
       </c>
-      <c r="F31" s="11">
+      <c r="I31" s="11"/>
+      <c r="J31" s="11">
         <v>-1.722E-3</v>
       </c>
-      <c r="G31" s="11">
+      <c r="K31" s="11"/>
+      <c r="L31" s="11">
         <v>8.9849999999999999E-2</v>
       </c>
-      <c r="H31" s="11">
+      <c r="M31" s="11"/>
+      <c r="N31" s="11">
         <v>3.8289999999999998E-2</v>
       </c>
-      <c r="I31" s="11">
+      <c r="O31" s="11"/>
+      <c r="P31" s="11">
         <v>1.4250000000000001E-2</v>
       </c>
-      <c r="J31" s="11">
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11">
         <v>-632.9</v>
       </c>
-      <c r="K31" s="11">
+      <c r="S31" s="11"/>
+      <c r="T31" s="11">
         <v>1.103</v>
       </c>
-      <c r="L31" s="11"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
         <v>224</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="I35" s="2"/>
+      <c r="J35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G35" t="s">
+      <c r="K35" s="2"/>
+      <c r="L35" t="s">
         <v>113</v>
       </c>
-      <c r="H35" t="s">
+      <c r="N35" t="s">
         <v>153</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="P35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J35" t="s">
+      <c r="Q35" s="2"/>
+      <c r="R35" t="s">
         <v>205</v>
       </c>
-      <c r="K35" t="s">
+      <c r="T35" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>210</v>
       </c>
       <c r="B37" s="11">
         <v>-7292.9106281102204</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11">
         <v>-19.604654051698098</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E37" s="11"/>
       <c r="F37" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="11"/>
+      <c r="H37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11">
         <v>9.5387859510192102E-2</v>
       </c>
-      <c r="H37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I37" s="11">
+      <c r="M37" s="11"/>
+      <c r="N37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11">
         <v>-602.50860116216597</v>
       </c>
-      <c r="J37" s="11">
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11">
         <v>1.1047216975923499</v>
       </c>
-      <c r="K37" s="11">
+      <c r="S37" s="11"/>
+      <c r="T37" s="11">
         <v>0.39926025302679902</v>
       </c>
-      <c r="L37" s="10"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U37" s="11"/>
+      <c r="V37" s="10"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>209</v>
       </c>
       <c r="B38" s="11">
         <v>-7309.81640132133</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E38" s="11"/>
       <c r="F38" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="11"/>
+      <c r="H38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11">
         <v>9.5822292121635094E-2</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I38" s="11">
+      <c r="M38" s="11"/>
+      <c r="N38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11">
         <v>-604.67939212219699</v>
       </c>
-      <c r="J38" s="11">
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11">
         <v>1.1105532210511799</v>
       </c>
-      <c r="K38" s="11">
+      <c r="S38" s="11"/>
+      <c r="T38" s="11">
         <v>0.221320269212085</v>
       </c>
-      <c r="L38" s="10"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U38" s="11"/>
+      <c r="V38" s="10"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>214</v>
       </c>
       <c r="B39" s="11">
         <v>-7313.4930552236001</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11">
         <v>-20.627212424781199</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="11">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11">
         <v>0.66978183677923597</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G39" s="11">
+      <c r="I39" s="11"/>
+      <c r="J39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11">
         <v>9.56437009743802E-2</v>
       </c>
-      <c r="H39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" s="11">
+      <c r="M39" s="11"/>
+      <c r="N39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11">
         <v>-606.74168405748901</v>
       </c>
-      <c r="J39" s="11">
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11">
         <v>1.10893997164933</v>
       </c>
-      <c r="K39" s="11">
+      <c r="S39" s="11"/>
+      <c r="T39" s="11">
         <v>6.0201197669689198E-2</v>
       </c>
-      <c r="L39" s="10"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U39" s="11"/>
+      <c r="V39" s="10"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>217</v>
       </c>
       <c r="B40" s="11">
         <v>-7114.8269621797999</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="11">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11">
         <v>-0.107836252205739</v>
       </c>
-      <c r="G40" s="11">
+      <c r="K40" s="11"/>
+      <c r="L40" s="11">
         <v>9.3353745354519194E-2</v>
       </c>
-      <c r="H40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I40" s="11">
+      <c r="M40" s="11"/>
+      <c r="N40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11">
         <v>-572.662038902468</v>
       </c>
-      <c r="J40" s="11">
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11">
         <v>1.0841183271819601</v>
       </c>
-      <c r="K40" s="11">
+      <c r="S40" s="11"/>
+      <c r="T40" s="11">
         <v>5.7436583956496798E-2</v>
       </c>
-      <c r="L40" s="10"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U40" s="11"/>
+      <c r="V40" s="10"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>218</v>
       </c>
       <c r="B41" s="11">
         <v>-7155.8636493685399</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11">
         <v>-18.143140505809999</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F41" s="11">
+      <c r="E41" s="11"/>
+      <c r="F41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11">
         <v>-7.6488963447794406E-2</v>
       </c>
-      <c r="G41" s="11">
+      <c r="K41" s="11"/>
+      <c r="L41" s="11">
         <v>9.3669289694699301E-2</v>
       </c>
-      <c r="H41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I41" s="11">
+      <c r="M41" s="11"/>
+      <c r="N41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11">
         <v>-579.960312771914</v>
       </c>
-      <c r="J41" s="11">
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11">
         <v>1.0864059894652001</v>
       </c>
-      <c r="K41" s="11">
+      <c r="S41" s="11"/>
+      <c r="T41" s="11">
         <v>5.14218444431708E-2</v>
       </c>
-      <c r="L41" s="10"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U41" s="11"/>
+      <c r="V41" s="10"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>213</v>
       </c>
       <c r="B42" s="11">
         <v>-7325.7028867234503</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="11"/>
+      <c r="F42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11">
         <v>0.49573112910573702</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G42" s="11">
+      <c r="I42" s="11"/>
+      <c r="J42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11">
         <v>9.6028421365964206E-2</v>
       </c>
-      <c r="H42" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I42" s="11">
+      <c r="M42" s="11"/>
+      <c r="N42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11">
         <v>-607.89626155153098</v>
       </c>
-      <c r="J42" s="11">
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11">
         <v>1.1139004518839499</v>
       </c>
-      <c r="K42" s="11">
+      <c r="S42" s="11"/>
+      <c r="T42" s="11">
         <v>3.2802819639660502E-2</v>
       </c>
-      <c r="L42" s="10"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U42" s="11"/>
+      <c r="V42" s="10"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>241</v>
       </c>
       <c r="B43" s="11">
         <v>-7390.5659924457104</v>
       </c>
-      <c r="C43" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E43" s="11"/>
       <c r="F43" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="11"/>
+      <c r="H43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11">
         <v>9.6382119014641998E-2</v>
       </c>
-      <c r="H43" s="11">
+      <c r="M43" s="11"/>
+      <c r="N43" s="11">
         <v>0.59696114204256701</v>
       </c>
-      <c r="I43" s="11">
+      <c r="O43" s="11"/>
+      <c r="P43" s="11">
         <v>-597.90082415760298</v>
       </c>
-      <c r="J43" s="11">
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11">
         <v>1.12732185825085</v>
       </c>
-      <c r="K43" s="11">
+      <c r="S43" s="11"/>
+      <c r="T43" s="11">
         <v>3.25273622864483E-2</v>
       </c>
-      <c r="L43" s="10"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U43" s="11"/>
+      <c r="V43" s="10"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>212</v>
       </c>
       <c r="B44" s="11">
         <v>-7263.1336664129904</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11">
         <v>-19.849631632379399</v>
       </c>
-      <c r="D44" s="11">
+      <c r="E44" s="11"/>
+      <c r="F44" s="11">
         <v>-2.4888768170442301E-2</v>
       </c>
-      <c r="E44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G44" s="11">
+      <c r="G44" s="11"/>
+      <c r="H44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11">
         <v>9.4934984524476906E-2</v>
       </c>
-      <c r="H44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I44" s="11">
+      <c r="M44" s="11"/>
+      <c r="N44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11">
         <v>-593.44984828006704</v>
       </c>
-      <c r="J44" s="11">
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11">
         <v>1.10170682452437</v>
       </c>
-      <c r="K44" s="11">
+      <c r="S44" s="11"/>
+      <c r="T44" s="11">
         <v>3.1432074573972103E-2</v>
       </c>
-      <c r="L44" s="10"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U44" s="11"/>
+      <c r="V44" s="10"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>242</v>
       </c>
       <c r="B45" s="11">
         <v>-7270.0423142262598</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11">
         <v>-20.3491331901275</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="E45" s="11"/>
       <c r="F45" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="11"/>
+      <c r="H45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11">
         <v>9.5217269756587106E-2</v>
       </c>
-      <c r="H45" s="11">
+      <c r="M45" s="11"/>
+      <c r="N45" s="11">
         <v>-0.164313545049564</v>
       </c>
-      <c r="I45" s="11">
+      <c r="O45" s="11"/>
+      <c r="P45" s="11">
         <v>-604.29196694358097</v>
       </c>
-      <c r="J45" s="11">
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11">
         <v>1.09988468062138</v>
       </c>
-      <c r="K45" s="11">
+      <c r="S45" s="11"/>
+      <c r="T45" s="11">
         <v>3.06175173232827E-2</v>
       </c>
-      <c r="L45" s="11"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>211</v>
       </c>
       <c r="B46" s="11">
         <v>-7304.6780003777103</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="11">
+      <c r="C46" s="11"/>
+      <c r="D46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11">
         <v>-4.3255674915304897E-3</v>
       </c>
-      <c r="E46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="G46" s="11">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11">
         <v>9.5744527748838598E-2</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I46" s="11">
+      <c r="M46" s="11"/>
+      <c r="N46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11">
         <v>-603.10973180273004</v>
       </c>
-      <c r="J46" s="11">
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11">
         <v>1.1100419127999299</v>
       </c>
-      <c r="K46" s="11">
+      <c r="S46" s="11"/>
+      <c r="T46" s="11">
         <v>2.4739936914797801E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="U46" s="11"/>
+    </row>
+    <row r="47" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>212</v>
       </c>
       <c r="B47" s="10">
         <v>-7283</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="10"/>
+      <c r="D47" s="10">
         <v>-11.94</v>
       </c>
-      <c r="D47" s="10">
+      <c r="E47" s="10"/>
+      <c r="F47" s="10">
         <v>-9.4430000000000002E-4</v>
       </c>
-      <c r="E47" s="10">
+      <c r="G47" s="10"/>
+      <c r="H47" s="10">
         <v>6.0080000000000001E-2</v>
       </c>
-      <c r="F47" s="10">
+      <c r="I47" s="10"/>
+      <c r="J47" s="10">
         <v>-1.0749999999999999E-2</v>
       </c>
-      <c r="G47" s="10">
+      <c r="K47" s="10"/>
+      <c r="L47" s="10">
         <v>9.5329999999999998E-2</v>
       </c>
-      <c r="H47" s="10">
+      <c r="M47" s="10"/>
+      <c r="N47" s="10">
         <v>1.528E-2</v>
       </c>
-      <c r="I47" s="10">
+      <c r="O47" s="10"/>
+      <c r="P47" s="10">
         <v>-600</v>
       </c>
-      <c r="J47" s="10">
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10">
         <v>1.105</v>
       </c>
+      <c r="S47" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4781,8 +5191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562815E0-203F-4D5B-96E0-A656DF752C95}">
   <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4819,7 +5229,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -5964,7 +6374,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -6832,7 +7242,7 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
@@ -7532,8 +7942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CEF00E-76FA-48D6-B21A-FF6CCE8B1018}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7558,7 +7968,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
@@ -7566,7 +7976,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -7820,7 +8230,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>
@@ -8082,7 +8492,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
@@ -8335,6 +8745,317 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01171B25-C7B7-4B7E-9F18-D774EB4029E3}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>-0.26719999999999999</v>
+      </c>
+      <c r="B4" s="11">
+        <v>4.705E-3</v>
+      </c>
+      <c r="C4" s="11">
+        <v>1.222E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <v>6.5340000000000005E-4</v>
+      </c>
+      <c r="E4" s="11">
+        <v>8.4720000000000004E-2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>7.5609999999999997E-2</v>
+      </c>
+      <c r="G4" s="11">
+        <v>-0.14069999999999999</v>
+      </c>
+      <c r="H4" s="11">
+        <v>-598.70000000000005</v>
+      </c>
+      <c r="I4" s="11">
+        <v>1.069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>-14.94</v>
+      </c>
+      <c r="B7" s="11">
+        <v>-8.298E-4</v>
+      </c>
+      <c r="C7" s="11">
+        <v>8.1980000000000004E-3</v>
+      </c>
+      <c r="D7" s="11">
+        <v>-1.722E-3</v>
+      </c>
+      <c r="E7" s="11">
+        <v>8.9849999999999999E-2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>3.8289999999999998E-2</v>
+      </c>
+      <c r="G7" s="11">
+        <v>1.4250000000000001E-2</v>
+      </c>
+      <c r="H7" s="11">
+        <v>-632.9</v>
+      </c>
+      <c r="I7" s="11">
+        <v>1.103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>-11.94</v>
+      </c>
+      <c r="B10" s="10">
+        <v>-9.4430000000000002E-4</v>
+      </c>
+      <c r="C10" s="10">
+        <v>6.0080000000000001E-2</v>
+      </c>
+      <c r="D10" s="10">
+        <v>-1.0749999999999999E-2</v>
+      </c>
+      <c r="E10" s="10">
+        <v>9.5329999999999998E-2</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1.528E-2</v>
+      </c>
+      <c r="G10" s="10">
+        <v>-600</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1.105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>5.246E-2</v>
+      </c>
+      <c r="B13" s="10">
+        <v>2.6460000000000001E-2</v>
+      </c>
+      <c r="C13" s="10">
+        <v>-2.3260000000000001E-5</v>
+      </c>
+      <c r="D13" s="10">
+        <v>5.9470000000000002E-2</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.004E-2</v>
+      </c>
+      <c r="F13" s="10">
+        <v>4.2970000000000001E-2</v>
+      </c>
+      <c r="G13" s="10">
+        <v>5.79E-3</v>
+      </c>
+      <c r="H13" s="10">
+        <v>9.9460000000000007E-2</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1.0680000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
+        <v>2.571E-2</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1.9980000000000001E-2</v>
+      </c>
+      <c r="C16" s="11">
+        <v>-7.1539999999999996E-5</v>
+      </c>
+      <c r="D16" s="11">
+        <v>5.9970000000000002E-2</v>
+      </c>
+      <c r="E16" s="11">
+        <v>-4.6020000000000002E-3</v>
+      </c>
+      <c r="F16" s="11">
+        <v>2.2589999999999999E-2</v>
+      </c>
+      <c r="G16" s="11">
+        <v>7.3559999999999997E-3</v>
+      </c>
+      <c r="H16" s="11">
+        <v>1.669E-2</v>
+      </c>
+      <c r="I16" s="11">
+        <v>1.0609999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="11">
+        <v>-2.027E-2</v>
+      </c>
+      <c r="B19" s="11">
+        <v>-1.8839999999999999E-2</v>
+      </c>
+      <c r="C19" s="11">
+        <v>-6.6530000000000002E-5</v>
+      </c>
+      <c r="D19" s="11">
+        <v>6.2359999999999999E-2</v>
+      </c>
+      <c r="E19" s="11">
+        <v>-2.6749999999999999E-3</v>
+      </c>
+      <c r="F19" s="11">
+        <v>-4.9450000000000004E-4</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1.872E-3</v>
+      </c>
+      <c r="H19" s="11">
+        <v>6.999E-3</v>
+      </c>
+      <c r="I19" s="11">
+        <v>1.0640000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="11">
+        <v>5.9650000000000002E-2</v>
+      </c>
+      <c r="B22" s="11">
+        <v>-2.8050000000000002E-3</v>
+      </c>
+      <c r="C22" s="11">
+        <v>2.0939999999999999E-3</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1.108E-2</v>
+      </c>
+      <c r="E22" s="11">
+        <v>-1.5970000000000001E-4</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1.071</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="11">
+        <v>6.0089999999999998E-2</v>
+      </c>
+      <c r="B25" s="11">
+        <v>2.019E-2</v>
+      </c>
+      <c r="C25" s="11">
+        <v>-1.091E-2</v>
+      </c>
+      <c r="D25" s="11">
+        <v>1.0580000000000001E-2</v>
+      </c>
+      <c r="E25" s="11">
+        <v>-2.47E-3</v>
+      </c>
+      <c r="F25" s="11">
+        <v>1.0620000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="11">
+        <v>6.198E-2</v>
+      </c>
+      <c r="B28" s="11">
+        <v>4.3810000000000002E-2</v>
+      </c>
+      <c r="C28" s="11">
+        <v>-1.9539999999999998E-2</v>
+      </c>
+      <c r="D28" s="11">
+        <v>-2.7109999999999999E-2</v>
+      </c>
+      <c r="E28" s="11">
+        <v>-8.1440000000000002E-3</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.075</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A4:G4 A7:G7 A10:F10 A13:H13 A16:H16 A19:H19 A22:E22 A25:E25 A28:E28">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
   <dimension ref="A1:I60"/>
   <sheetViews>
@@ -8354,15 +9075,15 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -8373,32 +9094,32 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -8408,10 +9129,10 @@
     </row>
     <row r="7" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -8422,21 +9143,21 @@
     </row>
     <row r="9" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -8446,21 +9167,21 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="C12" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>276</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -8470,59 +9191,59 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" t="s">
         <v>282</v>
-      </c>
-      <c r="C15" t="s">
-        <v>283</v>
-      </c>
-      <c r="D15" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>282</v>
-      </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19" t="s">
         <v>286</v>
       </c>
-      <c r="B19" t="s">
-        <v>288</v>
-      </c>
       <c r="C19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -8532,40 +9253,40 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B22" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C22" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B23" t="s">
+        <v>295</v>
+      </c>
+      <c r="C23" t="s">
         <v>291</v>
-      </c>
-      <c r="B23" t="s">
-        <v>297</v>
-      </c>
-      <c r="C23" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B25" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -8575,98 +9296,98 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="B28" t="s">
         <v>302</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>303</v>
+      </c>
+      <c r="D28" t="s">
         <v>304</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>305</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>306</v>
-      </c>
-      <c r="E28" t="s">
-        <v>307</v>
-      </c>
-      <c r="F28" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D31" t="s">
+        <v>302</v>
+      </c>
+      <c r="E31" t="s">
+        <v>303</v>
+      </c>
+      <c r="F31" t="s">
         <v>304</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>305</v>
-      </c>
-      <c r="F31" t="s">
-        <v>306</v>
-      </c>
-      <c r="G31" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C32" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D32" t="s">
+        <v>302</v>
+      </c>
+      <c r="E32" t="s">
+        <v>303</v>
+      </c>
+      <c r="F32" t="s">
         <v>304</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>305</v>
-      </c>
-      <c r="F32" t="s">
-        <v>306</v>
-      </c>
-      <c r="G32" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -8674,202 +9395,202 @@
         <v>32</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C33" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D33" t="s">
+        <v>302</v>
+      </c>
+      <c r="E33" t="s">
+        <v>303</v>
+      </c>
+      <c r="F33" t="s">
         <v>304</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>305</v>
-      </c>
-      <c r="F33" t="s">
-        <v>306</v>
-      </c>
-      <c r="G33" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C34" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D34" t="s">
+        <v>302</v>
+      </c>
+      <c r="E34" t="s">
+        <v>303</v>
+      </c>
+      <c r="F34" t="s">
         <v>304</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>305</v>
-      </c>
-      <c r="F34" t="s">
-        <v>306</v>
-      </c>
-      <c r="G34" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C35" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D35" t="s">
+        <v>302</v>
+      </c>
+      <c r="E35" t="s">
+        <v>303</v>
+      </c>
+      <c r="F35" t="s">
         <v>304</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>305</v>
-      </c>
-      <c r="F35" t="s">
-        <v>306</v>
-      </c>
-      <c r="G35" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C36" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D36" t="s">
+        <v>302</v>
+      </c>
+      <c r="E36" t="s">
+        <v>303</v>
+      </c>
+      <c r="F36" t="s">
         <v>304</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>305</v>
-      </c>
-      <c r="F36" t="s">
-        <v>306</v>
-      </c>
-      <c r="G36" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C37" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D37" t="s">
+        <v>302</v>
+      </c>
+      <c r="E37" t="s">
+        <v>303</v>
+      </c>
+      <c r="F37" t="s">
         <v>304</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>305</v>
-      </c>
-      <c r="F37" t="s">
-        <v>306</v>
-      </c>
-      <c r="G37" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C38" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D38" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E38" t="s">
+        <v>302</v>
+      </c>
+      <c r="F38" t="s">
+        <v>303</v>
+      </c>
+      <c r="G38" t="s">
         <v>304</v>
       </c>
-      <c r="F38" t="s">
+      <c r="H38" t="s">
         <v>305</v>
-      </c>
-      <c r="G38" t="s">
-        <v>306</v>
-      </c>
-      <c r="H38" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C39" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D39" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E39" t="s">
+        <v>302</v>
+      </c>
+      <c r="F39" t="s">
+        <v>303</v>
+      </c>
+      <c r="G39" t="s">
         <v>304</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" t="s">
         <v>305</v>
-      </c>
-      <c r="G39" t="s">
-        <v>306</v>
-      </c>
-      <c r="H39" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B40" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D40" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E40" t="s">
+        <v>302</v>
+      </c>
+      <c r="F40" t="s">
+        <v>303</v>
+      </c>
+      <c r="G40" t="s">
         <v>304</v>
       </c>
-      <c r="F40" t="s">
+      <c r="H40" t="s">
         <v>305</v>
-      </c>
-      <c r="G40" t="s">
-        <v>306</v>
-      </c>
-      <c r="H40" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="25" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B42" s="26" t="s">
         <v>22</v>
@@ -8877,138 +9598,138 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C43" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C46" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="C47" t="s">
         <v>332</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>333</v>
-      </c>
-      <c r="C47" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C50" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C51" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D52" t="s">
+        <v>302</v>
+      </c>
+      <c r="E52" t="s">
+        <v>303</v>
+      </c>
+      <c r="F52" t="s">
         <v>304</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>305</v>
-      </c>
-      <c r="F52" t="s">
-        <v>306</v>
-      </c>
-      <c r="G52" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B53" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C53" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D53" t="s">
+        <v>302</v>
+      </c>
+      <c r="E53" t="s">
+        <v>303</v>
+      </c>
+      <c r="F53" t="s">
         <v>304</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>305</v>
-      </c>
-      <c r="F53" t="s">
-        <v>306</v>
-      </c>
-      <c r="G53" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -9016,166 +9737,166 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C54" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D54" t="s">
+        <v>302</v>
+      </c>
+      <c r="E54" t="s">
+        <v>303</v>
+      </c>
+      <c r="F54" t="s">
         <v>304</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>305</v>
-      </c>
-      <c r="F54" t="s">
-        <v>306</v>
-      </c>
-      <c r="G54" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B55" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C55" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D55" t="s">
+        <v>302</v>
+      </c>
+      <c r="E55" t="s">
+        <v>303</v>
+      </c>
+      <c r="F55" t="s">
         <v>304</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>305</v>
-      </c>
-      <c r="F55" t="s">
-        <v>306</v>
-      </c>
-      <c r="G55" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C56" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D56" t="s">
+        <v>302</v>
+      </c>
+      <c r="E56" t="s">
+        <v>303</v>
+      </c>
+      <c r="F56" t="s">
         <v>304</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>305</v>
-      </c>
-      <c r="F56" t="s">
-        <v>306</v>
-      </c>
-      <c r="G56" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B57" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C57" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D57" t="s">
+        <v>302</v>
+      </c>
+      <c r="E57" t="s">
+        <v>303</v>
+      </c>
+      <c r="F57" t="s">
         <v>304</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>305</v>
-      </c>
-      <c r="F57" t="s">
-        <v>306</v>
-      </c>
-      <c r="G57" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C58" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D58" t="s">
+        <v>302</v>
+      </c>
+      <c r="E58" t="s">
+        <v>303</v>
+      </c>
+      <c r="F58" t="s">
         <v>304</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" t="s">
         <v>305</v>
-      </c>
-      <c r="F58" t="s">
-        <v>306</v>
-      </c>
-      <c r="G58" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B59" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D59" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E59" t="s">
+        <v>302</v>
+      </c>
+      <c r="F59" t="s">
+        <v>303</v>
+      </c>
+      <c r="G59" t="s">
         <v>304</v>
       </c>
-      <c r="F59" t="s">
+      <c r="H59" t="s">
         <v>305</v>
-      </c>
-      <c r="G59" t="s">
-        <v>306</v>
-      </c>
-      <c r="H59" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B60" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C60" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D60" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E60" t="s">
+        <v>302</v>
+      </c>
+      <c r="F60" t="s">
+        <v>303</v>
+      </c>
+      <c r="G60" t="s">
         <v>304</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>305</v>
-      </c>
-      <c r="G60" t="s">
-        <v>306</v>
-      </c>
-      <c r="H60" t="s">
-        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -9268,7 +9989,7 @@
         <v>150</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -11010,13 +11731,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B2" s="3"/>
     </row>
@@ -11043,7 +11764,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -11185,7 +11906,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -11243,7 +11964,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -11256,7 +11977,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -11269,7 +11990,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -11282,7 +12003,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -11295,7 +12016,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -11308,7 +12029,7 @@
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -11321,7 +12042,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -11346,10 +12067,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858278ED-196A-4B59-8830-674E5B382BAC}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11519,31 +12240,48 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>112</v>
+      <c r="A13" t="s">
+        <v>29</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -11555,15 +12293,15 @@
         <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -11572,29 +12310,29 @@
         <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -11606,68 +12344,68 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>47</v>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>52</v>
+      <c r="A22" t="s">
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>40</v>
@@ -11684,7 +12422,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -11701,7 +12439,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -11718,7 +12456,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -11734,55 +12472,38 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" t="s">
         <v>12</v>
       </c>
-      <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>91</v>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
         <v>16</v>
       </c>
     </row>
@@ -11796,8 +12517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661002B2-E508-42DE-AAF7-55B64A4B61E8}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12054,7 +12775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED94DC-32EE-4CB2-B393-F68209908457}">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -12206,7 +12927,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -13619,7 +14340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B568554-EE5E-4148-B92D-3C63A1452433}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -13715,7 +14436,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
@@ -14328,7 +15049,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated tables & effects comparisons
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66EAF9-FF9D-47B7-8E15-2AB7772FC1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54CDDD-0D6E-406F-9349-AAB14D490FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="6" activeTab="10" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="3" activeTab="4" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
     <sheet name="Table 2" sheetId="2" r:id="rId2"/>
     <sheet name="Table 3" sheetId="5" r:id="rId3"/>
     <sheet name="table 3_v2" sheetId="10" r:id="rId4"/>
-    <sheet name="Table 4" sheetId="6" r:id="rId5"/>
-    <sheet name="Table S1" sheetId="3" r:id="rId6"/>
-    <sheet name="Table S2 - CCI bands" sheetId="4" r:id="rId7"/>
-    <sheet name="Tables S3_S5" sheetId="7" r:id="rId8"/>
-    <sheet name="Tables S6_S8" sheetId="8" r:id="rId9"/>
-    <sheet name="Tables S9_S11" sheetId="9" r:id="rId10"/>
-    <sheet name="Tables S12_S14" sheetId="11" r:id="rId11"/>
-    <sheet name="Tables S15_S17" sheetId="12" r:id="rId12"/>
-    <sheet name="Tables S18_S20" sheetId="13" r:id="rId13"/>
-    <sheet name="Largest_effects" sheetId="15" r:id="rId14"/>
-    <sheet name="Table S21" sheetId="14" r:id="rId15"/>
+    <sheet name="effect_sizes" sheetId="16" r:id="rId5"/>
+    <sheet name="Table 4" sheetId="6" r:id="rId6"/>
+    <sheet name="Table S1" sheetId="3" r:id="rId7"/>
+    <sheet name="Table S2 - CCI bands" sheetId="4" r:id="rId8"/>
+    <sheet name="Tables S3_S5" sheetId="7" r:id="rId9"/>
+    <sheet name="Tables S6_S8" sheetId="8" r:id="rId10"/>
+    <sheet name="Tables S9_S11" sheetId="9" r:id="rId11"/>
+    <sheet name="Tables S12_S14" sheetId="11" r:id="rId12"/>
+    <sheet name="Tables S15_S17" sheetId="12" r:id="rId13"/>
+    <sheet name="Tables S18_S20" sheetId="13" r:id="rId14"/>
+    <sheet name="Largest_effects" sheetId="15" r:id="rId15"/>
+    <sheet name="Table S21" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="355">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -1100,6 +1101,18 @@
   </si>
   <si>
     <t xml:space="preserve">Table Sx. Raw model coefficients and full averaged coefficients from the top economic models (dAIC &lt; 6) with 2 year time lag. </t>
+  </si>
+  <si>
+    <t>Rate ratio</t>
+  </si>
+  <si>
+    <t>No lag</t>
+  </si>
+  <si>
+    <t>1 yr lag</t>
+  </si>
+  <si>
+    <t>2 yr lag</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1223,10 +1236,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
-      <right/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1239,16 +1263,14 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1278,7 +1300,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1293,10 +1314,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1311,6 +1338,14 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1985,6 +2020,1373 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B568554-EE5E-4148-B92D-3C63A1452433}">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B9" s="10">
+        <v>17.18</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.5569999999999999E-2</v>
+      </c>
+      <c r="D9" s="10">
+        <v>6.5979999999999997E-3</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-6.5440000000000003E-3</v>
+      </c>
+      <c r="F9" s="10">
+        <v>-8.9479999999999996E-4</v>
+      </c>
+      <c r="G9" s="10">
+        <v>1.336E-2</v>
+      </c>
+      <c r="H9" s="10">
+        <v>-1.698</v>
+      </c>
+      <c r="I9" s="10">
+        <v>5.0750000000000003E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" t="s">
+        <v>222</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K13" t="s">
+        <v>205</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>186</v>
+      </c>
+      <c r="B15" s="11">
+        <v>19.009683355491202</v>
+      </c>
+      <c r="C15" s="11">
+        <v>1.29608290177501E-2</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="11">
+        <v>-1.84532899937581E-4</v>
+      </c>
+      <c r="G15" s="11">
+        <v>8.9895527555435301E-3</v>
+      </c>
+      <c r="H15" s="11">
+        <v>-6.7625486018793599E-3</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="11">
+        <v>7.3849377864736903E-3</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.266233744495813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>249</v>
+      </c>
+      <c r="B16" s="11">
+        <v>17.791917474132401</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="11">
+        <v>-1.7143199173686401E-4</v>
+      </c>
+      <c r="G16" s="11">
+        <v>4.09785003072615E-3</v>
+      </c>
+      <c r="H16" s="11">
+        <v>-1.5871515486556901E-3</v>
+      </c>
+      <c r="I16" s="11">
+        <v>4.39231821585213E-4</v>
+      </c>
+      <c r="J16" s="11">
+        <v>6.72550356216593E-3</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0.178477643773784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>250</v>
+      </c>
+      <c r="B17" s="11">
+        <v>18.238780266223401</v>
+      </c>
+      <c r="C17" s="11">
+        <v>7.2257116178215302E-3</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="11">
+        <v>-1.7614452199371801E-4</v>
+      </c>
+      <c r="G17" s="11">
+        <v>6.7506961184131001E-3</v>
+      </c>
+      <c r="H17" s="11">
+        <v>-4.4415916510793501E-3</v>
+      </c>
+      <c r="I17" s="11">
+        <v>2.2030303542616499E-4</v>
+      </c>
+      <c r="J17" s="11">
+        <v>6.8796476315811997E-3</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="10">
+        <v>8.1447073791342306E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="14">
+        <v>446</v>
+      </c>
+      <c r="B18" s="11">
+        <v>16.292790577390001</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1.09740411901045E-2</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="11">
+        <v>1.41862161101489E-6</v>
+      </c>
+      <c r="F18" s="11">
+        <v>-1.5489787022817899E-4</v>
+      </c>
+      <c r="G18" s="11">
+        <v>8.4352556606180195E-3</v>
+      </c>
+      <c r="H18" s="11">
+        <v>-5.5961388582716001E-3</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J18" s="11">
+        <v>8.1371661521309306E-3</v>
+      </c>
+      <c r="K18" s="11">
+        <v>7.0453351777090495E-4</v>
+      </c>
+      <c r="L18" s="10">
+        <v>8.0380629516945801E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>442</v>
+      </c>
+      <c r="B19" s="11">
+        <v>18.933888188050801</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1.27204007729679E-2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="11">
+        <v>-1.83613354627066E-4</v>
+      </c>
+      <c r="G19" s="11">
+        <v>9.2651727566647798E-3</v>
+      </c>
+      <c r="H19" s="11">
+        <v>-6.7871509061906699E-3</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="11">
+        <v>7.4565847270431198E-3</v>
+      </c>
+      <c r="K19" s="11">
+        <v>3.6907273823718299E-4</v>
+      </c>
+      <c r="L19" s="10">
+        <v>7.3310335878910393E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>251</v>
+      </c>
+      <c r="B20" s="11">
+        <v>17.249397001262501</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="11">
+        <v>3.8451081773854799E-3</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="11">
+        <v>-1.6666525775224701E-4</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4.1277007854361204E-3</v>
+      </c>
+      <c r="H20" s="11">
+        <v>-1.9347858632567899E-3</v>
+      </c>
+      <c r="I20" s="11">
+        <v>4.0482648807792102E-4</v>
+      </c>
+      <c r="J20" s="11">
+        <v>5.9564273387460098E-3</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" s="10">
+        <v>7.2547265918478904E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>190</v>
+      </c>
+      <c r="B21" s="11">
+        <v>17.891599666362001</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1.2108022021667501E-2</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="11">
+        <v>7.23686347282587E-7</v>
+      </c>
+      <c r="F21" s="11">
+        <v>-1.72433083556121E-4</v>
+      </c>
+      <c r="G21" s="11">
+        <v>8.3822834474565101E-3</v>
+      </c>
+      <c r="H21" s="11">
+        <v>-6.0963889412872204E-3</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J21" s="11">
+        <v>7.6684196861511204E-3</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L21" s="10">
+        <v>6.9527526338365897E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>188</v>
+      </c>
+      <c r="B22" s="11">
+        <v>18.5920030366721</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.2207173055958E-2</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2.0443801661234398E-3</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="11">
+        <v>-1.80610406572904E-4</v>
+      </c>
+      <c r="G22" s="11">
+        <v>8.7601465733685192E-3</v>
+      </c>
+      <c r="H22" s="11">
+        <v>-6.66542893793201E-3</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J22" s="11">
+        <v>7.0199032768215397E-3</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" s="10">
+        <v>4.0171754058928102E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>218</v>
+      </c>
+      <c r="B23" s="11">
+        <v>17.811374600908302</v>
+      </c>
+      <c r="C23" s="11">
+        <v>-2.75211460807106E-3</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="11">
+        <v>-1.71820579369805E-4</v>
+      </c>
+      <c r="G23" s="11">
+        <v>2.8246973996307301E-3</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="11">
+        <v>5.2987624187635801E-4</v>
+      </c>
+      <c r="J23" s="11">
+        <v>6.6093939776072199E-3</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" s="10">
+        <v>3.2169456070832797E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>217</v>
+      </c>
+      <c r="B24" s="11">
+        <v>17.982687422475699</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="11">
+        <v>-1.7365512747779201E-4</v>
+      </c>
+      <c r="G24" s="11">
+        <v>3.13788101386714E-3</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" s="11">
+        <v>4.5986822953149602E-4</v>
+      </c>
+      <c r="J24" s="11">
+        <v>6.35203075536448E-3</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L24" s="10">
+        <v>3.0135542544931199E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>253</v>
+      </c>
+      <c r="B25" s="11">
+        <v>17.3599049168132</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E25" s="11">
+        <v>3.0202037120308401E-7</v>
+      </c>
+      <c r="F25" s="11">
+        <v>-1.6676584263045999E-4</v>
+      </c>
+      <c r="G25" s="11">
+        <v>3.9975876375509898E-3</v>
+      </c>
+      <c r="H25" s="11">
+        <v>-1.45756291327818E-3</v>
+      </c>
+      <c r="I25" s="11">
+        <v>4.22830045051132E-4</v>
+      </c>
+      <c r="J25" s="11">
+        <v>6.90671508065428E-3</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L25" s="10">
+        <v>2.26474393626315E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>505</v>
+      </c>
+      <c r="B26" s="11">
+        <v>17.848673967184599</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26" s="11">
+        <v>-1.7203748206080601E-4</v>
+      </c>
+      <c r="G26" s="11">
+        <v>4.2449302038568898E-3</v>
+      </c>
+      <c r="H26" s="11">
+        <v>-1.6423675450923201E-3</v>
+      </c>
+      <c r="I26" s="11">
+        <v>4.30725117609008E-4</v>
+      </c>
+      <c r="J26" s="11">
+        <v>6.8075216947054203E-3</v>
+      </c>
+      <c r="K26" s="11">
+        <v>1.2572313639363399E-4</v>
+      </c>
+      <c r="L26" s="10">
+        <v>2.1730668619851401E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>221</v>
+      </c>
+      <c r="B27" s="11">
+        <v>16.911549401152701</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="11">
+        <v>9.5109173465066103E-7</v>
+      </c>
+      <c r="F27" s="11">
+        <v>-1.6215742624764499E-4</v>
+      </c>
+      <c r="G27" s="11">
+        <v>3.1039446438607802E-3</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" s="11">
+        <v>4.0263140725682801E-4</v>
+      </c>
+      <c r="J27" s="11">
+        <v>7.0342366376967601E-3</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L27" s="10">
+        <v>1.6463050402586301E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>220</v>
+      </c>
+      <c r="B28" s="11">
+        <v>17.224218560369501</v>
+      </c>
+      <c r="C28" s="11">
+        <v>-3.9155880576206897E-3</v>
+      </c>
+      <c r="D28" s="11">
+        <v>4.1841045266635003E-3</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="11">
+        <v>-1.66687416045079E-4</v>
+      </c>
+      <c r="G28" s="11">
+        <v>2.4886482796275598E-3</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" s="11">
+        <v>5.2644999811742998E-4</v>
+      </c>
+      <c r="J28" s="11">
+        <v>5.7417922381403502E-3</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="L28" s="10">
+        <v>1.47578692265985E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="10">
+        <v>18.09</v>
+      </c>
+      <c r="C29" s="10">
+        <v>7.0400000000000003E-3</v>
+      </c>
+      <c r="D29" s="10">
+        <v>4.2279999999999998E-4</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1.8680000000000001E-7</v>
+      </c>
+      <c r="F29" s="10">
+        <v>-1.7469999999999999E-4</v>
+      </c>
+      <c r="G29" s="10">
+        <v>6.7219999999999997E-3</v>
+      </c>
+      <c r="H29" s="10">
+        <v>-4.2940000000000001E-3</v>
+      </c>
+      <c r="I29" s="10">
+        <v>1.8990000000000001E-4</v>
+      </c>
+      <c r="J29" s="10">
+        <v>7.084E-3</v>
+      </c>
+      <c r="K29" s="10">
+        <v>8.6420000000000003E-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" t="s">
+        <v>224</v>
+      </c>
+      <c r="C33" t="s">
+        <v>216</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E33" t="s">
+        <v>222</v>
+      </c>
+      <c r="F33" t="s">
+        <v>113</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="K33" t="s">
+        <v>205</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>410</v>
+      </c>
+      <c r="B35" s="11">
+        <v>12.2030866660689</v>
+      </c>
+      <c r="C35" s="11">
+        <v>-6.7019935890024699E-3</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="11">
+        <v>-1.1118693345988001E-4</v>
+      </c>
+      <c r="G35" s="11">
+        <v>-3.6025136466945299E-3</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J35" s="11">
+        <v>8.18196829626564E-3</v>
+      </c>
+      <c r="K35" s="11">
+        <v>-1.1024210994762E-3</v>
+      </c>
+      <c r="L35">
+        <v>0.290088335638363</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>395</v>
+      </c>
+      <c r="B36" s="11">
+        <v>16.331518985578501</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36" s="11">
+        <v>-9.2205756109065493E-3</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="11">
+        <v>-1.5286706634028499E-4</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J36" s="11">
+        <v>9.7018334379725905E-3</v>
+      </c>
+      <c r="K36" s="11">
+        <v>-8.8792403223106504E-4</v>
+      </c>
+      <c r="L36">
+        <v>0.133297053622733</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>459</v>
+      </c>
+      <c r="B37" s="11">
+        <v>15.177145875226801</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" s="11">
+        <v>-6.7163087448920402E-3</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="11">
+        <v>-1.4083336345925901E-4</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I37" s="11">
+        <v>-1.7429952558927801E-4</v>
+      </c>
+      <c r="J37" s="11">
+        <v>9.6427767895367993E-3</v>
+      </c>
+      <c r="K37" s="11">
+        <v>-8.0688455088703196E-4</v>
+      </c>
+      <c r="L37">
+        <v>0.12458991421073499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>396</v>
+      </c>
+      <c r="B38" s="11">
+        <v>14.7796214596646</v>
+      </c>
+      <c r="C38" s="11">
+        <v>-3.0024683268318102E-3</v>
+      </c>
+      <c r="D38" s="11">
+        <v>-5.8202868137717401E-3</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="11">
+        <v>-1.3683483081216799E-4</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J38" s="11">
+        <v>9.1604464318543102E-3</v>
+      </c>
+      <c r="K38" s="11">
+        <v>-7.9094434579269799E-4</v>
+      </c>
+      <c r="L38">
+        <v>9.0814849494256097E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>394</v>
+      </c>
+      <c r="B39" s="11">
+        <v>13.4169021279987</v>
+      </c>
+      <c r="C39" s="11">
+        <v>-4.8970846317684903E-3</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" s="11">
+        <v>-1.23464167016551E-4</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J39" s="11">
+        <v>8.0177530532582197E-3</v>
+      </c>
+      <c r="K39" s="11">
+        <v>-7.9967030200243396E-4</v>
+      </c>
+      <c r="L39">
+        <v>8.8559745096395096E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>457</v>
+      </c>
+      <c r="B40" s="11">
+        <v>13.6913485165172</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="11">
+        <v>-1.26274995775291E-4</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I40" s="11">
+        <v>-2.7754840618315701E-4</v>
+      </c>
+      <c r="J40" s="11">
+        <v>8.5616687138373102E-3</v>
+      </c>
+      <c r="K40" s="11">
+        <v>-8.4000287358655798E-4</v>
+      </c>
+      <c r="L40">
+        <v>3.9086879040320002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>442</v>
+      </c>
+      <c r="B41" s="11">
+        <v>12.668914949325</v>
+      </c>
+      <c r="C41" s="11">
+        <v>-7.8816161433989708E-3</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="11">
+        <v>-1.1614389368061701E-4</v>
+      </c>
+      <c r="G41" s="11">
+        <v>-3.72582925220617E-3</v>
+      </c>
+      <c r="H41" s="11">
+        <v>1.4845949725894099E-3</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J41" s="11">
+        <v>8.3059087769866997E-3</v>
+      </c>
+      <c r="K41" s="11">
+        <v>-1.10556489826584E-3</v>
+      </c>
+      <c r="L41">
+        <v>3.55257783815522E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>414</v>
+      </c>
+      <c r="B42" s="11">
+        <v>12.548012938183501</v>
+      </c>
+      <c r="C42" s="11">
+        <v>-6.6835771811303499E-3</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="11">
+        <v>-3.4227810960955603E-7</v>
+      </c>
+      <c r="F42" s="11">
+        <v>-1.14899608093455E-4</v>
+      </c>
+      <c r="G42" s="11">
+        <v>-3.6521784818772502E-3</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" s="11">
+        <v>7.9971310623995605E-3</v>
+      </c>
+      <c r="K42" s="11">
+        <v>-1.2008813565588801E-3</v>
+      </c>
+      <c r="L42">
+        <v>3.3274437595173602E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>412</v>
+      </c>
+      <c r="B43" s="11">
+        <v>12.8706734877037</v>
+      </c>
+      <c r="C43" s="11">
+        <v>-5.7333571960685404E-3</v>
+      </c>
+      <c r="D43" s="11">
+        <v>-2.0100716640069202E-3</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="11">
+        <v>-1.1779100757794399E-4</v>
+      </c>
+      <c r="G43" s="11">
+        <v>-2.9951338928099099E-3</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" s="11">
+        <v>8.5515852096896793E-3</v>
+      </c>
+      <c r="K43" s="11">
+        <v>-1.0485054959573001E-3</v>
+      </c>
+      <c r="L43">
+        <v>3.3108590822126999E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>474</v>
+      </c>
+      <c r="B44" s="11">
+        <v>12.203412151650101</v>
+      </c>
+      <c r="C44" s="11">
+        <v>-6.6987750581719401E-3</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F44" s="11">
+        <v>-1.11189944282559E-4</v>
+      </c>
+      <c r="G44" s="11">
+        <v>-3.6011187443048798E-3</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I44" s="11">
+        <v>-2.1970005569780001E-7</v>
+      </c>
+      <c r="J44" s="11">
+        <v>8.1822602798279093E-3</v>
+      </c>
+      <c r="K44" s="11">
+        <v>-1.10227617282494E-3</v>
+      </c>
+      <c r="L44">
+        <v>2.8861098774862599E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>458</v>
+      </c>
+      <c r="B45" s="11">
+        <v>13.362492790886799</v>
+      </c>
+      <c r="C45" s="11">
+        <v>-3.2835830629038701E-3</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="11">
+        <v>-1.22792049285E-4</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" s="11">
+        <v>-1.36845196802897E-4</v>
+      </c>
+      <c r="J45" s="11">
+        <v>8.2983232930694591E-3</v>
+      </c>
+      <c r="K45" s="11">
+        <v>-7.8439712462329599E-4</v>
+      </c>
+      <c r="L45">
+        <v>2.6801590006555201E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>427</v>
+      </c>
+      <c r="B46" s="11">
+        <v>15.712482738359499</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="11">
+        <v>-8.3779499907201908E-3</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="11">
+        <v>-1.4643067424642401E-4</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H46" s="11">
+        <v>-8.3198412283799598E-4</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J46" s="11">
+        <v>9.4998563183490703E-3</v>
+      </c>
+      <c r="K46" s="11">
+        <v>-8.7572285577487404E-4</v>
+      </c>
+      <c r="L46">
+        <v>2.0473486954457502E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>399</v>
+      </c>
+      <c r="B47" s="11">
+        <v>16.692819279833</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="11">
+        <v>-9.1529615648768096E-3</v>
+      </c>
+      <c r="E47" s="11">
+        <v>-2.8587048338658701E-7</v>
+      </c>
+      <c r="F47" s="11">
+        <v>-1.56789502445103E-4</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J47" s="11">
+        <v>9.5337004311087693E-3</v>
+      </c>
+      <c r="K47" s="11">
+        <v>-9.7464282233480795E-4</v>
+      </c>
+      <c r="L47">
+        <v>2.0290060899236601E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>411</v>
+      </c>
+      <c r="B48" s="11">
+        <v>16.364609687305101</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="11">
+        <v>-9.24282117747139E-3</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F48" s="11">
+        <v>-1.53167102547072E-4</v>
+      </c>
+      <c r="G48" s="11">
+        <v>2.0694220439543E-4</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="J48" s="11">
+        <v>9.7054910083236405E-3</v>
+      </c>
+      <c r="K48" s="11">
+        <v>-8.6381988833561995E-4</v>
+      </c>
+      <c r="L48">
+        <v>1.8285093453651501E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>460</v>
+      </c>
+      <c r="B49" s="11">
+        <v>14.701126711804999</v>
+      </c>
+      <c r="C49" s="11">
+        <v>-1.6307691413593099E-3</v>
+      </c>
+      <c r="D49" s="11">
+        <v>-5.6138266669088404E-3</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F49" s="11">
+        <v>-1.3595817354291299E-4</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I49" s="11">
+        <v>-1.21901158409955E-4</v>
+      </c>
+      <c r="J49" s="11">
+        <v>9.3525931796689405E-3</v>
+      </c>
+      <c r="K49" s="11">
+        <v>-7.7968330795068598E-4</v>
+      </c>
+      <c r="L49">
+        <v>1.6943086009582099E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B50" s="10">
+        <v>13.89</v>
+      </c>
+      <c r="C50" s="10">
+        <v>-3.6519999999999999E-3</v>
+      </c>
+      <c r="D50" s="10">
+        <v>-3.2820000000000002E-3</v>
+      </c>
+      <c r="E50" s="10">
+        <v>-1.719E-8</v>
+      </c>
+      <c r="F50" s="10">
+        <v>-1.281E-4</v>
+      </c>
+      <c r="G50" s="10">
+        <v>-1.498E-3</v>
+      </c>
+      <c r="H50" s="10">
+        <v>3.5710000000000002E-5</v>
+      </c>
+      <c r="I50" s="10">
+        <v>-3.8300000000000003E-5</v>
+      </c>
+      <c r="J50" s="10">
+        <v>8.7709999999999993E-3</v>
+      </c>
+      <c r="K50" s="10">
+        <v>-9.477E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CC06C8-D6DD-4712-AE2C-7A06B115AEAD}">
   <dimension ref="A1:J69"/>
   <sheetViews>
@@ -3529,11 +4931,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C9C45A-A9C7-442D-AE82-61DCD6C978E2}">
   <dimension ref="A1:V47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -4091,67 +5493,67 @@
       <c r="A17" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="33">
         <v>-6327</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="33">
         <v>167.5</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="33">
         <v>-0.26719999999999999</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="33">
         <v>1.911</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="33">
         <v>4.705E-3</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="33">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="33">
         <v>1.222E-2</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="33">
         <v>0.1014</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="33">
         <v>6.5340000000000005E-4</v>
       </c>
-      <c r="K17" s="32">
+      <c r="K17" s="33">
         <v>9.6550000000000004E-3</v>
       </c>
-      <c r="L17" s="32">
+      <c r="L17" s="33">
         <v>8.4720000000000004E-2</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="34">
         <v>2.2339999999999999E-3</v>
       </c>
-      <c r="N17" s="32">
+      <c r="N17" s="33">
         <v>7.5609999999999997E-2</v>
       </c>
-      <c r="O17" s="32">
+      <c r="O17" s="33">
         <v>0.23280000000000001</v>
       </c>
-      <c r="P17" s="32">
+      <c r="P17" s="33">
         <v>-0.14069999999999999</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="33">
         <v>0.82130000000000003</v>
       </c>
-      <c r="R17" s="32">
+      <c r="R17" s="33">
         <v>-598.70000000000005</v>
       </c>
-      <c r="S17" s="32">
+      <c r="S17" s="33">
         <v>46.15</v>
       </c>
-      <c r="T17" s="32">
+      <c r="T17" s="33">
         <v>1.069</v>
       </c>
-      <c r="U17" s="32">
+      <c r="U17" s="33">
         <v>1.804E-2</v>
       </c>
-      <c r="V17" s="32"/>
+      <c r="V17" s="33"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -4204,7 +5606,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A23" s="20">
+      <c r="A23" s="19">
         <v>402</v>
       </c>
       <c r="B23" s="11">
@@ -4252,7 +5654,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+      <c r="A24" s="19">
         <v>401</v>
       </c>
       <c r="B24" s="11">
@@ -4300,7 +5702,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
+      <c r="A25" s="19">
         <v>410</v>
       </c>
       <c r="B25" s="11">
@@ -4348,7 +5750,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
+      <c r="A26" s="19">
         <v>434</v>
       </c>
       <c r="B26" s="11">
@@ -4396,7 +5798,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
+      <c r="A27" s="19">
         <v>406</v>
       </c>
       <c r="B27" s="11">
@@ -4444,7 +5846,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
+      <c r="A28" s="19">
         <v>404</v>
       </c>
       <c r="B28" s="11">
@@ -4492,7 +5894,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="19">
         <v>466</v>
       </c>
       <c r="B29" s="11">
@@ -4540,7 +5942,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="20">
+      <c r="A30" s="19">
         <v>433</v>
       </c>
       <c r="B30" s="11">
@@ -5187,7 +6589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562815E0-203F-4D5B-96E0-A656DF752C95}">
   <dimension ref="A1:L88"/>
   <sheetViews>
@@ -7938,7 +9340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CEF00E-76FA-48D6-B21A-FF6CCE8B1018}">
   <dimension ref="A1:L36"/>
   <sheetViews>
@@ -8744,7 +10146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01171B25-C7B7-4B7E-9F18-D774EB4029E3}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -9055,7 +10457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
   <dimension ref="A1:I60"/>
   <sheetViews>
@@ -9074,7 +10476,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>261</v>
       </c>
     </row>
@@ -9082,15 +10484,15 @@
       <c r="A2" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -9115,7 +10517,7 @@
       <c r="A5" t="s">
         <v>266</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>22</v>
       </c>
       <c r="I5" t="s">
@@ -9131,7 +10533,7 @@
       <c r="A7" t="s">
         <v>267</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>268</v>
       </c>
     </row>
@@ -9156,7 +10558,7 @@
       <c r="A10" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>271</v>
       </c>
     </row>
@@ -9348,7 +10750,7 @@
       <c r="A31" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C31" t="s">
@@ -9371,7 +10773,7 @@
       <c r="A32" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="25" t="s">
         <v>268</v>
       </c>
       <c r="C32" t="s">
@@ -9394,7 +10796,7 @@
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="25" t="s">
         <v>271</v>
       </c>
       <c r="C33" t="s">
@@ -9417,7 +10819,7 @@
       <c r="A34" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>276</v>
       </c>
       <c r="C34" t="s">
@@ -9440,7 +10842,7 @@
       <c r="A35" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="25" t="s">
         <v>280</v>
       </c>
       <c r="C35" t="s">
@@ -9463,7 +10865,7 @@
       <c r="A36" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="25" t="s">
         <v>286</v>
       </c>
       <c r="C36" t="s">
@@ -9486,7 +10888,7 @@
       <c r="A37" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>291</v>
       </c>
       <c r="C37" t="s">
@@ -9509,7 +10911,7 @@
       <c r="A38" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>268</v>
       </c>
       <c r="C38" t="s">
@@ -9535,7 +10937,7 @@
       <c r="A39" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="25" t="s">
         <v>318</v>
       </c>
       <c r="C39" t="s">
@@ -9561,7 +10963,7 @@
       <c r="A40" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C40" t="s">
@@ -9584,7 +10986,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="24" t="s">
         <v>320</v>
       </c>
     </row>
@@ -9592,7 +10994,7 @@
       <c r="A42" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="25" t="s">
         <v>22</v>
       </c>
     </row>
@@ -9600,7 +11002,7 @@
       <c r="A43" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="25" t="s">
         <v>287</v>
       </c>
       <c r="C43" t="s">
@@ -9611,7 +11013,7 @@
       <c r="A44" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="25" t="s">
         <v>290</v>
       </c>
       <c r="C44" t="s">
@@ -9622,7 +11024,7 @@
       <c r="A45" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="25" t="s">
         <v>321</v>
       </c>
     </row>
@@ -9630,7 +11032,7 @@
       <c r="A46" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="25" t="s">
         <v>322</v>
       </c>
       <c r="C46" t="s">
@@ -9641,7 +11043,7 @@
       <c r="A47" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="25" t="s">
         <v>331</v>
       </c>
       <c r="C47" t="s">
@@ -9652,7 +11054,7 @@
       <c r="A48" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="25" t="s">
         <v>280</v>
       </c>
     </row>
@@ -9660,7 +11062,7 @@
       <c r="A49" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="25" t="s">
         <v>299</v>
       </c>
     </row>
@@ -9668,7 +11070,7 @@
       <c r="A50" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="25" t="s">
         <v>302</v>
       </c>
       <c r="C50" t="s">
@@ -9679,7 +11081,7 @@
       <c r="A51" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="25" t="s">
         <v>304</v>
       </c>
       <c r="C51" t="s">
@@ -11048,36 +12450,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC824D0-1825-4576-8153-73AE15FAEC82}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="3" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="30"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -11089,17 +12495,26 @@
       <c r="C2" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="E2" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="37" t="s">
+        <v>351</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>159</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -11108,10 +12523,12 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -11123,21 +12540,29 @@
       <c r="C4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="39" t="e">
+        <f>EXP(B4)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E4" s="16">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="E4" s="16">
+      <c r="F4" s="16">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="F4" s="16">
+      <c r="G4" s="39">
+        <f>EXP(E4)</f>
+        <v>0.98511193960306265</v>
+      </c>
+      <c r="H4" s="16">
         <v>-2.5999999999999999E-2</v>
       </c>
-      <c r="G4" s="16">
+      <c r="I4" s="16">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="J4">
-        <f>EXP(D4)</f>
-        <v>0.98511193960306265</v>
+      <c r="J4" s="40">
+        <f>EXP(H4)</f>
+        <v>0.97433508960874937</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
@@ -11150,21 +12575,29 @@
       <c r="C5" s="16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="39">
+        <f t="shared" ref="D5:D26" si="0">EXP(B5)</f>
+        <v>1.3099644507332473</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.25</v>
       </c>
-      <c r="E5" s="16">
+      <c r="F5" s="16">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="F5" s="16">
+      <c r="G5" s="39">
+        <f t="shared" ref="G5:G26" si="1">EXP(E5)</f>
+        <v>1.2840254166877414</v>
+      </c>
+      <c r="H5" s="16">
         <v>-3.4000000000000002E-2</v>
       </c>
-      <c r="G5" s="16">
+      <c r="I5" s="16">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="J5">
-        <f>EXP(D5)</f>
-        <v>1.2840254166877414</v>
+      <c r="J5" s="40">
+        <f t="shared" ref="J5:J26" si="2">EXP(H5)</f>
+        <v>0.96657150463750663</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -11177,21 +12610,29 @@
       <c r="C6" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>151</v>
+      <c r="D6" s="39" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" s="39" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H6" s="16">
         <v>-5.0000000000000002E-5</v>
       </c>
-      <c r="G6" s="16">
+      <c r="I6" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J6" t="e">
-        <f t="shared" ref="J6:J26" si="0">EXP(D6)</f>
-        <v>#VALUE!</v>
+      <c r="J6" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99995000124997913</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11204,21 +12645,29 @@
       <c r="C7" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>151</v>
+      <c r="D7" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0314855038865227</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G7" s="39" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="16">
         <v>-2.5999999999999999E-3</v>
       </c>
-      <c r="G7" s="16">
+      <c r="I7" s="16">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="J7" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="J7" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99740337707256976</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -11231,21 +12680,29 @@
       <c r="C8" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="39" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E8" s="16">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="E8" s="16">
+      <c r="F8" s="16">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F8" s="16">
+      <c r="G8" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0036064877830035</v>
+      </c>
+      <c r="H8" s="16">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="G8" s="16">
+      <c r="I8" s="16">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>1.0036064877830035</v>
+      <c r="J8" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0004000800106678</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -11258,21 +12715,29 @@
       <c r="C9" s="16">
         <v>0.85</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="39">
+        <f t="shared" si="0"/>
+        <v>1.1914489672789647E-2</v>
+      </c>
+      <c r="E9" s="16">
         <v>-6.09</v>
       </c>
-      <c r="E9" s="16">
+      <c r="F9" s="16">
         <v>0.81</v>
       </c>
-      <c r="F9" s="16">
+      <c r="G9" s="39">
+        <f t="shared" si="1"/>
+        <v>2.265408914814322E-3</v>
+      </c>
+      <c r="H9" s="16">
         <v>-7.68</v>
       </c>
-      <c r="G9" s="16">
+      <c r="I9" s="16">
         <v>0.95</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>2.265408914814322E-3</v>
+      <c r="J9" s="40">
+        <f t="shared" si="2"/>
+        <v>4.619748987816513E-4</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -11285,21 +12750,29 @@
       <c r="C10" s="16">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99970004499550036</v>
+      </c>
+      <c r="E10" s="17">
         <v>-4.0000000000000003E-5</v>
       </c>
-      <c r="E10" s="16">
+      <c r="F10" s="16">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F10" s="17">
+      <c r="G10" s="39">
+        <f t="shared" si="1"/>
+        <v>0.99996000079998937</v>
+      </c>
+      <c r="H10" s="17">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="G10" s="16">
+      <c r="I10" s="16">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>0.99996000079998937</v>
+      <c r="J10" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0000400008000108</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -11308,12 +12781,20 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="D11" s="39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="J11">
-        <f t="shared" si="0"/>
+      <c r="G11" s="39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="40">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11322,26 +12803,34 @@
         <v>183</v>
       </c>
       <c r="B12" s="16">
-        <v>2.5999999999999999E-2</v>
+        <v>-3.3019999999999998E-3</v>
       </c>
       <c r="C12" s="16">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="D12" s="16">
+        <v>5.6969999999999998E-3</v>
+      </c>
+      <c r="D12" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99670344560655344</v>
+      </c>
+      <c r="E12" s="16">
         <v>7.0400000000000003E-3</v>
       </c>
-      <c r="E12" s="16">
+      <c r="F12" s="16">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="F12" s="16">
-        <v>-3.65E-3</v>
-      </c>
-      <c r="G12" s="16">
-        <v>3.29E-3</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
+      <c r="G12" s="39">
+        <f t="shared" si="1"/>
         <v>1.0070648390547696</v>
+      </c>
+      <c r="H12" s="16">
+        <v>-3.6519999999999999E-3</v>
+      </c>
+      <c r="I12" s="16">
+        <v>3.2989999999999998E-3</v>
+      </c>
+      <c r="J12" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99635466044155552</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11349,26 +12838,34 @@
         <v>184</v>
       </c>
       <c r="B13" s="16">
-        <v>-7.0000000000000001E-3</v>
+        <v>9.3240000000000007E-3</v>
       </c>
       <c r="C13" s="16">
-        <v>2.8E-3</v>
-      </c>
-      <c r="D13" s="16">
+        <v>1.98E-3</v>
+      </c>
+      <c r="D13" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0093676039035671</v>
+      </c>
+      <c r="E13" s="16">
         <v>-4.2900000000000004E-3</v>
       </c>
-      <c r="E13" s="16">
+      <c r="F13" s="16">
         <v>2.7200000000000002E-3</v>
       </c>
-      <c r="F13" s="16">
-        <v>3.57E-5</v>
-      </c>
-      <c r="G13" s="16">
-        <v>5.7899999999999998E-4</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
+      <c r="G13" s="39">
+        <f t="shared" si="1"/>
         <v>0.99571918890516931</v>
+      </c>
+      <c r="H13" s="16">
+        <v>3.5710000000000002E-5</v>
+      </c>
+      <c r="I13" s="16">
+        <v>5.7959999999999999E-4</v>
+      </c>
+      <c r="J13" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0000357106376097</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11376,26 +12873,34 @@
         <v>185</v>
       </c>
       <c r="B14" s="16">
-        <v>-8.9999999999999998E-4</v>
+        <v>1.2470000000000001E-3</v>
       </c>
       <c r="C14" s="16">
-        <v>3.1E-4</v>
-      </c>
-      <c r="D14" s="16">
+        <v>2.352E-4</v>
+      </c>
+      <c r="D14" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0012477778277835</v>
+      </c>
+      <c r="E14" s="16">
         <v>1.8900000000000001E-4</v>
       </c>
-      <c r="E14" s="16">
+      <c r="F14" s="16">
         <v>2.206E-4</v>
       </c>
-      <c r="F14" s="16">
+      <c r="G14" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0001890178616253</v>
+      </c>
+      <c r="H14" s="16">
         <v>-3.8300000000000003E-5</v>
       </c>
-      <c r="G14" s="16">
-        <v>9.1299999999999997E-5</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
-        <v>1.0001890178616253</v>
+      <c r="I14" s="16">
+        <v>9.1260000000000004E-5</v>
+      </c>
+      <c r="J14" s="40">
+        <f t="shared" si="2"/>
+        <v>0.9999617007334356</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11403,26 +12908,34 @@
         <v>186</v>
       </c>
       <c r="B15" s="16">
-        <v>1.336E-2</v>
+        <v>-4.621E-5</v>
       </c>
       <c r="C15" s="16">
-        <v>1.5E-3</v>
-      </c>
-      <c r="D15" s="16">
+        <v>1.931E-3</v>
+      </c>
+      <c r="D15" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99995379106766558</v>
+      </c>
+      <c r="E15" s="16">
         <v>7.084E-3</v>
       </c>
-      <c r="E15" s="16">
+      <c r="F15" s="16">
         <v>1.268E-3</v>
       </c>
-      <c r="F15" s="16">
-        <v>8.77E-3</v>
-      </c>
-      <c r="G15" s="16">
+      <c r="G15" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0071091508825412</v>
+      </c>
+      <c r="H15" s="16">
+        <v>8.7709999999999993E-3</v>
+      </c>
+      <c r="I15" s="16">
         <v>1.24E-3</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
-        <v>1.0071091508825412</v>
+      <c r="J15" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0088095779270116</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11430,26 +12943,34 @@
         <v>187</v>
       </c>
       <c r="B16" s="16">
-        <v>6.5900000000000004E-3</v>
+        <v>-9.953E-3</v>
       </c>
       <c r="C16" s="16">
-        <v>2.9499999999999999E-3</v>
-      </c>
-      <c r="D16" s="16">
+        <v>1.751E-3</v>
+      </c>
+      <c r="D16" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99009636718488148</v>
+      </c>
+      <c r="E16" s="16">
         <v>6.7200000000000003E-3</v>
       </c>
-      <c r="E16" s="16">
+      <c r="F16" s="16">
         <v>2.64E-3</v>
       </c>
-      <c r="F16" s="16">
+      <c r="G16" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0067426298624924</v>
+      </c>
+      <c r="H16" s="16">
         <v>-1.49E-3</v>
       </c>
-      <c r="G16" s="16">
+      <c r="I16" s="16">
         <v>2.0300000000000001E-3</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
-        <v>1.0067426298624924</v>
+      <c r="J16" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99851110949888044</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -11458,21 +12979,26 @@
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="16">
+      <c r="D17" s="39"/>
+      <c r="E17" s="16">
         <v>4.2200000000000001E-4</v>
       </c>
-      <c r="E17" s="16">
+      <c r="F17" s="16">
         <v>1.4400000000000001E-3</v>
       </c>
-      <c r="F17" s="16">
+      <c r="G17" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0004220890545266</v>
+      </c>
+      <c r="H17" s="16">
         <v>-3.2799999999999999E-3</v>
       </c>
-      <c r="G17" s="16">
+      <c r="I17" s="16">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
-        <v>1.0004220890545266</v>
+      <c r="J17" s="40">
+        <f>EXP(H17)</f>
+        <v>0.99672537332356081</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -11485,21 +13011,29 @@
       <c r="C18" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="39" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E18" s="16">
         <v>1.8680000000000001E-7</v>
       </c>
-      <c r="E18" s="16">
+      <c r="F18" s="16">
         <v>5.0299999999999999E-7</v>
       </c>
-      <c r="F18" s="16">
+      <c r="G18" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0000001868000175</v>
+      </c>
+      <c r="H18" s="16">
         <v>-1.7199999999999999E-8</v>
       </c>
-      <c r="G18" s="16">
+      <c r="I18" s="16">
         <v>1.6E-7</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
-        <v>1.0000001868000175</v>
+      <c r="J18" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99999998280000013</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -11507,26 +13041,34 @@
         <v>113</v>
       </c>
       <c r="B19" s="16">
-        <v>-1.6899999999999999E-4</v>
+        <v>-1.3909999999999999E-4</v>
       </c>
       <c r="C19" s="16">
-        <v>3.6600000000000002E-5</v>
-      </c>
-      <c r="D19" s="16">
+        <v>2.41E-5</v>
+      </c>
+      <c r="D19" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99986090967395647</v>
+      </c>
+      <c r="E19" s="16">
         <v>-1.7469999999999999E-4</v>
       </c>
-      <c r="E19" s="16">
+      <c r="F19" s="16">
         <v>2.51E-5</v>
       </c>
-      <c r="F19" s="16">
+      <c r="G19" s="39">
+        <f t="shared" si="1"/>
+        <v>0.99982531525915641</v>
+      </c>
+      <c r="H19" s="16">
         <v>-1.2799999999999999E-4</v>
       </c>
-      <c r="G19" s="16">
+      <c r="I19" s="16">
         <v>2.55E-5</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
-        <v>0.99982531525915641</v>
+      <c r="J19" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99987200819165045</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -11535,12 +13077,20 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="D20" s="39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="J20">
-        <f t="shared" si="0"/>
+      <c r="G20" s="39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="40">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -11554,21 +13104,29 @@
       <c r="C21" s="16">
         <v>3.5500000000000002E-3</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0041586231745985</v>
+      </c>
+      <c r="E21" s="16">
         <v>1.093E-2</v>
       </c>
-      <c r="E21" s="16">
+      <c r="F21" s="16">
         <v>2.395E-3</v>
       </c>
-      <c r="F21" s="16">
+      <c r="G21" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0109899506711895</v>
+      </c>
+      <c r="H21" s="16">
         <v>1.439E-4</v>
       </c>
-      <c r="G21" s="16">
+      <c r="I21" s="16">
         <v>8.1450000000000001E-4</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
-        <v>1.0109899506711895</v>
+      <c r="J21" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0001439103541017</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -11581,21 +13139,29 @@
       <c r="C22" s="16">
         <v>4.3600000000000002E-3</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="39">
+        <f t="shared" si="0"/>
+        <v>0.97565133024224471</v>
+      </c>
+      <c r="E22" s="16">
         <v>4.5199999999999997E-3</v>
       </c>
-      <c r="E22" s="16">
+      <c r="F22" s="16">
         <v>5.6389999999999999E-3</v>
       </c>
-      <c r="F22" s="16">
+      <c r="G22" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0045302306083088</v>
+      </c>
+      <c r="H22" s="16">
         <v>1.2579999999999999E-2</v>
       </c>
-      <c r="G22" s="16">
+      <c r="I22" s="16">
         <v>4.7349999999999996E-3</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
-        <v>1.0045302306083088</v>
+      <c r="J22" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0126594610570951</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -11608,21 +13174,29 @@
       <c r="C23" s="16">
         <v>4.0099999999999997E-3</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0348329368321532</v>
+      </c>
+      <c r="E23" s="16">
         <v>-7.4629999999999998E-4</v>
       </c>
-      <c r="E23" s="16">
+      <c r="F23" s="16">
         <v>2.2780000000000001E-3</v>
       </c>
-      <c r="F23" s="16">
+      <c r="G23" s="39">
+        <f t="shared" si="1"/>
+        <v>0.9992539784125809</v>
+      </c>
+      <c r="H23" s="16">
         <v>-4.3049999999999998E-3</v>
       </c>
-      <c r="G23" s="16">
+      <c r="I23" s="16">
         <v>4.6719999999999999E-3</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
-        <v>0.9992539784125809</v>
+      <c r="J23" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99570425322935363</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -11635,21 +13209,29 @@
       <c r="C24" s="16">
         <v>9.7419999999999999E-5</v>
       </c>
-      <c r="D24" s="16">
+      <c r="D24" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0000361306526964</v>
+      </c>
+      <c r="E24" s="16">
         <v>1.5640000000000001E-4</v>
       </c>
-      <c r="E24" s="16">
+      <c r="F24" s="16">
         <v>1.7550000000000001E-4</v>
       </c>
-      <c r="F24" s="16">
+      <c r="G24" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0001564122311177</v>
+      </c>
+      <c r="H24" s="16">
         <v>4.899E-6</v>
       </c>
-      <c r="G24" s="16">
+      <c r="I24" s="16">
         <v>5.8400000000000003E-5</v>
       </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
-        <v>1.0001564122311177</v>
+      <c r="J24" s="40">
+        <f t="shared" si="2"/>
+        <v>1.0000048990120001</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -11662,21 +13244,29 @@
       <c r="C25" s="16">
         <v>1.2340000000000001E-3</v>
       </c>
-      <c r="D25" s="16">
+      <c r="D25" s="39">
+        <f t="shared" si="0"/>
+        <v>1.0003212515902435</v>
+      </c>
+      <c r="E25" s="16">
         <v>5.5550000000000002E-5</v>
       </c>
-      <c r="E25" s="16">
+      <c r="F25" s="16">
         <v>7.5509999999999998E-4</v>
       </c>
-      <c r="F25" s="16">
+      <c r="G25" s="39">
+        <f t="shared" si="1"/>
+        <v>1.0000555515429299</v>
+      </c>
+      <c r="H25" s="16">
         <v>-1.7909999999999999E-2</v>
       </c>
-      <c r="G25" s="16">
+      <c r="I25" s="16">
         <v>2.1419999999999998E-3</v>
       </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
-        <v>1.0000555515429299</v>
+      <c r="J25" s="40">
+        <f t="shared" si="2"/>
+        <v>0.98224943082908445</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -11689,28 +13279,40 @@
       <c r="C26" s="16">
         <v>2.3779999999999999E-5</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="39">
+        <f t="shared" si="0"/>
+        <v>0.99977342567184091</v>
+      </c>
+      <c r="E26" s="16">
         <v>-1.529E-4</v>
       </c>
-      <c r="E26" s="16">
+      <c r="F26" s="16">
         <v>2.124E-5</v>
       </c>
-      <c r="F26" s="16">
+      <c r="G26" s="39">
+        <f t="shared" si="1"/>
+        <v>0.99984711168860929</v>
+      </c>
+      <c r="H26" s="16">
         <v>-1.3070000000000001E-4</v>
       </c>
-      <c r="G26" s="16">
+      <c r="I26" s="16">
         <v>2.035E-5</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="0"/>
-        <v>0.99984711168860929</v>
-      </c>
+      <c r="J26" s="40">
+        <f t="shared" si="2"/>
+        <v>0.99986930854087286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D27" s="38"/>
+      <c r="G27" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11718,6 +13320,367 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9FA71-8CE5-4C6B-887E-5FA553777DF5}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3">
+        <v>0.98511193960306265</v>
+      </c>
+      <c r="D3">
+        <v>0.97433508960874937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4">
+        <v>1.3099644507332473</v>
+      </c>
+      <c r="C4">
+        <v>1.2840254166877414</v>
+      </c>
+      <c r="D4">
+        <v>0.96657150463750663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5">
+        <v>0.99995000124997913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>1.0314855038865227</v>
+      </c>
+      <c r="D6">
+        <v>0.99740337707256976</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7">
+        <v>1.0036064877830035</v>
+      </c>
+      <c r="D7">
+        <v>1.0004000800106678</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>1.1914489672789647E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.265408914814322E-3</v>
+      </c>
+      <c r="D8">
+        <v>4.619748987816513E-4</v>
+      </c>
+      <c r="G8">
+        <f>G7*B8</f>
+        <v>1.1914489672789648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9">
+        <v>0.99970004499550036</v>
+      </c>
+      <c r="C9">
+        <v>0.99996000079998937</v>
+      </c>
+      <c r="D9">
+        <v>1.0000400008000108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B11" s="16">
+        <v>0.99670344560655344</v>
+      </c>
+      <c r="C11">
+        <v>1.0070648390547696</v>
+      </c>
+      <c r="D11">
+        <v>0.99635466044155552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="16">
+        <v>1.0093676039035671</v>
+      </c>
+      <c r="C12">
+        <v>0.99571918890516931</v>
+      </c>
+      <c r="D12">
+        <v>1.0000357106376097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1.0012477778277835</v>
+      </c>
+      <c r="C13">
+        <v>1.0001890178616253</v>
+      </c>
+      <c r="D13">
+        <v>0.9999617007334356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" s="16">
+        <v>0.99995379106766558</v>
+      </c>
+      <c r="C14">
+        <v>1.0071091508825412</v>
+      </c>
+      <c r="D14">
+        <v>1.0088095779270116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.99009636718488148</v>
+      </c>
+      <c r="C15">
+        <v>1.0067426298624924</v>
+      </c>
+      <c r="D15">
+        <v>0.99851110949888044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16">
+        <v>1.0004220890545266</v>
+      </c>
+      <c r="D16">
+        <v>0.99672537332356081</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="16" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C17">
+        <v>1.0000001868000175</v>
+      </c>
+      <c r="D17">
+        <v>0.99999998280000013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B18" s="16">
+        <v>0.99986090967395647</v>
+      </c>
+      <c r="C18">
+        <v>0.99982531525915641</v>
+      </c>
+      <c r="D18">
+        <v>0.99987200819165045</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>1.0041586231745985</v>
+      </c>
+      <c r="C20">
+        <v>1.0109899506711895</v>
+      </c>
+      <c r="D20">
+        <v>1.0001439103541017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B21">
+        <v>0.97565133024224471</v>
+      </c>
+      <c r="C21">
+        <v>1.0045302306083088</v>
+      </c>
+      <c r="D21">
+        <v>1.0126594610570951</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22">
+        <v>1.0348329368321532</v>
+      </c>
+      <c r="C22">
+        <v>0.9992539784125809</v>
+      </c>
+      <c r="D22">
+        <v>0.99570425322935363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23">
+        <v>1.0000361306526964</v>
+      </c>
+      <c r="C23">
+        <v>1.0001564122311177</v>
+      </c>
+      <c r="D23">
+        <v>1.0000048990120001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>1.0003212515902435</v>
+      </c>
+      <c r="C24">
+        <v>1.0000555515429299</v>
+      </c>
+      <c r="D24">
+        <v>0.98224943082908445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25">
+        <v>0.99977342567184091</v>
+      </c>
+      <c r="C25">
+        <v>0.99984711168860929</v>
+      </c>
+      <c r="D25">
+        <v>0.99986930854087286</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B11:D18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -11746,19 +13709,19 @@
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>159</v>
       </c>
     </row>
@@ -11892,15 +13855,15 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22">
         <v>9.2510000000000005E-3</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <v>1.4290000000000001E-2</v>
       </c>
     </row>
@@ -12065,7 +14028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858278ED-196A-4B59-8830-674E5B382BAC}">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -12513,7 +14476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661002B2-E508-42DE-AAF7-55B64A4B61E8}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -12771,7 +14734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED94DC-32EE-4CB2-B393-F68209908457}">
   <dimension ref="A1:K58"/>
   <sheetViews>
@@ -14334,1371 +16297,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B568554-EE5E-4148-B92D-3C63A1452433}">
-  <dimension ref="A1:L50"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E7" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B9" s="10">
-        <v>17.18</v>
-      </c>
-      <c r="C9" s="10">
-        <v>2.5569999999999999E-2</v>
-      </c>
-      <c r="D9" s="10">
-        <v>6.5979999999999997E-3</v>
-      </c>
-      <c r="E9" s="10">
-        <v>-6.5440000000000003E-3</v>
-      </c>
-      <c r="F9" s="10">
-        <v>-8.9479999999999996E-4</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1.336E-2</v>
-      </c>
-      <c r="H9" s="10">
-        <v>-1.698</v>
-      </c>
-      <c r="I9" s="10">
-        <v>5.0750000000000003E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" t="s">
-        <v>216</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" t="s">
-        <v>222</v>
-      </c>
-      <c r="F13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="K13" t="s">
-        <v>205</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
-        <v>186</v>
-      </c>
-      <c r="B15" s="11">
-        <v>19.009683355491202</v>
-      </c>
-      <c r="C15" s="11">
-        <v>1.29608290177501E-2</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F15" s="11">
-        <v>-1.84532899937581E-4</v>
-      </c>
-      <c r="G15" s="11">
-        <v>8.9895527555435301E-3</v>
-      </c>
-      <c r="H15" s="11">
-        <v>-6.7625486018793599E-3</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J15" s="11">
-        <v>7.3849377864736903E-3</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L15" s="10">
-        <v>0.266233744495813</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
-        <v>249</v>
-      </c>
-      <c r="B16" s="11">
-        <v>17.791917474132401</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F16" s="11">
-        <v>-1.7143199173686401E-4</v>
-      </c>
-      <c r="G16" s="11">
-        <v>4.09785003072615E-3</v>
-      </c>
-      <c r="H16" s="11">
-        <v>-1.5871515486556901E-3</v>
-      </c>
-      <c r="I16" s="11">
-        <v>4.39231821585213E-4</v>
-      </c>
-      <c r="J16" s="11">
-        <v>6.72550356216593E-3</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L16" s="10">
-        <v>0.178477643773784</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
-        <v>250</v>
-      </c>
-      <c r="B17" s="11">
-        <v>18.238780266223401</v>
-      </c>
-      <c r="C17" s="11">
-        <v>7.2257116178215302E-3</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F17" s="11">
-        <v>-1.7614452199371801E-4</v>
-      </c>
-      <c r="G17" s="11">
-        <v>6.7506961184131001E-3</v>
-      </c>
-      <c r="H17" s="11">
-        <v>-4.4415916510793501E-3</v>
-      </c>
-      <c r="I17" s="11">
-        <v>2.2030303542616499E-4</v>
-      </c>
-      <c r="J17" s="11">
-        <v>6.8796476315811997E-3</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L17" s="10">
-        <v>8.1447073791342306E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="14">
-        <v>446</v>
-      </c>
-      <c r="B18" s="11">
-        <v>16.292790577390001</v>
-      </c>
-      <c r="C18" s="11">
-        <v>1.09740411901045E-2</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E18" s="11">
-        <v>1.41862161101489E-6</v>
-      </c>
-      <c r="F18" s="11">
-        <v>-1.5489787022817899E-4</v>
-      </c>
-      <c r="G18" s="11">
-        <v>8.4352556606180195E-3</v>
-      </c>
-      <c r="H18" s="11">
-        <v>-5.5961388582716001E-3</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J18" s="11">
-        <v>8.1371661521309306E-3</v>
-      </c>
-      <c r="K18" s="11">
-        <v>7.0453351777090495E-4</v>
-      </c>
-      <c r="L18" s="10">
-        <v>8.0380629516945801E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>442</v>
-      </c>
-      <c r="B19" s="11">
-        <v>18.933888188050801</v>
-      </c>
-      <c r="C19" s="11">
-        <v>1.27204007729679E-2</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="11">
-        <v>-1.83613354627066E-4</v>
-      </c>
-      <c r="G19" s="11">
-        <v>9.2651727566647798E-3</v>
-      </c>
-      <c r="H19" s="11">
-        <v>-6.7871509061906699E-3</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J19" s="11">
-        <v>7.4565847270431198E-3</v>
-      </c>
-      <c r="K19" s="11">
-        <v>3.6907273823718299E-4</v>
-      </c>
-      <c r="L19" s="10">
-        <v>7.3310335878910393E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>251</v>
-      </c>
-      <c r="B20" s="11">
-        <v>17.249397001262501</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="11">
-        <v>3.8451081773854799E-3</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F20" s="11">
-        <v>-1.6666525775224701E-4</v>
-      </c>
-      <c r="G20" s="11">
-        <v>4.1277007854361204E-3</v>
-      </c>
-      <c r="H20" s="11">
-        <v>-1.9347858632567899E-3</v>
-      </c>
-      <c r="I20" s="11">
-        <v>4.0482648807792102E-4</v>
-      </c>
-      <c r="J20" s="11">
-        <v>5.9564273387460098E-3</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L20" s="10">
-        <v>7.2547265918478904E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>190</v>
-      </c>
-      <c r="B21" s="11">
-        <v>17.891599666362001</v>
-      </c>
-      <c r="C21" s="11">
-        <v>1.2108022021667501E-2</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E21" s="11">
-        <v>7.23686347282587E-7</v>
-      </c>
-      <c r="F21" s="11">
-        <v>-1.72433083556121E-4</v>
-      </c>
-      <c r="G21" s="11">
-        <v>8.3822834474565101E-3</v>
-      </c>
-      <c r="H21" s="11">
-        <v>-6.0963889412872204E-3</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J21" s="11">
-        <v>7.6684196861511204E-3</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L21" s="10">
-        <v>6.9527526338365897E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>188</v>
-      </c>
-      <c r="B22" s="11">
-        <v>18.5920030366721</v>
-      </c>
-      <c r="C22" s="11">
-        <v>1.2207173055958E-2</v>
-      </c>
-      <c r="D22" s="11">
-        <v>2.0443801661234398E-3</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F22" s="11">
-        <v>-1.80610406572904E-4</v>
-      </c>
-      <c r="G22" s="11">
-        <v>8.7601465733685192E-3</v>
-      </c>
-      <c r="H22" s="11">
-        <v>-6.66542893793201E-3</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J22" s="11">
-        <v>7.0199032768215397E-3</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L22" s="10">
-        <v>4.0171754058928102E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>218</v>
-      </c>
-      <c r="B23" s="11">
-        <v>17.811374600908302</v>
-      </c>
-      <c r="C23" s="11">
-        <v>-2.75211460807106E-3</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="11">
-        <v>-1.71820579369805E-4</v>
-      </c>
-      <c r="G23" s="11">
-        <v>2.8246973996307301E-3</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I23" s="11">
-        <v>5.2987624187635801E-4</v>
-      </c>
-      <c r="J23" s="11">
-        <v>6.6093939776072199E-3</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L23" s="10">
-        <v>3.2169456070832797E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>217</v>
-      </c>
-      <c r="B24" s="11">
-        <v>17.982687422475699</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="11">
-        <v>-1.7365512747779201E-4</v>
-      </c>
-      <c r="G24" s="11">
-        <v>3.13788101386714E-3</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I24" s="11">
-        <v>4.5986822953149602E-4</v>
-      </c>
-      <c r="J24" s="11">
-        <v>6.35203075536448E-3</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L24" s="10">
-        <v>3.0135542544931199E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>253</v>
-      </c>
-      <c r="B25" s="11">
-        <v>17.3599049168132</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="11">
-        <v>3.0202037120308401E-7</v>
-      </c>
-      <c r="F25" s="11">
-        <v>-1.6676584263045999E-4</v>
-      </c>
-      <c r="G25" s="11">
-        <v>3.9975876375509898E-3</v>
-      </c>
-      <c r="H25" s="11">
-        <v>-1.45756291327818E-3</v>
-      </c>
-      <c r="I25" s="11">
-        <v>4.22830045051132E-4</v>
-      </c>
-      <c r="J25" s="11">
-        <v>6.90671508065428E-3</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L25" s="10">
-        <v>2.26474393626315E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>505</v>
-      </c>
-      <c r="B26" s="11">
-        <v>17.848673967184599</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F26" s="11">
-        <v>-1.7203748206080601E-4</v>
-      </c>
-      <c r="G26" s="11">
-        <v>4.2449302038568898E-3</v>
-      </c>
-      <c r="H26" s="11">
-        <v>-1.6423675450923201E-3</v>
-      </c>
-      <c r="I26" s="11">
-        <v>4.30725117609008E-4</v>
-      </c>
-      <c r="J26" s="11">
-        <v>6.8075216947054203E-3</v>
-      </c>
-      <c r="K26" s="11">
-        <v>1.2572313639363399E-4</v>
-      </c>
-      <c r="L26" s="10">
-        <v>2.1730668619851401E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>221</v>
-      </c>
-      <c r="B27" s="11">
-        <v>16.911549401152701</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="11">
-        <v>9.5109173465066103E-7</v>
-      </c>
-      <c r="F27" s="11">
-        <v>-1.6215742624764499E-4</v>
-      </c>
-      <c r="G27" s="11">
-        <v>3.1039446438607802E-3</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I27" s="11">
-        <v>4.0263140725682801E-4</v>
-      </c>
-      <c r="J27" s="11">
-        <v>7.0342366376967601E-3</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L27" s="10">
-        <v>1.6463050402586301E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>220</v>
-      </c>
-      <c r="B28" s="11">
-        <v>17.224218560369501</v>
-      </c>
-      <c r="C28" s="11">
-        <v>-3.9155880576206897E-3</v>
-      </c>
-      <c r="D28" s="11">
-        <v>4.1841045266635003E-3</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F28" s="11">
-        <v>-1.66687416045079E-4</v>
-      </c>
-      <c r="G28" s="11">
-        <v>2.4886482796275598E-3</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I28" s="11">
-        <v>5.2644999811742998E-4</v>
-      </c>
-      <c r="J28" s="11">
-        <v>5.7417922381403502E-3</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="L28" s="10">
-        <v>1.47578692265985E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B29" s="10">
-        <v>18.09</v>
-      </c>
-      <c r="C29" s="10">
-        <v>7.0400000000000003E-3</v>
-      </c>
-      <c r="D29" s="10">
-        <v>4.2279999999999998E-4</v>
-      </c>
-      <c r="E29" s="10">
-        <v>1.8680000000000001E-7</v>
-      </c>
-      <c r="F29" s="10">
-        <v>-1.7469999999999999E-4</v>
-      </c>
-      <c r="G29" s="10">
-        <v>6.7219999999999997E-3</v>
-      </c>
-      <c r="H29" s="10">
-        <v>-4.2940000000000001E-3</v>
-      </c>
-      <c r="I29" s="10">
-        <v>1.8990000000000001E-4</v>
-      </c>
-      <c r="J29" s="10">
-        <v>7.084E-3</v>
-      </c>
-      <c r="K29" s="10">
-        <v>8.6420000000000003E-5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" t="s">
-        <v>224</v>
-      </c>
-      <c r="C33" t="s">
-        <v>216</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E33" t="s">
-        <v>222</v>
-      </c>
-      <c r="F33" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="K33" t="s">
-        <v>205</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>410</v>
-      </c>
-      <c r="B35" s="11">
-        <v>12.2030866660689</v>
-      </c>
-      <c r="C35" s="11">
-        <v>-6.7019935890024699E-3</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F35" s="11">
-        <v>-1.1118693345988001E-4</v>
-      </c>
-      <c r="G35" s="11">
-        <v>-3.6025136466945299E-3</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J35" s="11">
-        <v>8.18196829626564E-3</v>
-      </c>
-      <c r="K35" s="11">
-        <v>-1.1024210994762E-3</v>
-      </c>
-      <c r="L35">
-        <v>0.290088335638363</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36">
-        <v>395</v>
-      </c>
-      <c r="B36" s="11">
-        <v>16.331518985578501</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D36" s="11">
-        <v>-9.2205756109065493E-3</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F36" s="11">
-        <v>-1.5286706634028499E-4</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J36" s="11">
-        <v>9.7018334379725905E-3</v>
-      </c>
-      <c r="K36" s="11">
-        <v>-8.8792403223106504E-4</v>
-      </c>
-      <c r="L36">
-        <v>0.133297053622733</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>459</v>
-      </c>
-      <c r="B37" s="11">
-        <v>15.177145875226801</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D37" s="11">
-        <v>-6.7163087448920402E-3</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F37" s="11">
-        <v>-1.4083336345925901E-4</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I37" s="11">
-        <v>-1.7429952558927801E-4</v>
-      </c>
-      <c r="J37" s="11">
-        <v>9.6427767895367993E-3</v>
-      </c>
-      <c r="K37" s="11">
-        <v>-8.0688455088703196E-4</v>
-      </c>
-      <c r="L37">
-        <v>0.12458991421073499</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>396</v>
-      </c>
-      <c r="B38" s="11">
-        <v>14.7796214596646</v>
-      </c>
-      <c r="C38" s="11">
-        <v>-3.0024683268318102E-3</v>
-      </c>
-      <c r="D38" s="11">
-        <v>-5.8202868137717401E-3</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F38" s="11">
-        <v>-1.3683483081216799E-4</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J38" s="11">
-        <v>9.1604464318543102E-3</v>
-      </c>
-      <c r="K38" s="11">
-        <v>-7.9094434579269799E-4</v>
-      </c>
-      <c r="L38">
-        <v>9.0814849494256097E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>394</v>
-      </c>
-      <c r="B39" s="11">
-        <v>13.4169021279987</v>
-      </c>
-      <c r="C39" s="11">
-        <v>-4.8970846317684903E-3</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F39" s="11">
-        <v>-1.23464167016551E-4</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J39" s="11">
-        <v>8.0177530532582197E-3</v>
-      </c>
-      <c r="K39" s="11">
-        <v>-7.9967030200243396E-4</v>
-      </c>
-      <c r="L39">
-        <v>8.8559745096395096E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>457</v>
-      </c>
-      <c r="B40" s="11">
-        <v>13.6913485165172</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="11">
-        <v>-1.26274995775291E-4</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I40" s="11">
-        <v>-2.7754840618315701E-4</v>
-      </c>
-      <c r="J40" s="11">
-        <v>8.5616687138373102E-3</v>
-      </c>
-      <c r="K40" s="11">
-        <v>-8.4000287358655798E-4</v>
-      </c>
-      <c r="L40">
-        <v>3.9086879040320002E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>442</v>
-      </c>
-      <c r="B41" s="11">
-        <v>12.668914949325</v>
-      </c>
-      <c r="C41" s="11">
-        <v>-7.8816161433989708E-3</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F41" s="11">
-        <v>-1.1614389368061701E-4</v>
-      </c>
-      <c r="G41" s="11">
-        <v>-3.72582925220617E-3</v>
-      </c>
-      <c r="H41" s="11">
-        <v>1.4845949725894099E-3</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J41" s="11">
-        <v>8.3059087769866997E-3</v>
-      </c>
-      <c r="K41" s="11">
-        <v>-1.10556489826584E-3</v>
-      </c>
-      <c r="L41">
-        <v>3.55257783815522E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>414</v>
-      </c>
-      <c r="B42" s="11">
-        <v>12.548012938183501</v>
-      </c>
-      <c r="C42" s="11">
-        <v>-6.6835771811303499E-3</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E42" s="11">
-        <v>-3.4227810960955603E-7</v>
-      </c>
-      <c r="F42" s="11">
-        <v>-1.14899608093455E-4</v>
-      </c>
-      <c r="G42" s="11">
-        <v>-3.6521784818772502E-3</v>
-      </c>
-      <c r="H42" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J42" s="11">
-        <v>7.9971310623995605E-3</v>
-      </c>
-      <c r="K42" s="11">
-        <v>-1.2008813565588801E-3</v>
-      </c>
-      <c r="L42">
-        <v>3.3274437595173602E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>412</v>
-      </c>
-      <c r="B43" s="11">
-        <v>12.8706734877037</v>
-      </c>
-      <c r="C43" s="11">
-        <v>-5.7333571960685404E-3</v>
-      </c>
-      <c r="D43" s="11">
-        <v>-2.0100716640069202E-3</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="11">
-        <v>-1.1779100757794399E-4</v>
-      </c>
-      <c r="G43" s="11">
-        <v>-2.9951338928099099E-3</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J43" s="11">
-        <v>8.5515852096896793E-3</v>
-      </c>
-      <c r="K43" s="11">
-        <v>-1.0485054959573001E-3</v>
-      </c>
-      <c r="L43">
-        <v>3.3108590822126999E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>474</v>
-      </c>
-      <c r="B44" s="11">
-        <v>12.203412151650101</v>
-      </c>
-      <c r="C44" s="11">
-        <v>-6.6987750581719401E-3</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F44" s="11">
-        <v>-1.11189944282559E-4</v>
-      </c>
-      <c r="G44" s="11">
-        <v>-3.6011187443048798E-3</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I44" s="11">
-        <v>-2.1970005569780001E-7</v>
-      </c>
-      <c r="J44" s="11">
-        <v>8.1822602798279093E-3</v>
-      </c>
-      <c r="K44" s="11">
-        <v>-1.10227617282494E-3</v>
-      </c>
-      <c r="L44">
-        <v>2.8861098774862599E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>458</v>
-      </c>
-      <c r="B45" s="11">
-        <v>13.362492790886799</v>
-      </c>
-      <c r="C45" s="11">
-        <v>-3.2835830629038701E-3</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45" s="11">
-        <v>-1.22792049285E-4</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I45" s="11">
-        <v>-1.36845196802897E-4</v>
-      </c>
-      <c r="J45" s="11">
-        <v>8.2983232930694591E-3</v>
-      </c>
-      <c r="K45" s="11">
-        <v>-7.8439712462329599E-4</v>
-      </c>
-      <c r="L45">
-        <v>2.6801590006555201E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46">
-        <v>427</v>
-      </c>
-      <c r="B46" s="11">
-        <v>15.712482738359499</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D46" s="11">
-        <v>-8.3779499907201908E-3</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F46" s="11">
-        <v>-1.4643067424642401E-4</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H46" s="11">
-        <v>-8.3198412283799598E-4</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J46" s="11">
-        <v>9.4998563183490703E-3</v>
-      </c>
-      <c r="K46" s="11">
-        <v>-8.7572285577487404E-4</v>
-      </c>
-      <c r="L46">
-        <v>2.0473486954457502E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>399</v>
-      </c>
-      <c r="B47" s="11">
-        <v>16.692819279833</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D47" s="11">
-        <v>-9.1529615648768096E-3</v>
-      </c>
-      <c r="E47" s="11">
-        <v>-2.8587048338658701E-7</v>
-      </c>
-      <c r="F47" s="11">
-        <v>-1.56789502445103E-4</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I47" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J47" s="11">
-        <v>9.5337004311087693E-3</v>
-      </c>
-      <c r="K47" s="11">
-        <v>-9.7464282233480795E-4</v>
-      </c>
-      <c r="L47">
-        <v>2.0290060899236601E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <v>411</v>
-      </c>
-      <c r="B48" s="11">
-        <v>16.364609687305101</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="D48" s="11">
-        <v>-9.24282117747139E-3</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F48" s="11">
-        <v>-1.53167102547072E-4</v>
-      </c>
-      <c r="G48" s="11">
-        <v>2.0694220439543E-4</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I48" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="J48" s="11">
-        <v>9.7054910083236405E-3</v>
-      </c>
-      <c r="K48" s="11">
-        <v>-8.6381988833561995E-4</v>
-      </c>
-      <c r="L48">
-        <v>1.8285093453651501E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49">
-        <v>460</v>
-      </c>
-      <c r="B49" s="11">
-        <v>14.701126711804999</v>
-      </c>
-      <c r="C49" s="11">
-        <v>-1.6307691413593099E-3</v>
-      </c>
-      <c r="D49" s="11">
-        <v>-5.6138266669088404E-3</v>
-      </c>
-      <c r="E49" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="F49" s="11">
-        <v>-1.3595817354291299E-4</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I49" s="11">
-        <v>-1.21901158409955E-4</v>
-      </c>
-      <c r="J49" s="11">
-        <v>9.3525931796689405E-3</v>
-      </c>
-      <c r="K49" s="11">
-        <v>-7.7968330795068598E-4</v>
-      </c>
-      <c r="L49">
-        <v>1.6943086009582099E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B50" s="10">
-        <v>13.89</v>
-      </c>
-      <c r="C50" s="10">
-        <v>-3.6519999999999999E-3</v>
-      </c>
-      <c r="D50" s="10">
-        <v>-3.2820000000000002E-3</v>
-      </c>
-      <c r="E50" s="10">
-        <v>-1.719E-8</v>
-      </c>
-      <c r="F50" s="10">
-        <v>-1.281E-4</v>
-      </c>
-      <c r="G50" s="10">
-        <v>-1.498E-3</v>
-      </c>
-      <c r="H50" s="10">
-        <v>3.5710000000000002E-5</v>
-      </c>
-      <c r="I50" s="10">
-        <v>-3.8300000000000003E-5</v>
-      </c>
-      <c r="J50" s="10">
-        <v>8.7709999999999993E-3</v>
-      </c>
-      <c r="K50" s="10">
-        <v>-9.477E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added rate ratios to Socioecon table
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54CDDD-0D6E-406F-9349-AAB14D490FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FBC881-72EC-4815-9436-5CC3EF91FECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="3" activeTab="4" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="2" activeTab="5" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Tables S18_S20" sheetId="13" r:id="rId14"/>
     <sheet name="Largest_effects" sheetId="15" r:id="rId15"/>
     <sheet name="Table S21" sheetId="14" r:id="rId16"/>
+    <sheet name="Table Sx_ELC summary" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1826" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1845" uniqueCount="370">
   <si>
     <t>Predictor variable</t>
   </si>
@@ -1113,17 +1114,63 @@
   </si>
   <si>
     <t>2 yr lag</t>
+  </si>
+  <si>
+    <t>Cassava</t>
+  </si>
+  <si>
+    <t>ELC primary crop</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>% of total</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Rubber</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Corn (maize)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Max value</t>
+  </si>
+  <si>
+    <t>Min value</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Commodity prices ($/ton)</t>
+  </si>
+  <si>
+    <t>Producer prices ($/ton)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1270,7 +1317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1317,6 +1364,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1331,19 +1392,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -5493,67 +5541,67 @@
       <c r="A17" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="28">
         <v>-6327</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="28">
         <v>167.5</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="28">
         <v>-0.26719999999999999</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="28">
         <v>1.911</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="28">
         <v>4.705E-3</v>
       </c>
-      <c r="G17" s="33">
+      <c r="G17" s="28">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="H17" s="33">
+      <c r="H17" s="28">
         <v>1.222E-2</v>
       </c>
-      <c r="I17" s="33">
+      <c r="I17" s="28">
         <v>0.1014</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J17" s="28">
         <v>6.5340000000000005E-4</v>
       </c>
-      <c r="K17" s="33">
+      <c r="K17" s="28">
         <v>9.6550000000000004E-3</v>
       </c>
-      <c r="L17" s="33">
+      <c r="L17" s="28">
         <v>8.4720000000000004E-2</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="29">
         <v>2.2339999999999999E-3</v>
       </c>
-      <c r="N17" s="33">
+      <c r="N17" s="28">
         <v>7.5609999999999997E-2</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="28">
         <v>0.23280000000000001</v>
       </c>
-      <c r="P17" s="33">
+      <c r="P17" s="28">
         <v>-0.14069999999999999</v>
       </c>
-      <c r="Q17" s="33">
+      <c r="Q17" s="28">
         <v>0.82130000000000003</v>
       </c>
-      <c r="R17" s="33">
+      <c r="R17" s="28">
         <v>-598.70000000000005</v>
       </c>
-      <c r="S17" s="33">
+      <c r="S17" s="28">
         <v>46.15</v>
       </c>
-      <c r="T17" s="33">
+      <c r="T17" s="28">
         <v>1.069</v>
       </c>
-      <c r="U17" s="33">
+      <c r="U17" s="28">
         <v>1.804E-2</v>
       </c>
-      <c r="V17" s="33"/>
+      <c r="V17" s="28"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -10484,15 +10532,15 @@
       <c r="A2" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -11304,6 +11352,241 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89174A3D-62DA-4500-8FDA-016886E9D261}">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="40" t="s">
+        <v>368</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40" t="s">
+        <v>369</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3">
+        <v>147</v>
+      </c>
+      <c r="C3" s="41">
+        <v>51.219512195121951</v>
+      </c>
+      <c r="D3">
+        <v>4830</v>
+      </c>
+      <c r="E3">
+        <v>585</v>
+      </c>
+      <c r="F3">
+        <v>1743</v>
+      </c>
+      <c r="G3">
+        <v>477</v>
+      </c>
+      <c r="H3">
+        <v>208</v>
+      </c>
+      <c r="I3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" s="41">
+        <v>8.0139372822299642</v>
+      </c>
+      <c r="D4">
+        <v>573</v>
+      </c>
+      <c r="E4">
+        <v>138</v>
+      </c>
+      <c r="F4">
+        <v>282</v>
+      </c>
+      <c r="G4">
+        <v>3714</v>
+      </c>
+      <c r="H4">
+        <v>1193</v>
+      </c>
+      <c r="I4">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="41">
+        <v>1.7421602787456445</v>
+      </c>
+      <c r="D5">
+        <v>647</v>
+      </c>
+      <c r="E5">
+        <v>172</v>
+      </c>
+      <c r="F5">
+        <v>348</v>
+      </c>
+      <c r="G5">
+        <v>270</v>
+      </c>
+      <c r="H5">
+        <v>96</v>
+      </c>
+      <c r="I5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" s="41">
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="G6">
+        <v>263</v>
+      </c>
+      <c r="H6">
+        <v>96</v>
+      </c>
+      <c r="I6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="41">
+        <v>0.69686411149825789</v>
+      </c>
+      <c r="D7">
+        <v>295</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7">
+        <v>151</v>
+      </c>
+      <c r="G7">
+        <v>316</v>
+      </c>
+      <c r="H7">
+        <v>74</v>
+      </c>
+      <c r="I7">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8">
+        <v>96</v>
+      </c>
+      <c r="C8" s="41">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B9">
+        <v>287</v>
+      </c>
+      <c r="C9" s="41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12452,7 +12735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC824D0-1825-4576-8153-73AE15FAEC82}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -12470,20 +12753,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="28"/>
+      <c r="C1" s="36"/>
       <c r="D1" s="26"/>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="30"/>
+      <c r="F1" s="38"/>
       <c r="G1" s="27"/>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="39" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="31"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -12495,7 +12778,7 @@
       <c r="C2" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="31" t="s">
         <v>351</v>
       </c>
       <c r="E2" s="18" t="s">
@@ -12504,7 +12787,7 @@
       <c r="F2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="32" t="s">
         <v>351</v>
       </c>
       <c r="H2" s="18" t="s">
@@ -12513,7 +12796,7 @@
       <c r="I2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="30" t="s">
         <v>351</v>
       </c>
     </row>
@@ -12523,10 +12806,10 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="37"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="37"/>
+      <c r="G3" s="32"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
     </row>
@@ -12540,7 +12823,7 @@
       <c r="C4" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D4" s="39" t="e">
+      <c r="D4" s="34" t="e">
         <f>EXP(B4)</f>
         <v>#VALUE!</v>
       </c>
@@ -12550,7 +12833,7 @@
       <c r="F4" s="16">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="34">
         <f>EXP(E4)</f>
         <v>0.98511193960306265</v>
       </c>
@@ -12560,7 +12843,7 @@
       <c r="I4" s="16">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="J4" s="40">
+      <c r="J4" s="35">
         <f>EXP(H4)</f>
         <v>0.97433508960874937</v>
       </c>
@@ -12575,7 +12858,7 @@
       <c r="C5" s="16">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="34">
         <f t="shared" ref="D5:D26" si="0">EXP(B5)</f>
         <v>1.3099644507332473</v>
       </c>
@@ -12585,7 +12868,7 @@
       <c r="F5" s="16">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="34">
         <f t="shared" ref="G5:G26" si="1">EXP(E5)</f>
         <v>1.2840254166877414</v>
       </c>
@@ -12595,7 +12878,7 @@
       <c r="I5" s="16">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="35">
         <f t="shared" ref="J5:J26" si="2">EXP(H5)</f>
         <v>0.96657150463750663</v>
       </c>
@@ -12610,7 +12893,7 @@
       <c r="C6" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D6" s="39" t="e">
+      <c r="D6" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -12620,7 +12903,7 @@
       <c r="F6" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G6" s="39" t="e">
+      <c r="G6" s="34" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -12630,7 +12913,7 @@
       <c r="I6" s="16">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="35">
         <f t="shared" si="2"/>
         <v>0.99995000124997913</v>
       </c>
@@ -12645,7 +12928,7 @@
       <c r="C7" s="16">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="34">
         <f t="shared" si="0"/>
         <v>1.0314855038865227</v>
       </c>
@@ -12655,7 +12938,7 @@
       <c r="F7" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="G7" s="39" t="e">
+      <c r="G7" s="34" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
@@ -12665,7 +12948,7 @@
       <c r="I7" s="16">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="35">
         <f t="shared" si="2"/>
         <v>0.99740337707256976</v>
       </c>
@@ -12680,7 +12963,7 @@
       <c r="C8" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="39" t="e">
+      <c r="D8" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -12690,7 +12973,7 @@
       <c r="F8" s="16">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="34">
         <f t="shared" si="1"/>
         <v>1.0036064877830035</v>
       </c>
@@ -12700,7 +12983,7 @@
       <c r="I8" s="16">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="35">
         <f t="shared" si="2"/>
         <v>1.0004000800106678</v>
       </c>
@@ -12715,7 +12998,7 @@
       <c r="C9" s="16">
         <v>0.85</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="34">
         <f t="shared" si="0"/>
         <v>1.1914489672789647E-2</v>
       </c>
@@ -12725,7 +13008,7 @@
       <c r="F9" s="16">
         <v>0.81</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="34">
         <f t="shared" si="1"/>
         <v>2.265408914814322E-3</v>
       </c>
@@ -12735,7 +13018,7 @@
       <c r="I9" s="16">
         <v>0.95</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="35">
         <f t="shared" si="2"/>
         <v>4.619748987816513E-4</v>
       </c>
@@ -12750,7 +13033,7 @@
       <c r="C10" s="16">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="34">
         <f t="shared" si="0"/>
         <v>0.99970004499550036</v>
       </c>
@@ -12760,7 +13043,7 @@
       <c r="F10" s="16">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="34">
         <f t="shared" si="1"/>
         <v>0.99996000079998937</v>
       </c>
@@ -12770,7 +13053,7 @@
       <c r="I10" s="16">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="J10" s="40">
+      <c r="J10" s="35">
         <f t="shared" si="2"/>
         <v>1.0000400008000108</v>
       </c>
@@ -12781,19 +13064,19 @@
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="39">
+      <c r="D11" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="39">
+      <c r="G11" s="34">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="40">
+      <c r="J11" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -12808,7 +13091,7 @@
       <c r="C12" s="16">
         <v>5.6969999999999998E-3</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="34">
         <f t="shared" si="0"/>
         <v>0.99670344560655344</v>
       </c>
@@ -12818,7 +13101,7 @@
       <c r="F12" s="16">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="34">
         <f t="shared" si="1"/>
         <v>1.0070648390547696</v>
       </c>
@@ -12828,7 +13111,7 @@
       <c r="I12" s="16">
         <v>3.2989999999999998E-3</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="35">
         <f t="shared" si="2"/>
         <v>0.99635466044155552</v>
       </c>
@@ -12843,7 +13126,7 @@
       <c r="C13" s="16">
         <v>1.98E-3</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="34">
         <f t="shared" si="0"/>
         <v>1.0093676039035671</v>
       </c>
@@ -12853,7 +13136,7 @@
       <c r="F13" s="16">
         <v>2.7200000000000002E-3</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="34">
         <f t="shared" si="1"/>
         <v>0.99571918890516931</v>
       </c>
@@ -12863,7 +13146,7 @@
       <c r="I13" s="16">
         <v>5.7959999999999999E-4</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="35">
         <f t="shared" si="2"/>
         <v>1.0000357106376097</v>
       </c>
@@ -12878,7 +13161,7 @@
       <c r="C14" s="16">
         <v>2.352E-4</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="34">
         <f t="shared" si="0"/>
         <v>1.0012477778277835</v>
       </c>
@@ -12888,7 +13171,7 @@
       <c r="F14" s="16">
         <v>2.206E-4</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="34">
         <f t="shared" si="1"/>
         <v>1.0001890178616253</v>
       </c>
@@ -12898,7 +13181,7 @@
       <c r="I14" s="16">
         <v>9.1260000000000004E-5</v>
       </c>
-      <c r="J14" s="40">
+      <c r="J14" s="35">
         <f t="shared" si="2"/>
         <v>0.9999617007334356</v>
       </c>
@@ -12913,7 +13196,7 @@
       <c r="C15" s="16">
         <v>1.931E-3</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="34">
         <f t="shared" si="0"/>
         <v>0.99995379106766558</v>
       </c>
@@ -12923,7 +13206,7 @@
       <c r="F15" s="16">
         <v>1.268E-3</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="34">
         <f t="shared" si="1"/>
         <v>1.0071091508825412</v>
       </c>
@@ -12933,7 +13216,7 @@
       <c r="I15" s="16">
         <v>1.24E-3</v>
       </c>
-      <c r="J15" s="40">
+      <c r="J15" s="35">
         <f t="shared" si="2"/>
         <v>1.0088095779270116</v>
       </c>
@@ -12948,7 +13231,7 @@
       <c r="C16" s="16">
         <v>1.751E-3</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="34">
         <f t="shared" si="0"/>
         <v>0.99009636718488148</v>
       </c>
@@ -12958,7 +13241,7 @@
       <c r="F16" s="16">
         <v>2.64E-3</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="34">
         <f t="shared" si="1"/>
         <v>1.0067426298624924</v>
       </c>
@@ -12968,7 +13251,7 @@
       <c r="I16" s="16">
         <v>2.0300000000000001E-3</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="35">
         <f t="shared" si="2"/>
         <v>0.99851110949888044</v>
       </c>
@@ -12979,14 +13262,14 @@
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="39"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="16">
         <v>4.2200000000000001E-4</v>
       </c>
       <c r="F17" s="16">
         <v>1.4400000000000001E-3</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="34">
         <f t="shared" si="1"/>
         <v>1.0004220890545266</v>
       </c>
@@ -12996,7 +13279,7 @@
       <c r="I17" s="16">
         <v>4.2700000000000004E-3</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="35">
         <f>EXP(H17)</f>
         <v>0.99672537332356081</v>
       </c>
@@ -13011,7 +13294,7 @@
       <c r="C18" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="39" t="e">
+      <c r="D18" s="34" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
@@ -13021,7 +13304,7 @@
       <c r="F18" s="16">
         <v>5.0299999999999999E-7</v>
       </c>
-      <c r="G18" s="39">
+      <c r="G18" s="34">
         <f t="shared" si="1"/>
         <v>1.0000001868000175</v>
       </c>
@@ -13031,7 +13314,7 @@
       <c r="I18" s="16">
         <v>1.6E-7</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="35">
         <f t="shared" si="2"/>
         <v>0.99999998280000013</v>
       </c>
@@ -13046,7 +13329,7 @@
       <c r="C19" s="16">
         <v>2.41E-5</v>
       </c>
-      <c r="D19" s="39">
+      <c r="D19" s="34">
         <f t="shared" si="0"/>
         <v>0.99986090967395647</v>
       </c>
@@ -13056,7 +13339,7 @@
       <c r="F19" s="16">
         <v>2.51E-5</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="34">
         <f t="shared" si="1"/>
         <v>0.99982531525915641</v>
       </c>
@@ -13066,7 +13349,7 @@
       <c r="I19" s="16">
         <v>2.55E-5</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="35">
         <f t="shared" si="2"/>
         <v>0.99987200819165045</v>
       </c>
@@ -13077,19 +13360,19 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="39">
+      <c r="D20" s="34">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="39">
+      <c r="G20" s="34">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16"/>
-      <c r="J20" s="40">
+      <c r="J20" s="35">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -13104,7 +13387,7 @@
       <c r="C21" s="16">
         <v>3.5500000000000002E-3</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="34">
         <f t="shared" si="0"/>
         <v>1.0041586231745985</v>
       </c>
@@ -13114,7 +13397,7 @@
       <c r="F21" s="16">
         <v>2.395E-3</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="34">
         <f t="shared" si="1"/>
         <v>1.0109899506711895</v>
       </c>
@@ -13124,7 +13407,7 @@
       <c r="I21" s="16">
         <v>8.1450000000000001E-4</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="35">
         <f t="shared" si="2"/>
         <v>1.0001439103541017</v>
       </c>
@@ -13139,7 +13422,7 @@
       <c r="C22" s="16">
         <v>4.3600000000000002E-3</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="34">
         <f t="shared" si="0"/>
         <v>0.97565133024224471</v>
       </c>
@@ -13149,7 +13432,7 @@
       <c r="F22" s="16">
         <v>5.6389999999999999E-3</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="34">
         <f t="shared" si="1"/>
         <v>1.0045302306083088</v>
       </c>
@@ -13159,7 +13442,7 @@
       <c r="I22" s="16">
         <v>4.7349999999999996E-3</v>
       </c>
-      <c r="J22" s="40">
+      <c r="J22" s="35">
         <f t="shared" si="2"/>
         <v>1.0126594610570951</v>
       </c>
@@ -13174,7 +13457,7 @@
       <c r="C23" s="16">
         <v>4.0099999999999997E-3</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="34">
         <f t="shared" si="0"/>
         <v>1.0348329368321532</v>
       </c>
@@ -13184,7 +13467,7 @@
       <c r="F23" s="16">
         <v>2.2780000000000001E-3</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="34">
         <f t="shared" si="1"/>
         <v>0.9992539784125809</v>
       </c>
@@ -13194,7 +13477,7 @@
       <c r="I23" s="16">
         <v>4.6719999999999999E-3</v>
       </c>
-      <c r="J23" s="40">
+      <c r="J23" s="35">
         <f t="shared" si="2"/>
         <v>0.99570425322935363</v>
       </c>
@@ -13209,7 +13492,7 @@
       <c r="C24" s="16">
         <v>9.7419999999999999E-5</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="34">
         <f t="shared" si="0"/>
         <v>1.0000361306526964</v>
       </c>
@@ -13219,7 +13502,7 @@
       <c r="F24" s="16">
         <v>1.7550000000000001E-4</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="34">
         <f t="shared" si="1"/>
         <v>1.0001564122311177</v>
       </c>
@@ -13229,7 +13512,7 @@
       <c r="I24" s="16">
         <v>5.8400000000000003E-5</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="35">
         <f t="shared" si="2"/>
         <v>1.0000048990120001</v>
       </c>
@@ -13244,7 +13527,7 @@
       <c r="C25" s="16">
         <v>1.2340000000000001E-3</v>
       </c>
-      <c r="D25" s="39">
+      <c r="D25" s="34">
         <f t="shared" si="0"/>
         <v>1.0003212515902435</v>
       </c>
@@ -13254,7 +13537,7 @@
       <c r="F25" s="16">
         <v>7.5509999999999998E-4</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="34">
         <f t="shared" si="1"/>
         <v>1.0000555515429299</v>
       </c>
@@ -13264,7 +13547,7 @@
       <c r="I25" s="16">
         <v>2.1419999999999998E-3</v>
       </c>
-      <c r="J25" s="40">
+      <c r="J25" s="35">
         <f t="shared" si="2"/>
         <v>0.98224943082908445</v>
       </c>
@@ -13279,7 +13562,7 @@
       <c r="C26" s="16">
         <v>2.3779999999999999E-5</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="34">
         <f t="shared" si="0"/>
         <v>0.99977342567184091</v>
       </c>
@@ -13289,7 +13572,7 @@
       <c r="F26" s="16">
         <v>2.124E-5</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="34">
         <f t="shared" si="1"/>
         <v>0.99984711168860929</v>
       </c>
@@ -13299,14 +13582,14 @@
       <c r="I26" s="16">
         <v>2.035E-5</v>
       </c>
-      <c r="J26" s="40">
+      <c r="J26" s="35">
         <f t="shared" si="2"/>
         <v>0.99986930854087286</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="D27" s="33"/>
+      <c r="G27" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -13323,8 +13606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9FA71-8CE5-4C6B-887E-5FA553777DF5}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13664,7 +13947,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B11:D18">
+  <conditionalFormatting sqref="B20:D25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -13682,9 +13965,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13692,23 +13977,23 @@
     <col min="4" max="4" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>251</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>252</v>
       </c>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>55</v>
       </c>
@@ -13724,8 +14009,11 @@
       <c r="E4" s="20" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="30" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>249</v>
       </c>
@@ -13734,12 +14022,12 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>170</v>
       </c>
@@ -13750,7 +14038,7 @@
         <v>3.2333599999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>172</v>
       </c>
@@ -13761,7 +14049,7 @@
         <v>6.7960000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -13772,7 +14060,7 @@
         <v>2.6024799999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>173</v>
       </c>
@@ -13783,12 +14071,12 @@
         <v>2.197E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>221</v>
       </c>
@@ -13799,7 +14087,7 @@
         <v>0.56200000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -13809,8 +14097,12 @@
       <c r="E13" s="10">
         <v>1.127</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="35">
+        <f t="shared" ref="F13:F18" si="0">EXP(D13)</f>
+        <v>5.4539513917295024E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -13820,8 +14112,12 @@
       <c r="E14" s="10">
         <v>0.122</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="35">
+        <f t="shared" si="0"/>
+        <v>2.8605101984831802</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>166</v>
       </c>
@@ -13831,8 +14127,12 @@
       <c r="E15" s="10">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="35">
+        <f t="shared" si="0"/>
+        <v>1.786931673257466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>167</v>
       </c>
@@ -13842,8 +14142,12 @@
       <c r="E16" s="10">
         <v>0.1114</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="35">
+        <f t="shared" si="0"/>
+        <v>1.9995056999733047</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -13853,8 +14157,12 @@
       <c r="E17" s="10">
         <v>2.4719999999999998E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" s="35">
+        <f t="shared" si="0"/>
+        <v>0.99999919650032276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>169</v>
       </c>
@@ -13866,18 +14174,22 @@
       <c r="E18" s="22">
         <v>1.4290000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="35">
+        <f t="shared" si="0"/>
+        <v>1.0092939227578768</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -13890,7 +14202,7 @@
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>173</v>
       </c>
@@ -13903,7 +14215,7 @@
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>162</v>
       </c>
@@ -13912,7 +14224,7 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>221</v>
       </c>
@@ -13925,7 +14237,7 @@
         <v>0.449712</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>254</v>
       </c>
@@ -13937,8 +14249,12 @@
       <c r="E25" s="10">
         <v>1.8799999999999999E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25" s="35">
+        <f>EXP(E25)</f>
+        <v>1.0018817683079659</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>255</v>
       </c>
@@ -13950,8 +14266,12 @@
       <c r="E26" s="10">
         <v>2.2330000000000002E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="35">
+        <f t="shared" ref="F26:F31" si="1">EXP(E26)</f>
+        <v>1.0022354950012671</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>256</v>
       </c>
@@ -13963,8 +14283,12 @@
       <c r="E27" s="10">
         <v>2.3519999999999999E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27" s="35">
+        <f t="shared" si="1"/>
+        <v>1.0023547681217821</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>257</v>
       </c>
@@ -13976,8 +14300,12 @@
       <c r="E28" s="10">
         <v>1.9120000000000001E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="35">
+        <f t="shared" si="1"/>
+        <v>1.0019138290375209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>258</v>
       </c>
@@ -13989,8 +14317,12 @@
       <c r="E29" s="10">
         <v>1.8569999999999999E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F29" s="35">
+        <f t="shared" si="1"/>
+        <v>1.0018587252922906</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>259</v>
       </c>
@@ -14002,8 +14334,12 @@
       <c r="E30" s="10">
         <v>0.40894999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30" s="35">
+        <f t="shared" si="1"/>
+        <v>1.5052364567811438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>260</v>
       </c>
@@ -14015,8 +14351,12 @@
       <c r="E31" s="10">
         <v>0.496452</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="35">
+        <f t="shared" si="1"/>
+        <v>1.6428819726719563</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>

</xml_diff>

<commit_message>
minor edits to table 4 (effect shading)
</commit_message>
<xml_diff>
--- a/Write up/Table_data sources and details.xlsx
+++ b/Write up/Table_data sources and details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Nuttall\Documents\PhD\PhD_Chapter1\Write up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A02D4DA-D8D6-4DA8-BC77-E49E9F5856A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32D1DCB-987B-46DC-84CD-692D99F672EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="3" activeTab="5" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" firstSheet="4" activeTab="5" xr2:uid="{0E90B39A-0A43-4036-9AD4-5826A0E24FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1171,7 +1171,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1318,7 +1318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1379,6 +1379,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1394,8 +1396,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7789,7 +7790,7 @@
         <v>8.1944309930366607E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>212</v>
       </c>
@@ -10511,8 +10512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7582E62-B1F2-409C-8ABA-4384911F8E33}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10534,15 +10535,15 @@
       <c r="A2" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -11384,16 +11385,16 @@
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="42" t="s">
         <v>368</v>
       </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42" t="s">
         <v>369</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -11431,7 +11432,7 @@
       <c r="B3">
         <v>147</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="36">
         <v>51.219512195121951</v>
       </c>
       <c r="D3">
@@ -11460,7 +11461,7 @@
       <c r="B4">
         <v>23</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="36">
         <v>8.0139372822299642</v>
       </c>
       <c r="D4">
@@ -11489,7 +11490,7 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="36">
         <v>1.7421602787456445</v>
       </c>
       <c r="D5">
@@ -11518,7 +11519,7 @@
       <c r="B6">
         <v>14</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="36">
         <v>4.8780487804878048</v>
       </c>
       <c r="G6">
@@ -11538,7 +11539,7 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="36">
         <v>0.69686411149825789</v>
       </c>
       <c r="D7">
@@ -11567,7 +11568,7 @@
       <c r="B8">
         <v>96</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="36">
         <v>33.4</v>
       </c>
     </row>
@@ -11578,12 +11579,12 @@
       <c r="B9">
         <v>287</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="36">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C11" s="41"/>
+      <c r="C11" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -12755,20 +12756,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="26"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="40"/>
       <c r="G1" s="27"/>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="I1" s="39"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -13969,8 +13970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F95D83-98CF-4790-A472-0B5005BEB99D}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14160,7 +14161,7 @@
       <c r="E17" s="10">
         <v>2.4719999999999998E-3</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="37">
         <f>EXP(D17)</f>
         <v>0.99999919650032276</v>
       </c>
@@ -14252,7 +14253,7 @@
       <c r="E25" s="10">
         <v>1.8799999999999999E-3</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="43">
         <f>EXP(E25)</f>
         <v>1.0018817683079659</v>
       </c>
@@ -14269,7 +14270,7 @@
       <c r="E26" s="10">
         <v>2.2330000000000002E-3</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="43">
         <f t="shared" ref="F26:F31" si="1">EXP(E26)</f>
         <v>1.0022354950012671</v>
       </c>
@@ -14286,7 +14287,7 @@
       <c r="E27" s="10">
         <v>2.3519999999999999E-3</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="43">
         <f t="shared" si="1"/>
         <v>1.0023547681217821</v>
       </c>
@@ -14303,7 +14304,7 @@
       <c r="E28" s="10">
         <v>1.9120000000000001E-3</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F28" s="43">
         <f t="shared" si="1"/>
         <v>1.0019138290375209</v>
       </c>
@@ -14320,7 +14321,7 @@
       <c r="E29" s="10">
         <v>1.8569999999999999E-3</v>
       </c>
-      <c r="F29" s="35">
+      <c r="F29" s="43">
         <f t="shared" si="1"/>
         <v>1.0018587252922906</v>
       </c>
@@ -14337,7 +14338,7 @@
       <c r="E30" s="10">
         <v>0.40894999999999998</v>
       </c>
-      <c r="F30" s="35">
+      <c r="F30" s="43">
         <f t="shared" si="1"/>
         <v>1.5052364567811438</v>
       </c>
@@ -14354,7 +14355,7 @@
       <c r="E31" s="10">
         <v>0.496452</v>
       </c>
-      <c r="F31" s="35">
+      <c r="F31" s="43">
         <f t="shared" si="1"/>
         <v>1.6428819726719563</v>
       </c>
@@ -14367,6 +14368,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F13:F18">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:F31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>